<commit_message>
Handle case where a reasigned cajero has a perfect fit
</commit_message>
<xml_diff>
--- a/PlantillaSemanal_Exportada.xlsx
+++ b/PlantillaSemanal_Exportada.xlsx
@@ -635,7 +635,7 @@
       <c r="A5" s="7" t="n"/>
       <c r="B5" s="8" t="inlineStr">
         <is>
-          <t>(T) HEREDIA CAHUAYA, SUSAN NAYELLI</t>
+          <t>HEREDIA CAHUAYA, SUSAN NAYELLI</t>
         </is>
       </c>
       <c r="C5" s="8" t="inlineStr">
@@ -653,7 +653,7 @@
       <c r="A6" s="1" t="n"/>
       <c r="B6" s="3" t="inlineStr">
         <is>
-          <t>(T) BRENIS LARTIGA, SEBASTIAN</t>
+          <t>BRENIS LARTIGA, SEBASTIAN</t>
         </is>
       </c>
       <c r="C6" s="3" t="inlineStr">
@@ -713,12 +713,12 @@
       <c r="E8" s="1" t="n"/>
       <c r="F8" s="3" t="inlineStr">
         <is>
-          <t>BRENIS LARTIGA, SEBASTIAN</t>
+          <t>LEON TICONA, MARIA FERNANDA</t>
         </is>
       </c>
       <c r="G8" s="3" t="inlineStr">
         <is>
-          <t>18:45-18:45</t>
+          <t>19:00-22:45</t>
         </is>
       </c>
       <c r="H8" s="3" t="n"/>
@@ -857,12 +857,12 @@
       </c>
       <c r="B15" s="3" t="inlineStr">
         <is>
-          <t>HEREDIA CAHUAYA, SUSAN NAYELLI</t>
+          <t>ALVITE CORNEJO, ANGIE LUCERO</t>
         </is>
       </c>
       <c r="C15" s="3" t="inlineStr">
         <is>
-          <t>10:00-10:00</t>
+          <t>10:15-14:00</t>
         </is>
       </c>
       <c r="D15" s="3" t="n"/>
@@ -871,12 +871,12 @@
       </c>
       <c r="F15" s="3" t="inlineStr">
         <is>
-          <t>SICHA JORGE, JOSE ANGELO</t>
+          <t>BARRIENTOS JERI, MILAGROS NICOL</t>
         </is>
       </c>
       <c r="G15" s="3" t="inlineStr">
         <is>
-          <t>15:15-19:00</t>
+          <t>19:00-22:45</t>
         </is>
       </c>
       <c r="H15" s="3" t="n"/>
@@ -885,26 +885,18 @@
       <c r="A16" s="1" t="n"/>
       <c r="B16" s="3" t="inlineStr">
         <is>
-          <t>ALVITE CORNEJO, ANGIE LUCERO</t>
+          <t>SICHA JORGE, JOSE ANGELO</t>
         </is>
       </c>
       <c r="C16" s="3" t="inlineStr">
         <is>
-          <t>10:15-14:00</t>
+          <t>15:15-19:00</t>
         </is>
       </c>
       <c r="D16" s="3" t="n"/>
       <c r="E16" s="1" t="n"/>
-      <c r="F16" s="3" t="inlineStr">
-        <is>
-          <t>BARRIENTOS JERI, MILAGROS NICOL</t>
-        </is>
-      </c>
-      <c r="G16" s="3" t="inlineStr">
-        <is>
-          <t>19:00-22:45</t>
-        </is>
-      </c>
+      <c r="F16" s="3" t="n"/>
+      <c r="G16" s="3" t="n"/>
       <c r="H16" s="3" t="n"/>
     </row>
     <row r="17" ht="19.5" customHeight="1">
@@ -1439,7 +1431,7 @@
       </c>
       <c r="B53" s="3" t="inlineStr">
         <is>
-          <t>CARHUANCHO RAYMUNDO, JAMES JESUS</t>
+          <t>HUAMANI QUICANO, EMELYN HEIDY</t>
         </is>
       </c>
       <c r="C53" s="3" t="inlineStr">
@@ -1473,7 +1465,7 @@
       </c>
       <c r="B54" s="3" t="inlineStr">
         <is>
-          <t>HUAMANI QUICANO, EMELYN HEIDY</t>
+          <t>CARHUANCHO RAYMUNDO, JAMES JESUS</t>
         </is>
       </c>
       <c r="C54" s="3" t="inlineStr">
@@ -1680,7 +1672,7 @@
       <c r="E5" s="7" t="n"/>
       <c r="F5" s="8" t="inlineStr">
         <is>
-          <t>(T) BRENIS LARTIGA, SEBASTIAN</t>
+          <t>BRENIS LARTIGA, SEBASTIAN</t>
         </is>
       </c>
       <c r="G5" s="8" t="inlineStr">
@@ -2034,12 +2026,12 @@
       </c>
       <c r="B21" s="3" t="inlineStr">
         <is>
-          <t>BRENIS LARTIGA, SEBASTIAN</t>
+          <t>PIÑA SHUPINGAHUA, SANDRA</t>
         </is>
       </c>
       <c r="C21" s="3" t="inlineStr">
         <is>
-          <t>18:00-18:00</t>
+          <t>18:15-22:00</t>
         </is>
       </c>
       <c r="D21" s="3" t="n"/>
@@ -2052,16 +2044,8 @@
     </row>
     <row r="22" ht="19.5" customHeight="1">
       <c r="A22" s="1" t="n"/>
-      <c r="B22" s="3" t="inlineStr">
-        <is>
-          <t>PIÑA SHUPINGAHUA, SANDRA</t>
-        </is>
-      </c>
-      <c r="C22" s="3" t="inlineStr">
-        <is>
-          <t>18:15-22:00</t>
-        </is>
-      </c>
+      <c r="B22" s="3" t="n"/>
+      <c r="C22" s="3" t="n"/>
       <c r="D22" s="3" t="n"/>
       <c r="E22" s="1" t="n"/>
       <c r="F22" s="3" t="n"/>
@@ -3750,7 +3734,7 @@
       <c r="A5" s="7" t="n"/>
       <c r="B5" s="8" t="inlineStr">
         <is>
-          <t>(T) HUAMAN HUAMANI, ALEXIS JAVIER</t>
+          <t>HUAMAN HUAMANI, ALEXIS JAVIER</t>
         </is>
       </c>
       <c r="C5" s="8" t="inlineStr">
@@ -3988,40 +3972,32 @@
       </c>
       <c r="B15" s="3" t="inlineStr">
         <is>
-          <t>HUAMAN HUAMANI, ALEXIS JAVIER</t>
+          <t>ALVITE CORNEJO, ANGIE LUCERO</t>
         </is>
       </c>
       <c r="C15" s="3" t="inlineStr">
         <is>
-          <t>10:00-10:00</t>
+          <t>10:15-14:00</t>
         </is>
       </c>
       <c r="D15" s="3" t="n"/>
       <c r="E15" s="1" t="n">
         <v>6</v>
       </c>
-      <c r="F15" s="3" t="inlineStr">
-        <is>
-          <t>HUAMANI LOPEZ, DREYDI BELINDA</t>
-        </is>
-      </c>
-      <c r="G15" s="3" t="inlineStr">
-        <is>
-          <t>18:15-22:00</t>
-        </is>
-      </c>
+      <c r="F15" s="3" t="n"/>
+      <c r="G15" s="3" t="n"/>
       <c r="H15" s="3" t="n"/>
     </row>
     <row r="16" ht="19.5" customHeight="1">
       <c r="A16" s="1" t="n"/>
       <c r="B16" s="3" t="inlineStr">
         <is>
-          <t>ALVITE CORNEJO, ANGIE LUCERO</t>
+          <t>HUAMANI LOPEZ, DREYDI BELINDA</t>
         </is>
       </c>
       <c r="C16" s="3" t="inlineStr">
         <is>
-          <t>10:15-14:00</t>
+          <t>18:15-22:00</t>
         </is>
       </c>
       <c r="D16" s="3" t="n"/>
@@ -4767,7 +4743,7 @@
       <c r="A5" s="7" t="n"/>
       <c r="B5" s="8" t="inlineStr">
         <is>
-          <t>(T) ERIQUE CALLE, MARIA ANTONIETA</t>
+          <t>ERIQUE CALLE, MARIA ANTONIETA</t>
         </is>
       </c>
       <c r="C5" s="8" t="inlineStr">
@@ -4785,7 +4761,7 @@
       <c r="A6" s="1" t="n"/>
       <c r="B6" s="3" t="inlineStr">
         <is>
-          <t>(T) RAMOS TINOCO, JORDAN JAVIER</t>
+          <t>RAMOS TINOCO, JORDAN JAVIER</t>
         </is>
       </c>
       <c r="C6" s="3" t="inlineStr">
@@ -4949,12 +4925,12 @@
       </c>
       <c r="B13" s="3" t="inlineStr">
         <is>
-          <t>ERIQUE CALLE, MARIA ANTONIETA</t>
+          <t>RUIZ SANTOS, CIELO CRISTHINA</t>
         </is>
       </c>
       <c r="C13" s="3" t="inlineStr">
         <is>
-          <t>10:00-10:00</t>
+          <t>10:15-14:00</t>
         </is>
       </c>
       <c r="D13" s="3" t="n"/>
@@ -4963,12 +4939,12 @@
       </c>
       <c r="F13" s="3" t="inlineStr">
         <is>
-          <t>VEGA CARDENAS, ANGELICA LOURDES</t>
+          <t>HUAMANI LOPEZ, DREYDI BELINDA</t>
         </is>
       </c>
       <c r="G13" s="3" t="inlineStr">
         <is>
-          <t>15:00-18:45</t>
+          <t>19:00-22:45</t>
         </is>
       </c>
       <c r="H13" s="3" t="n"/>
@@ -4977,26 +4953,18 @@
       <c r="A14" s="1" t="n"/>
       <c r="B14" s="3" t="inlineStr">
         <is>
-          <t>RUIZ SANTOS, CIELO CRISTHINA</t>
+          <t>VEGA CARDENAS, ANGELICA LOURDES</t>
         </is>
       </c>
       <c r="C14" s="3" t="inlineStr">
         <is>
-          <t>10:15-14:00</t>
+          <t>15:00-18:45</t>
         </is>
       </c>
       <c r="D14" s="3" t="n"/>
       <c r="E14" s="1" t="n"/>
-      <c r="F14" s="3" t="inlineStr">
-        <is>
-          <t>RAMOS TINOCO, JORDAN JAVIER</t>
-        </is>
-      </c>
-      <c r="G14" s="3" t="inlineStr">
-        <is>
-          <t>18:45-18:45</t>
-        </is>
-      </c>
+      <c r="F14" s="3" t="n"/>
+      <c r="G14" s="3" t="n"/>
       <c r="H14" s="3" t="n"/>
     </row>
     <row r="15" ht="19.5" customHeight="1">
@@ -5784,7 +5752,7 @@
       <c r="A5" s="7" t="n"/>
       <c r="B5" s="8" t="inlineStr">
         <is>
-          <t>(T) NINA OSCCO, FRANCIS GABRIELA</t>
+          <t>NINA OSCCO, FRANCIS GABRIELA</t>
         </is>
       </c>
       <c r="C5" s="8" t="inlineStr">
@@ -6022,40 +5990,32 @@
       </c>
       <c r="B17" s="3" t="inlineStr">
         <is>
-          <t>NINA OSCCO, FRANCIS GABRIELA</t>
+          <t>RAMOS TINOCO, JORDAN JAVIER</t>
         </is>
       </c>
       <c r="C17" s="3" t="inlineStr">
         <is>
-          <t>10:00-10:00</t>
+          <t>10:15-19:15</t>
         </is>
       </c>
       <c r="D17" s="3" t="n"/>
       <c r="E17" s="1" t="n">
         <v>7</v>
       </c>
-      <c r="F17" s="3" t="inlineStr">
-        <is>
-          <t>VILCAPOMA CHILIN, JULISSA JAZMIN</t>
-        </is>
-      </c>
-      <c r="G17" s="3" t="inlineStr">
-        <is>
-          <t>19:15-22:00</t>
-        </is>
-      </c>
+      <c r="F17" s="3" t="n"/>
+      <c r="G17" s="3" t="n"/>
       <c r="H17" s="3" t="n"/>
     </row>
     <row r="18" ht="19.5" customHeight="1">
       <c r="A18" s="1" t="n"/>
       <c r="B18" s="3" t="inlineStr">
         <is>
-          <t>RAMOS TINOCO, JORDAN JAVIER</t>
+          <t>VILCAPOMA CHILIN, JULISSA JAZMIN</t>
         </is>
       </c>
       <c r="C18" s="3" t="inlineStr">
         <is>
-          <t>10:15-19:15</t>
+          <t>19:15-22:00</t>
         </is>
       </c>
       <c r="D18" s="3" t="n"/>
@@ -6825,7 +6785,7 @@
       <c r="A5" s="7" t="n"/>
       <c r="B5" s="8" t="inlineStr">
         <is>
-          <t>(T) BRANCACHO RAMIREZ, BRINDY</t>
+          <t>BRANCACHO RAMIREZ, BRINDY</t>
         </is>
       </c>
       <c r="C5" s="8" t="inlineStr">
@@ -7079,40 +7039,32 @@
       </c>
       <c r="B17" s="3" t="inlineStr">
         <is>
-          <t>BRANCACHO RAMIREZ, BRINDY</t>
+          <t>CASAPAICO RIVERA, ENZO MANUEL</t>
         </is>
       </c>
       <c r="C17" s="3" t="inlineStr">
         <is>
-          <t>10:00-10:00</t>
+          <t>10:15-14:00</t>
         </is>
       </c>
       <c r="D17" s="3" t="n"/>
       <c r="E17" s="1" t="n">
         <v>7</v>
       </c>
-      <c r="F17" s="3" t="inlineStr">
-        <is>
-          <t>RAMOS TINOCO, JORDAN JAVIER</t>
-        </is>
-      </c>
-      <c r="G17" s="3" t="inlineStr">
-        <is>
-          <t>14:15-22:45</t>
-        </is>
-      </c>
+      <c r="F17" s="3" t="n"/>
+      <c r="G17" s="3" t="n"/>
       <c r="H17" s="3" t="n"/>
     </row>
     <row r="18" ht="19.5" customHeight="1">
       <c r="A18" s="1" t="n"/>
       <c r="B18" s="3" t="inlineStr">
         <is>
-          <t>CASAPAICO RIVERA, ENZO MANUEL</t>
+          <t>RAMOS TINOCO, JORDAN JAVIER</t>
         </is>
       </c>
       <c r="C18" s="3" t="inlineStr">
         <is>
-          <t>10:15-14:00</t>
+          <t>14:15-22:45</t>
         </is>
       </c>
       <c r="D18" s="3" t="n"/>

</xml_diff>

<commit_message>
Refactor PDF files and update asignar_cajeros function for improved sorting and assignment logic
</commit_message>
<xml_diff>
--- a/PlantillaSemanal_Exportada.xlsx
+++ b/PlantillaSemanal_Exportada.xlsx
@@ -619,7 +619,7 @@
     <row r="2" ht="19.5" customHeight="1">
       <c r="A2" s="14" t="inlineStr">
         <is>
-          <t>FECHA</t>
+          <t>LUNES 11 DE NOVIEMBRE 2024</t>
         </is>
       </c>
       <c r="B2" s="16" t="n"/>
@@ -1413,7 +1413,7 @@
     <row r="2" ht="19.5" customHeight="1">
       <c r="A2" s="14" t="inlineStr">
         <is>
-          <t>FECHA</t>
+          <t>MARTES 12 DE NOVIEMBRE 2024</t>
         </is>
       </c>
       <c r="B2" s="16" t="n"/>
@@ -2207,7 +2207,7 @@
     <row r="2" ht="19.5" customHeight="1">
       <c r="A2" s="14" t="inlineStr">
         <is>
-          <t>FECHA</t>
+          <t>MIÉRCOLES 13 DE NOVIEMBRE 2024</t>
         </is>
       </c>
       <c r="B2" s="16" t="n"/>
@@ -3001,7 +3001,7 @@
     <row r="2" ht="19.5" customHeight="1">
       <c r="A2" s="14" t="inlineStr">
         <is>
-          <t>FECHA</t>
+          <t>JUEVES 14 DE NOVIEMBRE 2024</t>
         </is>
       </c>
       <c r="B2" s="16" t="n"/>
@@ -3138,12 +3138,12 @@
       </c>
       <c r="B7" s="3" t="inlineStr">
         <is>
-          <t>ALVITE CORNEJO, ANGIE LUCERO</t>
+          <t>QUISPE MONDRAGON, JUAN ALFONSO</t>
         </is>
       </c>
       <c r="C7" s="3" t="inlineStr">
         <is>
-          <t>07:00-10:45</t>
+          <t>07:30-11:15</t>
         </is>
       </c>
       <c r="D7" s="3" t="n"/>
@@ -3152,12 +3152,12 @@
       </c>
       <c r="F7" s="3" t="inlineStr">
         <is>
-          <t>HUANCAS SHUAN, JOSELYN JAZMIN</t>
+          <t>GONZALES OLIVARES, JEFFERSON ISRAEL</t>
         </is>
       </c>
       <c r="G7" s="3" t="inlineStr">
         <is>
-          <t>15:00-18:45</t>
+          <t>15:15-19:00</t>
         </is>
       </c>
       <c r="H7" s="3" t="n"/>
@@ -3166,24 +3166,24 @@
       <c r="A8" s="14" t="n"/>
       <c r="B8" s="3" t="inlineStr">
         <is>
-          <t>SOTO VELAZCO, EMIR ALESSANDRO</t>
+          <t>QUIQUIA MALLQUI, CYNTHIA ANGELLINE</t>
         </is>
       </c>
       <c r="C8" s="3" t="inlineStr">
         <is>
-          <t>11:00-14:45</t>
+          <t>11:15-15:00</t>
         </is>
       </c>
       <c r="D8" s="3" t="n"/>
       <c r="E8" s="14" t="n"/>
       <c r="F8" s="3" t="inlineStr">
         <is>
-          <t>POVEA CANTARO, FARID YASSER</t>
+          <t>HUAMANI LOPEZ, DREYDI BELINDA</t>
         </is>
       </c>
       <c r="G8" s="3" t="inlineStr">
         <is>
-          <t>18:45-22:30</t>
+          <t>19:00-19:30</t>
         </is>
       </c>
       <c r="H8" s="3" t="n"/>
@@ -3194,12 +3194,12 @@
       </c>
       <c r="B9" s="3" t="inlineStr">
         <is>
-          <t>QUISPE MONDRAGON, JUAN ALFONSO</t>
+          <t>PIÑA SHUPINGAHUA, SANDRA</t>
         </is>
       </c>
       <c r="C9" s="3" t="inlineStr">
         <is>
-          <t>07:30-11:15</t>
+          <t>08:45-12:30</t>
         </is>
       </c>
       <c r="D9" s="3" t="n"/>
@@ -3208,12 +3208,12 @@
       </c>
       <c r="F9" s="3" t="inlineStr">
         <is>
-          <t>GONZALES OLIVARES, JEFFERSON ISRAEL</t>
+          <t>MUÑOZ SOTOMAYOR, MIRIAN RAQUEL</t>
         </is>
       </c>
       <c r="G9" s="3" t="inlineStr">
         <is>
-          <t>15:15-19:00</t>
+          <t>13:15-17:00</t>
         </is>
       </c>
       <c r="H9" s="3" t="n"/>
@@ -3222,24 +3222,24 @@
       <c r="A10" s="14" t="n"/>
       <c r="B10" s="3" t="inlineStr">
         <is>
-          <t>QUIQUIA MALLQUI, CYNTHIA ANGELLINE</t>
+          <t>GARRIDO SOTO, VICTORIA CELESTE</t>
         </is>
       </c>
       <c r="C10" s="3" t="inlineStr">
         <is>
-          <t>11:15-15:00</t>
+          <t>12:30-13:00</t>
         </is>
       </c>
       <c r="D10" s="3" t="n"/>
       <c r="E10" s="14" t="n"/>
       <c r="F10" s="3" t="inlineStr">
         <is>
-          <t>HUAMANI LOPEZ, DREYDI BELINDA</t>
+          <t>SICHA JORGE, JOSE ANGELO</t>
         </is>
       </c>
       <c r="G10" s="3" t="inlineStr">
         <is>
-          <t>19:00-19:30</t>
+          <t>17:00-20:45</t>
         </is>
       </c>
       <c r="H10" s="3" t="n"/>
@@ -3250,12 +3250,12 @@
       </c>
       <c r="B11" s="3" t="inlineStr">
         <is>
-          <t>PIÑA SHUPINGAHUA, SANDRA</t>
+          <t>HUAYANAY VELASCO, ATHINA</t>
         </is>
       </c>
       <c r="C11" s="3" t="inlineStr">
         <is>
-          <t>08:45-12:30</t>
+          <t>09:30-10:00</t>
         </is>
       </c>
       <c r="D11" s="3" t="n"/>
@@ -3278,12 +3278,12 @@
       <c r="A12" s="14" t="n"/>
       <c r="B12" s="3" t="inlineStr">
         <is>
-          <t>GARRIDO SOTO, VICTORIA CELESTE</t>
+          <t>RUIZ SANTOS, CIELO CRISTHINA</t>
         </is>
       </c>
       <c r="C12" s="3" t="inlineStr">
         <is>
-          <t>12:30-13:00</t>
+          <t>10:15-14:00</t>
         </is>
       </c>
       <c r="D12" s="3" t="n"/>
@@ -3298,40 +3298,32 @@
       </c>
       <c r="B13" s="3" t="inlineStr">
         <is>
-          <t>HUAYANAY VELASCO, ATHINA</t>
+          <t>CUSI QUISPE, ANDREA ESTEFANY</t>
         </is>
       </c>
       <c r="C13" s="3" t="inlineStr">
         <is>
-          <t>09:30-10:00</t>
+          <t>11:00-14:45</t>
         </is>
       </c>
       <c r="D13" s="3" t="n"/>
       <c r="E13" s="14" t="n">
         <v>5</v>
       </c>
-      <c r="F13" s="3" t="inlineStr">
-        <is>
-          <t>SICHA JORGE, JOSE ANGELO</t>
-        </is>
-      </c>
-      <c r="G13" s="3" t="inlineStr">
-        <is>
-          <t>17:00-20:45</t>
-        </is>
-      </c>
+      <c r="F13" s="3" t="n"/>
+      <c r="G13" s="3" t="n"/>
       <c r="H13" s="3" t="n"/>
     </row>
     <row r="14" ht="19.5" customHeight="1">
       <c r="A14" s="14" t="n"/>
       <c r="B14" s="3" t="inlineStr">
         <is>
-          <t>RUIZ SANTOS, CIELO CRISTHINA</t>
+          <t>NAVARRO MORENO, ARIADNA NAYLEA</t>
         </is>
       </c>
       <c r="C14" s="3" t="inlineStr">
         <is>
-          <t>10:15-14:00</t>
+          <t>18:00-21:45</t>
         </is>
       </c>
       <c r="D14" s="3" t="n"/>
@@ -3346,12 +3338,12 @@
       </c>
       <c r="B15" s="3" t="inlineStr">
         <is>
-          <t>CUSI QUISPE, ANDREA ESTEFANY</t>
+          <t>BRANCACHO RAMIREZ, BRINDY</t>
         </is>
       </c>
       <c r="C15" s="3" t="inlineStr">
         <is>
-          <t>11:00-14:45</t>
+          <t>11:15-15:00</t>
         </is>
       </c>
       <c r="D15" s="3" t="n"/>
@@ -3366,7 +3358,7 @@
       <c r="A16" s="14" t="n"/>
       <c r="B16" s="3" t="inlineStr">
         <is>
-          <t>NAVARRO MORENO, ARIADNA NAYLEA</t>
+          <t>BONILLA SANCHEZ, RAUL FERNANDO</t>
         </is>
       </c>
       <c r="C16" s="3" t="inlineStr">
@@ -3386,7 +3378,7 @@
       </c>
       <c r="B17" s="3" t="inlineStr">
         <is>
-          <t>BRANCACHO RAMIREZ, BRINDY</t>
+          <t>ROCA IBARAN, MIRLA VALENTINA</t>
         </is>
       </c>
       <c r="C17" s="3" t="inlineStr">
@@ -3406,12 +3398,12 @@
       <c r="A18" s="14" t="n"/>
       <c r="B18" s="3" t="inlineStr">
         <is>
-          <t>BONILLA SANCHEZ, RAUL FERNANDO</t>
+          <t>LIZARME HUINCHO, BRIYITH JASUMI</t>
         </is>
       </c>
       <c r="C18" s="3" t="inlineStr">
         <is>
-          <t>18:00-21:45</t>
+          <t>18:15-22:00</t>
         </is>
       </c>
       <c r="D18" s="3" t="n"/>
@@ -3426,12 +3418,12 @@
       </c>
       <c r="B19" s="3" t="inlineStr">
         <is>
-          <t>ROCA IBARAN, MIRLA VALENTINA</t>
+          <t>CARRIL DARRIGO, RENZO</t>
         </is>
       </c>
       <c r="C19" s="3" t="inlineStr">
         <is>
-          <t>11:15-15:00</t>
+          <t>18:15-22:00</t>
         </is>
       </c>
       <c r="D19" s="3" t="n"/>
@@ -3444,16 +3436,8 @@
     </row>
     <row r="20" ht="19.5" customHeight="1">
       <c r="A20" s="14" t="n"/>
-      <c r="B20" s="3" t="inlineStr">
-        <is>
-          <t>CARRIL DARRIGO, RENZO</t>
-        </is>
-      </c>
-      <c r="C20" s="3" t="inlineStr">
-        <is>
-          <t>18:15-22:00</t>
-        </is>
-      </c>
+      <c r="B20" s="3" t="n"/>
+      <c r="C20" s="3" t="n"/>
       <c r="D20" s="3" t="n"/>
       <c r="E20" s="14" t="n"/>
       <c r="F20" s="3" t="n"/>
@@ -3784,46 +3768,70 @@
       </c>
       <c r="B46" s="3" t="inlineStr">
         <is>
-          <t>MUÑOZ SOTOMAYOR, MIRIAN RAQUEL</t>
+          <t>ALVITE CORNEJO, ANGIE LUCERO</t>
         </is>
       </c>
       <c r="C46" s="3" t="inlineStr">
         <is>
-          <t>13:15-17:00</t>
+          <t>07:00-10:45</t>
         </is>
       </c>
       <c r="D46" s="3" t="n"/>
       <c r="E46" s="14" t="n">
         <v>22</v>
       </c>
-      <c r="F46" s="3" t="n"/>
-      <c r="G46" s="3" t="n"/>
+      <c r="F46" s="3" t="inlineStr">
+        <is>
+          <t>HUANCAS SHUAN, JOSELYN JAZMIN</t>
+        </is>
+      </c>
+      <c r="G46" s="3" t="inlineStr">
+        <is>
+          <t>15:00-18:45</t>
+        </is>
+      </c>
       <c r="H46" s="3" t="n"/>
     </row>
     <row r="47" ht="18.75" customHeight="1">
       <c r="A47" s="14" t="n"/>
       <c r="B47" s="3" t="inlineStr">
         <is>
-          <t>LIZARME HUINCHO, BRIYITH JASUMI</t>
+          <t>SOTO VELAZCO, EMIR ALESSANDRO</t>
         </is>
       </c>
       <c r="C47" s="3" t="inlineStr">
         <is>
-          <t>18:15-22:00</t>
+          <t>11:00-14:45</t>
         </is>
       </c>
       <c r="D47" s="3" t="n"/>
       <c r="E47" s="14" t="n"/>
-      <c r="F47" s="3" t="n"/>
-      <c r="G47" s="3" t="n"/>
+      <c r="F47" s="3" t="inlineStr">
+        <is>
+          <t>POVEA CANTARO, FARID YASSER</t>
+        </is>
+      </c>
+      <c r="G47" s="3" t="inlineStr">
+        <is>
+          <t>18:45-22:30</t>
+        </is>
+      </c>
       <c r="H47" s="3" t="n"/>
     </row>
     <row r="48" ht="18.75" customHeight="1">
       <c r="A48" s="14" t="n">
         <v>23</v>
       </c>
-      <c r="B48" s="3" t="n"/>
-      <c r="C48" s="3" t="n"/>
+      <c r="B48" s="3" t="inlineStr">
+        <is>
+          <t>ZAPATA VILLANUEVA, FIORELLA YASMIN</t>
+        </is>
+      </c>
+      <c r="C48" s="3" t="inlineStr">
+        <is>
+          <t>19:00-22:45</t>
+        </is>
+      </c>
       <c r="D48" s="3" t="n"/>
       <c r="E48" s="14" t="n">
         <v>23</v>
@@ -4027,7 +4035,7 @@
     <row r="2" ht="19.5" customHeight="1">
       <c r="A2" s="14" t="inlineStr">
         <is>
-          <t>FECHA</t>
+          <t>VIERNES 15 DE NOVIEMBRE 2024</t>
         </is>
       </c>
       <c r="B2" s="16" t="n"/>
@@ -4164,12 +4172,12 @@
       </c>
       <c r="B7" s="3" t="inlineStr">
         <is>
-          <t>QUISPE MONDRAGON, JUAN ALFONSO</t>
+          <t>CASAPAICO RIVERA, ENZO MANUEL</t>
         </is>
       </c>
       <c r="C7" s="3" t="inlineStr">
         <is>
-          <t>07:00-10:45</t>
+          <t>08:15-12:00</t>
         </is>
       </c>
       <c r="D7" s="3" t="n"/>
@@ -4178,12 +4186,12 @@
       </c>
       <c r="F7" s="3" t="inlineStr">
         <is>
-          <t>RAMOS TINOCO, JORDAN JAVIER</t>
+          <t>TITO LAURA, NANCY FIORELLA</t>
         </is>
       </c>
       <c r="G7" s="3" t="inlineStr">
         <is>
-          <t>15:30-19:00</t>
+          <t>13:45-19:15</t>
         </is>
       </c>
       <c r="H7" s="3" t="n"/>
@@ -4192,26 +4200,18 @@
       <c r="A8" s="14" t="n"/>
       <c r="B8" s="3" t="inlineStr">
         <is>
-          <t>CUSI QUISPE, ANDREA ESTEFANY</t>
+          <t>NINA OSCCO, FRANCIS GABRIELA</t>
         </is>
       </c>
       <c r="C8" s="3" t="inlineStr">
         <is>
-          <t>11:00-14:45</t>
+          <t>12:15-13:15</t>
         </is>
       </c>
       <c r="D8" s="3" t="n"/>
       <c r="E8" s="14" t="n"/>
-      <c r="F8" s="3" t="inlineStr">
-        <is>
-          <t>HUAMANI LOPEZ, DREYDI BELINDA</t>
-        </is>
-      </c>
-      <c r="G8" s="3" t="inlineStr">
-        <is>
-          <t>19:00-22:45</t>
-        </is>
-      </c>
+      <c r="F8" s="3" t="n"/>
+      <c r="G8" s="3" t="n"/>
       <c r="H8" s="3" t="n"/>
     </row>
     <row r="9" ht="19.5" customHeight="1">
@@ -4220,12 +4220,12 @@
       </c>
       <c r="B9" s="3" t="inlineStr">
         <is>
-          <t>CASAPAICO RIVERA, ENZO MANUEL</t>
+          <t>QUISPE MENDOZA, ANTONY MAURICIO</t>
         </is>
       </c>
       <c r="C9" s="3" t="inlineStr">
         <is>
-          <t>08:15-12:00</t>
+          <t>09:15-13:30</t>
         </is>
       </c>
       <c r="D9" s="3" t="n"/>
@@ -4234,12 +4234,12 @@
       </c>
       <c r="F9" s="3" t="inlineStr">
         <is>
-          <t>TITO LAURA, NANCY FIORELLA</t>
+          <t>INGA DELGADO, CARLOS DANIEL</t>
         </is>
       </c>
       <c r="G9" s="3" t="inlineStr">
         <is>
-          <t>13:45-19:15</t>
+          <t>18:00-21:45</t>
         </is>
       </c>
       <c r="H9" s="3" t="n"/>
@@ -4248,12 +4248,12 @@
       <c r="A10" s="14" t="n"/>
       <c r="B10" s="3" t="inlineStr">
         <is>
-          <t>NINA OSCCO, FRANCIS GABRIELA</t>
+          <t>LEON TICONA, MARIA FERNANDA</t>
         </is>
       </c>
       <c r="C10" s="3" t="inlineStr">
         <is>
-          <t>12:15-13:15</t>
+          <t>14:00-17:45</t>
         </is>
       </c>
       <c r="D10" s="3" t="n"/>
@@ -4268,12 +4268,12 @@
       </c>
       <c r="B11" s="3" t="inlineStr">
         <is>
-          <t>QUISPE MENDOZA, ANTONY MAURICIO</t>
+          <t>SOTO VELAZCO, EMIR ALESSANDRO</t>
         </is>
       </c>
       <c r="C11" s="3" t="inlineStr">
         <is>
-          <t>09:15-13:30</t>
+          <t>09:45-10:00</t>
         </is>
       </c>
       <c r="D11" s="3" t="n"/>
@@ -4282,12 +4282,12 @@
       </c>
       <c r="F11" s="3" t="inlineStr">
         <is>
-          <t>NAVARRO MORENO, ARIADNA NAYLEA</t>
+          <t>MUÑOZ SOTOMAYOR, MIRIAN RAQUEL</t>
         </is>
       </c>
       <c r="G11" s="3" t="inlineStr">
         <is>
-          <t>18:00-21:45</t>
+          <t>14:15-18:00</t>
         </is>
       </c>
       <c r="H11" s="3" t="n"/>
@@ -4296,18 +4296,26 @@
       <c r="A12" s="14" t="n"/>
       <c r="B12" s="3" t="inlineStr">
         <is>
-          <t>LEON TICONA, MARIA FERNANDA</t>
+          <t>IDELFONSO MOTTA, JHOSSEP ANGELO</t>
         </is>
       </c>
       <c r="C12" s="3" t="inlineStr">
         <is>
-          <t>14:00-17:45</t>
+          <t>10:15-14:00</t>
         </is>
       </c>
       <c r="D12" s="3" t="n"/>
       <c r="E12" s="14" t="n"/>
-      <c r="F12" s="3" t="n"/>
-      <c r="G12" s="3" t="n"/>
+      <c r="F12" s="3" t="inlineStr">
+        <is>
+          <t>NAVARRO MORENO, ARIADNA NAYLEA</t>
+        </is>
+      </c>
+      <c r="G12" s="3" t="inlineStr">
+        <is>
+          <t>18:00-21:45</t>
+        </is>
+      </c>
       <c r="H12" s="3" t="n"/>
     </row>
     <row r="13" ht="19.5" customHeight="1">
@@ -4316,12 +4324,12 @@
       </c>
       <c r="B13" s="3" t="inlineStr">
         <is>
-          <t>SOTO VELAZCO, EMIR ALESSANDRO</t>
+          <t>HUAMAN HUAMANI, ALEXIS JAVIER</t>
         </is>
       </c>
       <c r="C13" s="3" t="inlineStr">
         <is>
-          <t>09:45-10:00</t>
+          <t>10:15-14:00</t>
         </is>
       </c>
       <c r="D13" s="3" t="n"/>
@@ -4330,12 +4338,12 @@
       </c>
       <c r="F13" s="3" t="inlineStr">
         <is>
-          <t>MUÑOZ SOTOMAYOR, MIRIAN RAQUEL</t>
+          <t>POVEA CANTARO, FARID YASSER</t>
         </is>
       </c>
       <c r="G13" s="3" t="inlineStr">
         <is>
-          <t>14:15-18:00</t>
+          <t>18:45-22:30</t>
         </is>
       </c>
       <c r="H13" s="3" t="n"/>
@@ -4344,26 +4352,18 @@
       <c r="A14" s="14" t="n"/>
       <c r="B14" s="3" t="inlineStr">
         <is>
-          <t>IDELFONSO MOTTA, JHOSSEP ANGELO</t>
+          <t>GARRIDO SOTO, VICTORIA CELESTE</t>
         </is>
       </c>
       <c r="C14" s="3" t="inlineStr">
         <is>
-          <t>10:15-14:00</t>
+          <t>14:30-18:15</t>
         </is>
       </c>
       <c r="D14" s="3" t="n"/>
       <c r="E14" s="14" t="n"/>
-      <c r="F14" s="3" t="inlineStr">
-        <is>
-          <t>GONZALES OLIVARES, JEFFERSON ISRAEL</t>
-        </is>
-      </c>
-      <c r="G14" s="3" t="inlineStr">
-        <is>
-          <t>18:00-21:45</t>
-        </is>
-      </c>
+      <c r="F14" s="3" t="n"/>
+      <c r="G14" s="3" t="n"/>
       <c r="H14" s="3" t="n"/>
     </row>
     <row r="15" ht="19.5" customHeight="1">
@@ -4372,40 +4372,32 @@
       </c>
       <c r="B15" s="3" t="inlineStr">
         <is>
-          <t>HUAMAN HUAMANI, ALEXIS JAVIER</t>
+          <t>QUIQUIA MALLQUI, CYNTHIA ANGELLINE</t>
         </is>
       </c>
       <c r="C15" s="3" t="inlineStr">
         <is>
-          <t>10:15-14:00</t>
+          <t>10:30-14:15</t>
         </is>
       </c>
       <c r="D15" s="3" t="n"/>
       <c r="E15" s="14" t="n">
         <v>6</v>
       </c>
-      <c r="F15" s="3" t="inlineStr">
-        <is>
-          <t>POVEA CANTARO, FARID YASSER</t>
-        </is>
-      </c>
-      <c r="G15" s="3" t="inlineStr">
-        <is>
-          <t>18:45-22:30</t>
-        </is>
-      </c>
+      <c r="F15" s="3" t="n"/>
+      <c r="G15" s="3" t="n"/>
       <c r="H15" s="3" t="n"/>
     </row>
     <row r="16" ht="19.5" customHeight="1">
       <c r="A16" s="14" t="n"/>
       <c r="B16" s="3" t="inlineStr">
         <is>
-          <t>GARRIDO SOTO, VICTORIA CELESTE</t>
+          <t>SICHA JORGE, JOSE ANGELO</t>
         </is>
       </c>
       <c r="C16" s="3" t="inlineStr">
         <is>
-          <t>14:30-18:15</t>
+          <t>16:15-20:00</t>
         </is>
       </c>
       <c r="D16" s="3" t="n"/>
@@ -4420,12 +4412,12 @@
       </c>
       <c r="B17" s="3" t="inlineStr">
         <is>
-          <t>QUIQUIA MALLQUI, CYNTHIA ANGELLINE</t>
+          <t>BRANCACHO RAMIREZ, BRINDY</t>
         </is>
       </c>
       <c r="C17" s="3" t="inlineStr">
         <is>
-          <t>10:30-14:15</t>
+          <t>11:00-14:45</t>
         </is>
       </c>
       <c r="D17" s="3" t="n"/>
@@ -4440,12 +4432,12 @@
       <c r="A18" s="14" t="n"/>
       <c r="B18" s="3" t="inlineStr">
         <is>
-          <t>SICHA JORGE, JOSE ANGELO</t>
+          <t>PEREZ GORMAS, ANTHONY</t>
         </is>
       </c>
       <c r="C18" s="3" t="inlineStr">
         <is>
-          <t>16:15-20:00</t>
+          <t>17:00-20:45</t>
         </is>
       </c>
       <c r="D18" s="3" t="n"/>
@@ -4460,12 +4452,12 @@
       </c>
       <c r="B19" s="3" t="inlineStr">
         <is>
-          <t>BRANCACHO RAMIREZ, BRINDY</t>
+          <t>ROCA IBARAN, MIRLA VALENTINA</t>
         </is>
       </c>
       <c r="C19" s="3" t="inlineStr">
         <is>
-          <t>11:00-14:45</t>
+          <t>11:15-15:00</t>
         </is>
       </c>
       <c r="D19" s="3" t="n"/>
@@ -4480,12 +4472,12 @@
       <c r="A20" s="14" t="n"/>
       <c r="B20" s="3" t="inlineStr">
         <is>
-          <t>LIZARME HUINCHO, BRIYITH JASUMI</t>
+          <t>ZAPATA VILLANUEVA, FIORELLA YASMIN</t>
         </is>
       </c>
       <c r="C20" s="3" t="inlineStr">
         <is>
-          <t>17:00-20:45</t>
+          <t>17:30-21:15</t>
         </is>
       </c>
       <c r="D20" s="3" t="n"/>
@@ -4500,12 +4492,12 @@
       </c>
       <c r="B21" s="3" t="inlineStr">
         <is>
-          <t>ROCA IBARAN, MIRLA VALENTINA</t>
+          <t>YANQUI BRAVO, MIRIAN LUZ</t>
         </is>
       </c>
       <c r="C21" s="3" t="inlineStr">
         <is>
-          <t>11:15-15:00</t>
+          <t>11:45-15:30</t>
         </is>
       </c>
       <c r="D21" s="3" t="n"/>
@@ -4520,12 +4512,12 @@
       <c r="A22" s="14" t="n"/>
       <c r="B22" s="3" t="inlineStr">
         <is>
-          <t>PEREZ GORMAS, ANTHONY</t>
+          <t>GONZALES OLIVARES, JEFFERSON ISRAEL</t>
         </is>
       </c>
       <c r="C22" s="3" t="inlineStr">
         <is>
-          <t>17:00-20:45</t>
+          <t>18:00-21:45</t>
         </is>
       </c>
       <c r="D22" s="3" t="n"/>
@@ -4540,12 +4532,12 @@
       </c>
       <c r="B23" s="3" t="inlineStr">
         <is>
-          <t>ZAPATA VILLANUEVA, FIORELLA YASMIN</t>
+          <t>HUAMANI LOPEZ, DREYDI BELINDA</t>
         </is>
       </c>
       <c r="C23" s="3" t="inlineStr">
         <is>
-          <t>17:30-21:15</t>
+          <t>19:00-22:45</t>
         </is>
       </c>
       <c r="D23" s="3" t="n"/>
@@ -4810,38 +4802,54 @@
       </c>
       <c r="B44" s="3" t="inlineStr">
         <is>
-          <t>JIMENEZ TORERO, ASTRID GERALDINE</t>
+          <t>QUISPE MONDRAGON, JUAN ALFONSO</t>
         </is>
       </c>
       <c r="C44" s="3" t="inlineStr">
         <is>
-          <t>08:00-17:00</t>
+          <t>07:00-10:45</t>
         </is>
       </c>
       <c r="D44" s="3" t="n"/>
       <c r="E44" s="14" t="n">
         <v>21</v>
       </c>
-      <c r="F44" s="3" t="n"/>
-      <c r="G44" s="3" t="n"/>
+      <c r="F44" s="3" t="inlineStr">
+        <is>
+          <t>RAMOS TINOCO, JORDAN JAVIER</t>
+        </is>
+      </c>
+      <c r="G44" s="3" t="inlineStr">
+        <is>
+          <t>15:30-19:00</t>
+        </is>
+      </c>
       <c r="H44" s="3" t="n"/>
     </row>
     <row r="45" ht="18.75" customHeight="1">
       <c r="A45" s="14" t="n"/>
       <c r="B45" s="3" t="inlineStr">
         <is>
-          <t>ROA ZARATE, ELIZABETH LUCY</t>
+          <t>CUSI QUISPE, ANDREA ESTEFANY</t>
         </is>
       </c>
       <c r="C45" s="3" t="inlineStr">
         <is>
-          <t>19:00-22:45</t>
+          <t>11:00-14:45</t>
         </is>
       </c>
       <c r="D45" s="3" t="n"/>
       <c r="E45" s="14" t="n"/>
-      <c r="F45" s="3" t="n"/>
-      <c r="G45" s="3" t="n"/>
+      <c r="F45" s="3" t="inlineStr">
+        <is>
+          <t>ROA ZARATE, ELIZABETH LUCY</t>
+        </is>
+      </c>
+      <c r="G45" s="3" t="inlineStr">
+        <is>
+          <t>19:00-22:45</t>
+        </is>
+      </c>
       <c r="H45" s="3" t="n"/>
     </row>
     <row r="46" ht="18.75" customHeight="1">
@@ -4850,12 +4858,12 @@
       </c>
       <c r="B46" s="3" t="inlineStr">
         <is>
-          <t>YANQUI BRAVO, MIRIAN LUZ</t>
+          <t>JIMENEZ TORERO, ASTRID GERALDINE</t>
         </is>
       </c>
       <c r="C46" s="3" t="inlineStr">
         <is>
-          <t>11:45-15:30</t>
+          <t>08:00-17:00</t>
         </is>
       </c>
       <c r="D46" s="3" t="n"/>
@@ -4870,12 +4878,12 @@
       <c r="A47" s="14" t="n"/>
       <c r="B47" s="3" t="inlineStr">
         <is>
-          <t>INGA DELGADO, CARLOS DANIEL</t>
+          <t>LIZARME HUINCHO, BRIYITH JASUMI</t>
         </is>
       </c>
       <c r="C47" s="3" t="inlineStr">
         <is>
-          <t>18:00-21:45</t>
+          <t>17:00-20:45</t>
         </is>
       </c>
       <c r="D47" s="3" t="n"/>
@@ -4888,8 +4896,16 @@
       <c r="A48" s="14" t="n">
         <v>23</v>
       </c>
-      <c r="B48" s="3" t="n"/>
-      <c r="C48" s="3" t="n"/>
+      <c r="B48" s="3" t="inlineStr">
+        <is>
+          <t>HUAMANI LOPEZ, DREYDI BELINDA</t>
+        </is>
+      </c>
+      <c r="C48" s="3" t="inlineStr">
+        <is>
+          <t>19:00-22:45</t>
+        </is>
+      </c>
       <c r="D48" s="3" t="n"/>
       <c r="E48" s="14" t="n">
         <v>23</v>
@@ -5093,7 +5109,7 @@
     <row r="2" ht="19.5" customHeight="1">
       <c r="A2" s="14" t="inlineStr">
         <is>
-          <t>FECHA</t>
+          <t>SÁBADO 16 DE NOVIEMBRE 2024</t>
         </is>
       </c>
       <c r="B2" s="16" t="n"/>
@@ -5222,54 +5238,38 @@
       </c>
       <c r="B7" s="3" t="inlineStr">
         <is>
-          <t>GONZALES OLIVARES, JEFFERSON ISRAEL</t>
+          <t>BARRIENTOS JERI, MILAGROS NICOL</t>
         </is>
       </c>
       <c r="C7" s="3" t="inlineStr">
         <is>
-          <t>07:00-10:45</t>
+          <t>08:30-17:30</t>
         </is>
       </c>
       <c r="D7" s="3" t="n"/>
       <c r="E7" s="14" t="n">
         <v>2</v>
       </c>
-      <c r="F7" s="3" t="inlineStr">
-        <is>
-          <t>LIZARME HUINCHO, BRIYITH JASUMI</t>
-        </is>
-      </c>
-      <c r="G7" s="3" t="inlineStr">
-        <is>
-          <t>14:30-18:15</t>
-        </is>
-      </c>
+      <c r="F7" s="3" t="n"/>
+      <c r="G7" s="3" t="n"/>
       <c r="H7" s="3" t="n"/>
     </row>
     <row r="8" ht="19.5" customHeight="1">
       <c r="A8" s="14" t="n"/>
       <c r="B8" s="3" t="inlineStr">
         <is>
-          <t>CASAPAICO RIVERA, ENZO MANUEL</t>
+          <t>ROA ZARATE, ELIZABETH LUCY</t>
         </is>
       </c>
       <c r="C8" s="3" t="inlineStr">
         <is>
-          <t>10:45-14:30</t>
+          <t>17:45-21:30</t>
         </is>
       </c>
       <c r="D8" s="3" t="n"/>
       <c r="E8" s="14" t="n"/>
-      <c r="F8" s="3" t="inlineStr">
-        <is>
-          <t>HUAMANI LOPEZ, DREYDI BELINDA</t>
-        </is>
-      </c>
-      <c r="G8" s="3" t="inlineStr">
-        <is>
-          <t>18:15-22:00</t>
-        </is>
-      </c>
+      <c r="F8" s="3" t="n"/>
+      <c r="G8" s="3" t="n"/>
       <c r="H8" s="3" t="n"/>
     </row>
     <row r="9" ht="19.5" customHeight="1">
@@ -5278,12 +5278,12 @@
       </c>
       <c r="B9" s="3" t="inlineStr">
         <is>
-          <t>SOTO VELAZCO, EMIR ALESSANDRO</t>
+          <t>HUAYANAY VELASCO, ATHINA</t>
         </is>
       </c>
       <c r="C9" s="3" t="inlineStr">
         <is>
-          <t>08:15-12:00</t>
+          <t>09:00-12:45</t>
         </is>
       </c>
       <c r="D9" s="3" t="n"/>
@@ -5298,12 +5298,12 @@
       <c r="A10" s="14" t="n"/>
       <c r="B10" s="3" t="inlineStr">
         <is>
-          <t>RAMOS TINOCO, JORDAN JAVIER</t>
+          <t>TITO LAURA, NANCY FIORELLA</t>
         </is>
       </c>
       <c r="C10" s="3" t="inlineStr">
         <is>
-          <t>12:00-21:00</t>
+          <t>12:45-21:45</t>
         </is>
       </c>
       <c r="D10" s="3" t="n"/>
@@ -5318,12 +5318,12 @@
       </c>
       <c r="B11" s="3" t="inlineStr">
         <is>
-          <t>BARRIENTOS JERI, MILAGROS NICOL</t>
+          <t>MUÑOZ SOTOMAYOR, MIRIAN RAQUEL</t>
         </is>
       </c>
       <c r="C11" s="3" t="inlineStr">
         <is>
-          <t>08:30-17:30</t>
+          <t>09:45-13:30</t>
         </is>
       </c>
       <c r="D11" s="3" t="n"/>
@@ -5338,12 +5338,12 @@
       <c r="A12" s="14" t="n"/>
       <c r="B12" s="3" t="inlineStr">
         <is>
-          <t>BONILLA SANCHEZ, RAUL FERNANDO</t>
+          <t>JIMENEZ TORERO, ASTRID GERALDINE</t>
         </is>
       </c>
       <c r="C12" s="3" t="inlineStr">
         <is>
-          <t>18:00-21:45</t>
+          <t>14:15-23:15</t>
         </is>
       </c>
       <c r="D12" s="3" t="n"/>
@@ -5358,32 +5358,40 @@
       </c>
       <c r="B13" s="3" t="inlineStr">
         <is>
-          <t>HUAYANAY VELASCO, ATHINA</t>
+          <t>BRANCACHO RAMIREZ, BRINDY</t>
         </is>
       </c>
       <c r="C13" s="3" t="inlineStr">
         <is>
-          <t>09:00-12:45</t>
+          <t>10:15-14:00</t>
         </is>
       </c>
       <c r="D13" s="3" t="n"/>
       <c r="E13" s="14" t="n">
         <v>5</v>
       </c>
-      <c r="F13" s="3" t="n"/>
-      <c r="G13" s="3" t="n"/>
+      <c r="F13" s="3" t="inlineStr">
+        <is>
+          <t>NAVARRO MORENO, ARIADNA NAYLEA</t>
+        </is>
+      </c>
+      <c r="G13" s="3" t="inlineStr">
+        <is>
+          <t>19:00-22:15</t>
+        </is>
+      </c>
       <c r="H13" s="3" t="n"/>
     </row>
     <row r="14" ht="19.5" customHeight="1">
       <c r="A14" s="14" t="n"/>
       <c r="B14" s="3" t="inlineStr">
         <is>
-          <t>TITO LAURA, NANCY FIORELLA</t>
+          <t>DEL AGUILA MURAYARI, DARLA</t>
         </is>
       </c>
       <c r="C14" s="3" t="inlineStr">
         <is>
-          <t>12:45-21:45</t>
+          <t>14:15-19:00</t>
         </is>
       </c>
       <c r="D14" s="3" t="n"/>
@@ -5398,12 +5406,12 @@
       </c>
       <c r="B15" s="3" t="inlineStr">
         <is>
-          <t>MUÑOZ SOTOMAYOR, MIRIAN RAQUEL</t>
+          <t>CUSI QUISPE, ANDREA ESTEFANY</t>
         </is>
       </c>
       <c r="C15" s="3" t="inlineStr">
         <is>
-          <t>09:45-13:30</t>
+          <t>10:30-14:15</t>
         </is>
       </c>
       <c r="D15" s="3" t="n"/>
@@ -5412,12 +5420,12 @@
       </c>
       <c r="F15" s="3" t="inlineStr">
         <is>
-          <t>NAVARRO MORENO, ARIADNA NAYLEA</t>
+          <t>HUANCAS SHUAN, JOSELYN JAZMIN</t>
         </is>
       </c>
       <c r="G15" s="3" t="inlineStr">
         <is>
-          <t>19:00-22:15</t>
+          <t>19:00-22:45</t>
         </is>
       </c>
       <c r="H15" s="3" t="n"/>
@@ -5426,12 +5434,12 @@
       <c r="A16" s="14" t="n"/>
       <c r="B16" s="3" t="inlineStr">
         <is>
-          <t>DEL AGUILA MURAYARI, DARLA</t>
+          <t>CARRIL DARRIGO, RENZO</t>
         </is>
       </c>
       <c r="C16" s="3" t="inlineStr">
         <is>
-          <t>14:15-19:00</t>
+          <t>14:45-18:30</t>
         </is>
       </c>
       <c r="D16" s="3" t="n"/>
@@ -5446,40 +5454,32 @@
       </c>
       <c r="B17" s="3" t="inlineStr">
         <is>
-          <t>BRANCACHO RAMIREZ, BRINDY</t>
+          <t>RUIZ SANTOS, CIELO CRISTHINA</t>
         </is>
       </c>
       <c r="C17" s="3" t="inlineStr">
         <is>
-          <t>10:15-14:00</t>
+          <t>10:45-14:30</t>
         </is>
       </c>
       <c r="D17" s="3" t="n"/>
       <c r="E17" s="14" t="n">
         <v>7</v>
       </c>
-      <c r="F17" s="3" t="inlineStr">
-        <is>
-          <t>HUANCAS SHUAN, JOSELYN JAZMIN</t>
-        </is>
-      </c>
-      <c r="G17" s="3" t="inlineStr">
-        <is>
-          <t>19:00-22:45</t>
-        </is>
-      </c>
+      <c r="F17" s="3" t="n"/>
+      <c r="G17" s="3" t="n"/>
       <c r="H17" s="3" t="n"/>
     </row>
     <row r="18" ht="19.5" customHeight="1">
       <c r="A18" s="14" t="n"/>
       <c r="B18" s="3" t="inlineStr">
         <is>
-          <t>CARRIL DARRIGO, RENZO</t>
+          <t>SICHA JORGE, JOSE ANGELO</t>
         </is>
       </c>
       <c r="C18" s="3" t="inlineStr">
         <is>
-          <t>14:45-18:30</t>
+          <t>15:00-18:45</t>
         </is>
       </c>
       <c r="D18" s="3" t="n"/>
@@ -5494,12 +5494,12 @@
       </c>
       <c r="B19" s="3" t="inlineStr">
         <is>
-          <t>CUSI QUISPE, ANDREA ESTEFANY</t>
+          <t>IDELFONSO MOTTA, JHOSSEP ANGELO</t>
         </is>
       </c>
       <c r="C19" s="3" t="inlineStr">
         <is>
-          <t>10:30-14:15</t>
+          <t>11:00-14:45</t>
         </is>
       </c>
       <c r="D19" s="3" t="n"/>
@@ -5514,7 +5514,7 @@
       <c r="A20" s="14" t="n"/>
       <c r="B20" s="3" t="inlineStr">
         <is>
-          <t>SICHA JORGE, JOSE ANGELO</t>
+          <t>PEREZ GORMAS, ANTHONY</t>
         </is>
       </c>
       <c r="C20" s="3" t="inlineStr">
@@ -5534,12 +5534,12 @@
       </c>
       <c r="B21" s="3" t="inlineStr">
         <is>
-          <t>RUIZ SANTOS, CIELO CRISTHINA</t>
+          <t>PIÑA SHUPINGAHUA, SANDRA</t>
         </is>
       </c>
       <c r="C21" s="3" t="inlineStr">
         <is>
-          <t>10:45-14:30</t>
+          <t>11:00-14:45</t>
         </is>
       </c>
       <c r="D21" s="3" t="n"/>
@@ -5554,12 +5554,12 @@
       <c r="A22" s="14" t="n"/>
       <c r="B22" s="3" t="inlineStr">
         <is>
-          <t>PEREZ GORMAS, ANTHONY</t>
+          <t>BONILLA SANCHEZ, RAUL FERNANDO</t>
         </is>
       </c>
       <c r="C22" s="3" t="inlineStr">
         <is>
-          <t>15:00-18:45</t>
+          <t>18:00-21:45</t>
         </is>
       </c>
       <c r="D22" s="3" t="n"/>
@@ -5574,12 +5574,12 @@
       </c>
       <c r="B23" s="3" t="inlineStr">
         <is>
-          <t>IDELFONSO MOTTA, JHOSSEP ANGELO</t>
+          <t>QUIQUIA MALLQUI, CYNTHIA ANGELLINE</t>
         </is>
       </c>
       <c r="C23" s="3" t="inlineStr">
         <is>
-          <t>11:00-14:45</t>
+          <t>11:15-15:00</t>
         </is>
       </c>
       <c r="D23" s="3" t="n"/>
@@ -5594,12 +5594,12 @@
       <c r="A24" s="14" t="n"/>
       <c r="B24" s="3" t="inlineStr">
         <is>
-          <t>LEON TICONA, MARIA FERNANDA</t>
+          <t>ZAPATA VILLANUEVA, FIORELLA YASMIN</t>
         </is>
       </c>
       <c r="C24" s="3" t="inlineStr">
         <is>
-          <t>17:00-20:45</t>
+          <t>18:00-21:45</t>
         </is>
       </c>
       <c r="D24" s="3" t="n"/>
@@ -5614,12 +5614,12 @@
       </c>
       <c r="B25" s="3" t="inlineStr">
         <is>
-          <t>PIÑA SHUPINGAHUA, SANDRA</t>
+          <t>NINA OSCCO, FRANCIS GABRIELA</t>
         </is>
       </c>
       <c r="C25" s="3" t="inlineStr">
         <is>
-          <t>11:00-14:45</t>
+          <t>11:30-20:15</t>
         </is>
       </c>
       <c r="D25" s="3" t="n"/>
@@ -5632,16 +5632,8 @@
     </row>
     <row r="26" ht="18.75" customHeight="1">
       <c r="A26" s="14" t="n"/>
-      <c r="B26" s="3" t="inlineStr">
-        <is>
-          <t>ZAPATA VILLANUEVA, FIORELLA YASMIN</t>
-        </is>
-      </c>
-      <c r="C26" s="3" t="inlineStr">
-        <is>
-          <t>18:00-21:45</t>
-        </is>
-      </c>
+      <c r="B26" s="3" t="n"/>
+      <c r="C26" s="3" t="n"/>
       <c r="D26" s="3" t="n"/>
       <c r="E26" s="14" t="n"/>
       <c r="F26" s="3" t="n"/>
@@ -5654,12 +5646,12 @@
       </c>
       <c r="B27" s="3" t="inlineStr">
         <is>
-          <t>QUIQUIA MALLQUI, CYNTHIA ANGELLINE</t>
+          <t>RAMOS TINOCO, JORDAN JAVIER</t>
         </is>
       </c>
       <c r="C27" s="3" t="inlineStr">
         <is>
-          <t>11:15-15:00</t>
+          <t>12:00-21:00</t>
         </is>
       </c>
       <c r="D27" s="3" t="n"/>
@@ -5684,16 +5676,8 @@
       <c r="A29" s="14" t="n">
         <v>13</v>
       </c>
-      <c r="B29" s="3" t="inlineStr">
-        <is>
-          <t>NINA OSCCO, FRANCIS GABRIELA</t>
-        </is>
-      </c>
-      <c r="C29" s="3" t="inlineStr">
-        <is>
-          <t>11:30-20:15</t>
-        </is>
-      </c>
+      <c r="B29" s="3" t="n"/>
+      <c r="C29" s="3" t="n"/>
       <c r="D29" s="3" t="n"/>
       <c r="E29" s="14" t="n">
         <v>13</v>
@@ -5876,30 +5860,54 @@
       </c>
       <c r="B44" s="3" t="inlineStr">
         <is>
-          <t>JIMENEZ TORERO, ASTRID GERALDINE</t>
+          <t>GONZALES OLIVARES, JEFFERSON ISRAEL</t>
         </is>
       </c>
       <c r="C44" s="3" t="inlineStr">
         <is>
-          <t>14:15-23:15</t>
+          <t>07:00-10:45</t>
         </is>
       </c>
       <c r="D44" s="3" t="n"/>
       <c r="E44" s="14" t="n">
         <v>21</v>
       </c>
-      <c r="F44" s="3" t="n"/>
-      <c r="G44" s="3" t="n"/>
+      <c r="F44" s="3" t="inlineStr">
+        <is>
+          <t>LIZARME HUINCHO, BRIYITH JASUMI</t>
+        </is>
+      </c>
+      <c r="G44" s="3" t="inlineStr">
+        <is>
+          <t>14:30-18:15</t>
+        </is>
+      </c>
       <c r="H44" s="3" t="n"/>
     </row>
     <row r="45" ht="18.75" customHeight="1">
       <c r="A45" s="14" t="n"/>
-      <c r="B45" s="3" t="n"/>
-      <c r="C45" s="3" t="n"/>
+      <c r="B45" s="3" t="inlineStr">
+        <is>
+          <t>CASAPAICO RIVERA, ENZO MANUEL</t>
+        </is>
+      </c>
+      <c r="C45" s="3" t="inlineStr">
+        <is>
+          <t>10:45-14:30</t>
+        </is>
+      </c>
       <c r="D45" s="3" t="n"/>
       <c r="E45" s="14" t="n"/>
-      <c r="F45" s="3" t="n"/>
-      <c r="G45" s="3" t="n"/>
+      <c r="F45" s="3" t="inlineStr">
+        <is>
+          <t>HUAMANI LOPEZ, DREYDI BELINDA</t>
+        </is>
+      </c>
+      <c r="G45" s="3" t="inlineStr">
+        <is>
+          <t>18:15-22:00</t>
+        </is>
+      </c>
       <c r="H45" s="3" t="n"/>
     </row>
     <row r="46" ht="18.75" customHeight="1">
@@ -5908,32 +5916,40 @@
       </c>
       <c r="B46" s="3" t="inlineStr">
         <is>
-          <t>YANQUI BRAVO, MIRIAN LUZ</t>
+          <t>SOTO VELAZCO, EMIR ALESSANDRO</t>
         </is>
       </c>
       <c r="C46" s="3" t="inlineStr">
         <is>
-          <t>12:00-15:45</t>
+          <t>08:15-12:00</t>
         </is>
       </c>
       <c r="D46" s="3" t="n"/>
       <c r="E46" s="14" t="n">
         <v>22</v>
       </c>
-      <c r="F46" s="3" t="n"/>
-      <c r="G46" s="3" t="n"/>
+      <c r="F46" s="3" t="inlineStr">
+        <is>
+          <t>LEON TICONA, MARIA FERNANDA</t>
+        </is>
+      </c>
+      <c r="G46" s="3" t="inlineStr">
+        <is>
+          <t>17:00-20:45</t>
+        </is>
+      </c>
       <c r="H46" s="3" t="n"/>
     </row>
     <row r="47" ht="18.75" customHeight="1">
       <c r="A47" s="14" t="n"/>
       <c r="B47" s="3" t="inlineStr">
         <is>
-          <t>ROA ZARATE, ELIZABETH LUCY</t>
+          <t>YANQUI BRAVO, MIRIAN LUZ</t>
         </is>
       </c>
       <c r="C47" s="3" t="inlineStr">
         <is>
-          <t>17:45-21:30</t>
+          <t>12:00-15:45</t>
         </is>
       </c>
       <c r="D47" s="3" t="n"/>
@@ -5946,8 +5962,16 @@
       <c r="A48" s="14" t="n">
         <v>23</v>
       </c>
-      <c r="B48" s="3" t="n"/>
-      <c r="C48" s="3" t="n"/>
+      <c r="B48" s="3" t="inlineStr">
+        <is>
+          <t>JIMENEZ TORERO, ASTRID GERALDINE</t>
+        </is>
+      </c>
+      <c r="C48" s="3" t="inlineStr">
+        <is>
+          <t>14:15-23:15</t>
+        </is>
+      </c>
       <c r="D48" s="3" t="n"/>
       <c r="E48" s="14" t="n">
         <v>23</v>
@@ -6151,7 +6175,7 @@
     <row r="2" ht="19.5" customHeight="1">
       <c r="A2" s="14" t="inlineStr">
         <is>
-          <t>FECHA</t>
+          <t>DOMINGO 17 DE NOVIEMBRE 2024</t>
         </is>
       </c>
       <c r="B2" s="16" t="n"/>
@@ -6228,7 +6252,7 @@
       </c>
       <c r="F4" s="8" t="inlineStr">
         <is>
-          <t>(T) GARRIDO SOTO, VICTORIA CELESTE</t>
+          <t>(T) QUISPE MENDOZA, ANTONY MAURICIO</t>
         </is>
       </c>
       <c r="G4" s="8" t="inlineStr">
@@ -6280,40 +6304,32 @@
       </c>
       <c r="B7" s="3" t="inlineStr">
         <is>
-          <t>HUANCAS SHUAN, JOSELYN JAZMIN</t>
+          <t>CUSI QUISPE, ANDREA ESTEFANY</t>
         </is>
       </c>
       <c r="C7" s="3" t="inlineStr">
         <is>
-          <t>07:00-10:45</t>
+          <t>08:15-12:00</t>
         </is>
       </c>
       <c r="D7" s="3" t="n"/>
       <c r="E7" s="14" t="n">
         <v>2</v>
       </c>
-      <c r="F7" s="3" t="inlineStr">
-        <is>
-          <t>TITO LAURA, NANCY FIORELLA</t>
-        </is>
-      </c>
-      <c r="G7" s="3" t="inlineStr">
-        <is>
-          <t>14:30-23:30</t>
-        </is>
-      </c>
+      <c r="F7" s="3" t="n"/>
+      <c r="G7" s="3" t="n"/>
       <c r="H7" s="3" t="n"/>
     </row>
     <row r="8" ht="19.5" customHeight="1">
       <c r="A8" s="14" t="n"/>
       <c r="B8" s="3" t="inlineStr">
         <is>
-          <t>HUAYANAY VELASCO, ATHINA</t>
+          <t>DEL AGUILA MURAYARI, DARLA</t>
         </is>
       </c>
       <c r="C8" s="3" t="inlineStr">
         <is>
-          <t>10:45-14:30</t>
+          <t>12:00-21:00</t>
         </is>
       </c>
       <c r="D8" s="3" t="n"/>
@@ -6328,12 +6344,12 @@
       </c>
       <c r="B9" s="3" t="inlineStr">
         <is>
-          <t>CUSI QUISPE, ANDREA ESTEFANY</t>
+          <t>JIMENEZ TORERO, ASTRID GERALDINE</t>
         </is>
       </c>
       <c r="C9" s="3" t="inlineStr">
         <is>
-          <t>08:15-12:00</t>
+          <t>08:30-17:30</t>
         </is>
       </c>
       <c r="D9" s="3" t="n"/>
@@ -6348,12 +6364,12 @@
       <c r="A10" s="14" t="n"/>
       <c r="B10" s="3" t="inlineStr">
         <is>
-          <t>DEL AGUILA MURAYARI, DARLA</t>
+          <t>IDELFONSO MOTTA, JHOSSEP ANGELO</t>
         </is>
       </c>
       <c r="C10" s="3" t="inlineStr">
         <is>
-          <t>12:00-21:00</t>
+          <t>17:30-21:15</t>
         </is>
       </c>
       <c r="D10" s="3" t="n"/>
@@ -6470,12 +6486,12 @@
       </c>
       <c r="F15" s="3" t="inlineStr">
         <is>
-          <t>GARRIDO SOTO, VICTORIA CELESTE</t>
+          <t>HUAMANI LOPEZ, DREYDI BELINDA</t>
         </is>
       </c>
       <c r="G15" s="3" t="inlineStr">
         <is>
-          <t>19:00-21:30</t>
+          <t>19:00-22:45</t>
         </is>
       </c>
       <c r="H15" s="3" t="n"/>
@@ -6668,16 +6684,8 @@
       <c r="E25" s="14" t="n">
         <v>11</v>
       </c>
-      <c r="F25" s="3" t="inlineStr">
-        <is>
-          <t>HUAMANI LOPEZ, DREYDI BELINDA</t>
-        </is>
-      </c>
-      <c r="G25" s="3" t="inlineStr">
-        <is>
-          <t>19:00-22:45</t>
-        </is>
-      </c>
+      <c r="F25" s="3" t="n"/>
+      <c r="G25" s="3" t="n"/>
       <c r="H25" s="3" t="n"/>
     </row>
     <row r="26" ht="18.75" customHeight="1">
@@ -6741,7 +6749,7 @@
       </c>
       <c r="C29" s="3" t="inlineStr">
         <is>
-          <t>13:45-22:45</t>
+          <t>13:45-21:30</t>
         </is>
       </c>
       <c r="D29" s="3" t="n"/>
@@ -6952,8 +6960,16 @@
     </row>
     <row r="45" ht="18.75" customHeight="1">
       <c r="A45" s="14" t="n"/>
-      <c r="B45" s="3" t="n"/>
-      <c r="C45" s="3" t="n"/>
+      <c r="B45" s="3" t="inlineStr">
+        <is>
+          <t>GARRIDO SOTO, VICTORIA CELESTE</t>
+        </is>
+      </c>
+      <c r="C45" s="3" t="inlineStr">
+        <is>
+          <t>19:00-22:45</t>
+        </is>
+      </c>
       <c r="D45" s="3" t="n"/>
       <c r="E45" s="14" t="n"/>
       <c r="F45" s="3" t="n"/>
@@ -6966,32 +6982,40 @@
       </c>
       <c r="B46" s="3" t="inlineStr">
         <is>
-          <t>JIMENEZ TORERO, ASTRID GERALDINE</t>
+          <t>HUANCAS SHUAN, JOSELYN JAZMIN</t>
         </is>
       </c>
       <c r="C46" s="3" t="inlineStr">
         <is>
-          <t>08:30-17:30</t>
+          <t>07:00-10:45</t>
         </is>
       </c>
       <c r="D46" s="3" t="n"/>
       <c r="E46" s="14" t="n">
         <v>22</v>
       </c>
-      <c r="F46" s="3" t="n"/>
-      <c r="G46" s="3" t="n"/>
+      <c r="F46" s="3" t="inlineStr">
+        <is>
+          <t>TITO LAURA, NANCY FIORELLA</t>
+        </is>
+      </c>
+      <c r="G46" s="3" t="inlineStr">
+        <is>
+          <t>14:30-23:30</t>
+        </is>
+      </c>
       <c r="H46" s="3" t="n"/>
     </row>
     <row r="47" ht="18.75" customHeight="1">
       <c r="A47" s="14" t="n"/>
       <c r="B47" s="3" t="inlineStr">
         <is>
-          <t>IDELFONSO MOTTA, JHOSSEP ANGELO</t>
+          <t>HUAYANAY VELASCO, ATHINA</t>
         </is>
       </c>
       <c r="C47" s="3" t="inlineStr">
         <is>
-          <t>17:30-21:15</t>
+          <t>10:45-14:30</t>
         </is>
       </c>
       <c r="D47" s="3" t="n"/>

</xml_diff>

<commit_message>
im back to func. items op. 1
</commit_message>
<xml_diff>
--- a/PlantillaSemanal_Exportada.xlsx
+++ b/PlantillaSemanal_Exportada.xlsx
@@ -696,12 +696,12 @@
       </c>
       <c r="F4" s="8" t="inlineStr">
         <is>
-          <t>LEON TICONA, MARIA FERNANDA</t>
+          <t>ALARCON SANDOVAL, ADRIANA FERNANDA</t>
         </is>
       </c>
       <c r="G4" s="8" t="inlineStr">
         <is>
-          <t>14:30-18:15</t>
+          <t>16:30-20:15</t>
         </is>
       </c>
       <c r="H4" s="8" t="n"/>
@@ -710,24 +710,24 @@
       <c r="A5" s="11" t="n"/>
       <c r="B5" s="12" t="inlineStr">
         <is>
-          <t>(T) JIMENEZ VERGARA, ADRIAN MARCELO</t>
+          <t>TARDILLO COPA, YOVANNA MELISSA</t>
         </is>
       </c>
       <c r="C5" s="12" t="inlineStr">
         <is>
-          <t>10:00-12:30</t>
+          <t>10:00-13:45</t>
         </is>
       </c>
       <c r="D5" s="12" t="n"/>
       <c r="E5" s="11" t="n"/>
       <c r="F5" s="12" t="inlineStr">
         <is>
-          <t>ALARCON SANDOVAL, ADRIANA FERNANDA</t>
+          <t>(T) JIMENEZ TORERO, ASTRID GERALDINE</t>
         </is>
       </c>
       <c r="G5" s="12" t="inlineStr">
         <is>
-          <t>18:00-21:45</t>
+          <t>20:00-22:45</t>
         </is>
       </c>
       <c r="H5" s="12" t="n"/>
@@ -736,26 +736,18 @@
       <c r="A6" s="9" t="n"/>
       <c r="B6" s="10" t="inlineStr">
         <is>
-          <t>(T) BRANCACHO RAMIREZ, BRINDY</t>
+          <t>(T) ALVITE CORNEJO, ANGIE LUCERO</t>
         </is>
       </c>
       <c r="C6" s="10" t="inlineStr">
         <is>
-          <t>12:15-14:45</t>
+          <t>13:30-16:45</t>
         </is>
       </c>
       <c r="D6" s="10" t="n"/>
       <c r="E6" s="9" t="n"/>
-      <c r="F6" s="10" t="inlineStr">
-        <is>
-          <t>(T) JIMENEZ TORERO, ASTRID GERALDINE</t>
-        </is>
-      </c>
-      <c r="G6" s="10" t="inlineStr">
-        <is>
-          <t>21:30-22:45</t>
-        </is>
-      </c>
+      <c r="F6" s="10" t="n"/>
+      <c r="G6" s="10" t="n"/>
       <c r="H6" s="10" t="n"/>
     </row>
     <row r="7" ht="19.5" customHeight="1">
@@ -764,32 +756,40 @@
       </c>
       <c r="B7" s="3" t="inlineStr">
         <is>
-          <t>QUIQUIA RICALDE, LILIA MARIA</t>
+          <t>ROCA IBARAN, MIRLA VALENTINA</t>
         </is>
       </c>
       <c r="C7" s="3" t="inlineStr">
         <is>
-          <t>08:00-17:00</t>
+          <t>07:45-11:30</t>
         </is>
       </c>
       <c r="D7" s="3" t="n"/>
       <c r="E7" s="14" t="n">
         <v>2</v>
       </c>
-      <c r="F7" s="3" t="n"/>
-      <c r="G7" s="3" t="n"/>
+      <c r="F7" s="3" t="inlineStr">
+        <is>
+          <t>FABIAN VALDIVIA, LINDSAY ZIYI</t>
+        </is>
+      </c>
+      <c r="G7" s="3" t="inlineStr">
+        <is>
+          <t>16:15-20:00</t>
+        </is>
+      </c>
       <c r="H7" s="3" t="n"/>
     </row>
     <row r="8" ht="19.5" customHeight="1">
       <c r="A8" s="14" t="n"/>
       <c r="B8" s="3" t="inlineStr">
         <is>
-          <t>HUANCAS SHUAN, JOSELYN JAZMIN</t>
+          <t>YANQUI BRAVO, MIRIAN LUZ</t>
         </is>
       </c>
       <c r="C8" s="3" t="inlineStr">
         <is>
-          <t>17:00-20:45</t>
+          <t>12:30-16:15</t>
         </is>
       </c>
       <c r="D8" s="3" t="n"/>
@@ -804,28 +804,20 @@
       </c>
       <c r="B9" s="3" t="inlineStr">
         <is>
-          <t>JIMENEZ VERGARA, ADRIAN MARCELO</t>
+          <t>QUIQUIA RICALDE, LILIA MARIA</t>
         </is>
       </c>
       <c r="C9" s="3" t="inlineStr">
         <is>
-          <t>08:45-10:00</t>
+          <t>08:00-17:00</t>
         </is>
       </c>
       <c r="D9" s="3" t="n"/>
       <c r="E9" s="14" t="n">
         <v>3</v>
       </c>
-      <c r="F9" s="3" t="inlineStr">
-        <is>
-          <t>HUAMANI LOPEZ, DREYDI BELINDA</t>
-        </is>
-      </c>
-      <c r="G9" s="3" t="inlineStr">
-        <is>
-          <t>14:00-17:45</t>
-        </is>
-      </c>
+      <c r="F9" s="3" t="n"/>
+      <c r="G9" s="3" t="n"/>
       <c r="H9" s="3" t="n"/>
     </row>
     <row r="10" ht="19.5" customHeight="1">
@@ -837,21 +829,13 @@
       </c>
       <c r="C10" s="3" t="inlineStr">
         <is>
-          <t>10:15-14:00</t>
+          <t>17:00-20:45</t>
         </is>
       </c>
       <c r="D10" s="3" t="n"/>
       <c r="E10" s="14" t="n"/>
-      <c r="F10" s="3" t="inlineStr">
-        <is>
-          <t>NEIRA CARMEN, MIRIAM DALESKA</t>
-        </is>
-      </c>
-      <c r="G10" s="3" t="inlineStr">
-        <is>
-          <t>17:45-21:30</t>
-        </is>
-      </c>
+      <c r="F10" s="3" t="n"/>
+      <c r="G10" s="3" t="n"/>
       <c r="H10" s="3" t="n"/>
     </row>
     <row r="11" ht="19.5" customHeight="1">
@@ -860,12 +844,12 @@
       </c>
       <c r="B11" s="3" t="inlineStr">
         <is>
-          <t>ROCA IBARAN, MIRLA VALENTINA</t>
+          <t>JIMENEZ VERGARA, ADRIAN MARCELO</t>
         </is>
       </c>
       <c r="C11" s="3" t="inlineStr">
         <is>
-          <t>10:15-14:00</t>
+          <t>08:45-12:30</t>
         </is>
       </c>
       <c r="D11" s="3" t="n"/>
@@ -874,12 +858,12 @@
       </c>
       <c r="F11" s="3" t="inlineStr">
         <is>
-          <t>ROA ZARATE, ELIZABETH LUCY</t>
+          <t>JIMENEZ TORERO, ASTRID GERALDINE</t>
         </is>
       </c>
       <c r="G11" s="3" t="inlineStr">
         <is>
-          <t>19:00-22:45</t>
+          <t>13:45-20:00</t>
         </is>
       </c>
       <c r="H11" s="3" t="n"/>
@@ -888,12 +872,12 @@
       <c r="A12" s="14" t="n"/>
       <c r="B12" s="3" t="inlineStr">
         <is>
-          <t>MUÑOZ SOTOMAYOR, MIRIAN RAQUEL</t>
+          <t>ALVITE CORNEJO, ANGIE LUCERO</t>
         </is>
       </c>
       <c r="C12" s="3" t="inlineStr">
         <is>
-          <t>15:15-19:00</t>
+          <t>13:00-13:30</t>
         </is>
       </c>
       <c r="D12" s="3" t="n"/>
@@ -908,32 +892,40 @@
       </c>
       <c r="B13" s="3" t="inlineStr">
         <is>
-          <t>QUIQUIA MALLQUI, CYNTHIA ANGELLINE</t>
+          <t>RAMOS FARFAN, BRYAN ENRIQUE</t>
         </is>
       </c>
       <c r="C13" s="3" t="inlineStr">
         <is>
-          <t>10:30-14:15</t>
+          <t>10:00-13:45</t>
         </is>
       </c>
       <c r="D13" s="3" t="n"/>
       <c r="E13" s="14" t="n">
         <v>5</v>
       </c>
-      <c r="F13" s="3" t="n"/>
-      <c r="G13" s="3" t="n"/>
+      <c r="F13" s="3" t="inlineStr">
+        <is>
+          <t>LEON TICONA, MARIA FERNANDA</t>
+        </is>
+      </c>
+      <c r="G13" s="3" t="inlineStr">
+        <is>
+          <t>18:00-21:45</t>
+        </is>
+      </c>
       <c r="H13" s="3" t="n"/>
     </row>
     <row r="14" ht="19.5" customHeight="1">
       <c r="A14" s="14" t="n"/>
       <c r="B14" s="3" t="inlineStr">
         <is>
-          <t>RAMOS FARFAN, BRYAN ENRIQUE</t>
+          <t>ZAPATA VILLANUEVA, FIORELLA YASMIN</t>
         </is>
       </c>
       <c r="C14" s="3" t="inlineStr">
         <is>
-          <t>16:15-20:00</t>
+          <t>14:15-18:00</t>
         </is>
       </c>
       <c r="D14" s="3" t="n"/>
@@ -948,32 +940,40 @@
       </c>
       <c r="B15" s="3" t="inlineStr">
         <is>
-          <t>ALVITE CORNEJO, ANGIE LUCERO</t>
+          <t>IDME GOMEZ, MILAGROS</t>
         </is>
       </c>
       <c r="C15" s="3" t="inlineStr">
         <is>
-          <t>11:00-14:45</t>
+          <t>10:15-14:00</t>
         </is>
       </c>
       <c r="D15" s="3" t="n"/>
       <c r="E15" s="14" t="n">
         <v>6</v>
       </c>
-      <c r="F15" s="3" t="n"/>
-      <c r="G15" s="3" t="n"/>
+      <c r="F15" s="3" t="inlineStr">
+        <is>
+          <t>LA ROSA EUSEBIO, SHADIA SHAMIRA</t>
+        </is>
+      </c>
+      <c r="G15" s="3" t="inlineStr">
+        <is>
+          <t>18:15-22:00</t>
+        </is>
+      </c>
       <c r="H15" s="3" t="n"/>
     </row>
     <row r="16" ht="19.5" customHeight="1">
       <c r="A16" s="14" t="n"/>
       <c r="B16" s="3" t="inlineStr">
         <is>
-          <t>GARRIDO SOTO, VICTORIA CELESTE</t>
+          <t>MUÑOZ SOTOMAYOR, MIRIAN RAQUEL</t>
         </is>
       </c>
       <c r="C16" s="3" t="inlineStr">
         <is>
-          <t>16:45-20:30</t>
+          <t>14:30-18:15</t>
         </is>
       </c>
       <c r="D16" s="3" t="n"/>
@@ -988,12 +988,12 @@
       </c>
       <c r="B17" s="3" t="inlineStr">
         <is>
-          <t>BRANCACHO RAMIREZ, BRINDY</t>
+          <t>CASAPAICO RIVERA, ENZO MANUEL</t>
         </is>
       </c>
       <c r="C17" s="3" t="inlineStr">
         <is>
-          <t>11:00-12:15</t>
+          <t>10:15-14:00</t>
         </is>
       </c>
       <c r="D17" s="3" t="n"/>
@@ -1002,12 +1002,12 @@
       </c>
       <c r="F17" s="3" t="inlineStr">
         <is>
-          <t>BARRIENTOS JERI, MILAGROS NICOL</t>
+          <t>POVEA CANTARO, FARID YASSER</t>
         </is>
       </c>
       <c r="G17" s="3" t="inlineStr">
         <is>
-          <t>17:00-22:00</t>
+          <t>18:15-22:00</t>
         </is>
       </c>
       <c r="H17" s="3" t="n"/>
@@ -1016,12 +1016,12 @@
       <c r="A18" s="14" t="n"/>
       <c r="B18" s="3" t="inlineStr">
         <is>
-          <t>LOPEZ SANCHEZ, NELLY ANDREA</t>
+          <t>HUAMANI LOPEZ, DREYDI BELINDA</t>
         </is>
       </c>
       <c r="C18" s="3" t="inlineStr">
         <is>
-          <t>13:00-16:45</t>
+          <t>14:30-18:15</t>
         </is>
       </c>
       <c r="D18" s="3" t="n"/>
@@ -1036,12 +1036,12 @@
       </c>
       <c r="B19" s="3" t="inlineStr">
         <is>
-          <t>JIMENEZ TORERO, ASTRID GERALDINE</t>
+          <t>LOPEZ SANCHEZ, NELLY ANDREA</t>
         </is>
       </c>
       <c r="C19" s="3" t="inlineStr">
         <is>
-          <t>13:45-21:30</t>
+          <t>10:30-14:15</t>
         </is>
       </c>
       <c r="D19" s="3" t="n"/>
@@ -1054,8 +1054,16 @@
     </row>
     <row r="20" ht="19.5" customHeight="1">
       <c r="A20" s="14" t="n"/>
-      <c r="B20" s="3" t="n"/>
-      <c r="C20" s="3" t="n"/>
+      <c r="B20" s="3" t="inlineStr">
+        <is>
+          <t>BARRIENTOS JERI, MILAGROS NICOL</t>
+        </is>
+      </c>
+      <c r="C20" s="3" t="inlineStr">
+        <is>
+          <t>17:00-22:00</t>
+        </is>
+      </c>
       <c r="D20" s="3" t="n"/>
       <c r="E20" s="14" t="n"/>
       <c r="F20" s="3" t="n"/>
@@ -1068,12 +1076,12 @@
       </c>
       <c r="B21" s="3" t="inlineStr">
         <is>
-          <t>MAYTA QUINTANA, ANDY KEVIN</t>
+          <t>BRANCACHO RAMIREZ, BRINDY</t>
         </is>
       </c>
       <c r="C21" s="3" t="inlineStr">
         <is>
-          <t>17:45-21:30</t>
+          <t>11:00-14:45</t>
         </is>
       </c>
       <c r="D21" s="3" t="n"/>
@@ -1086,8 +1094,16 @@
     </row>
     <row r="22" ht="19.5" customHeight="1">
       <c r="A22" s="14" t="n"/>
-      <c r="B22" s="3" t="n"/>
-      <c r="C22" s="3" t="n"/>
+      <c r="B22" s="3" t="inlineStr">
+        <is>
+          <t>GARRIDO SOTO, VICTORIA CELESTE</t>
+        </is>
+      </c>
+      <c r="C22" s="3" t="inlineStr">
+        <is>
+          <t>17:15-21:00</t>
+        </is>
+      </c>
       <c r="D22" s="3" t="n"/>
       <c r="E22" s="14" t="n"/>
       <c r="F22" s="3" t="n"/>
@@ -1100,12 +1116,12 @@
       </c>
       <c r="B23" s="3" t="inlineStr">
         <is>
-          <t>YANQUI BRAVO, MIRIAN LUZ</t>
+          <t>QUIQUIA MALLQUI, CYNTHIA ANGELLINE</t>
         </is>
       </c>
       <c r="C23" s="3" t="inlineStr">
         <is>
-          <t>18:00-21:45</t>
+          <t>11:15-15:00</t>
         </is>
       </c>
       <c r="D23" s="3" t="n"/>
@@ -1118,8 +1134,16 @@
     </row>
     <row r="24" ht="18.75" customHeight="1">
       <c r="A24" s="14" t="n"/>
-      <c r="B24" s="3" t="n"/>
-      <c r="C24" s="3" t="n"/>
+      <c r="B24" s="3" t="inlineStr">
+        <is>
+          <t>PEREZ GORMAS, ANTHONY</t>
+        </is>
+      </c>
+      <c r="C24" s="3" t="inlineStr">
+        <is>
+          <t>17:15-21:00</t>
+        </is>
+      </c>
       <c r="D24" s="3" t="n"/>
       <c r="E24" s="14" t="n"/>
       <c r="F24" s="3" t="n"/>
@@ -1132,12 +1156,12 @@
       </c>
       <c r="B25" s="3" t="inlineStr">
         <is>
-          <t>POVEA CANTARO, FARID YASSER</t>
+          <t>HUANCAS SHUAN, JOSELYN JAZMIN</t>
         </is>
       </c>
       <c r="C25" s="3" t="inlineStr">
         <is>
-          <t>18:15-22:00</t>
+          <t>18:00-21:45</t>
         </is>
       </c>
       <c r="D25" s="3" t="n"/>
@@ -1162,8 +1186,16 @@
       <c r="A27" s="14" t="n">
         <v>12</v>
       </c>
-      <c r="B27" s="3" t="n"/>
-      <c r="C27" s="3" t="n"/>
+      <c r="B27" s="3" t="inlineStr">
+        <is>
+          <t>MAYTA QUINTANA, ANDY KEVIN</t>
+        </is>
+      </c>
+      <c r="C27" s="3" t="inlineStr">
+        <is>
+          <t>18:15-22:00</t>
+        </is>
+      </c>
       <c r="D27" s="3" t="n"/>
       <c r="E27" s="14" t="n">
         <v>12</v>
@@ -1186,8 +1218,16 @@
       <c r="A29" s="14" t="n">
         <v>13</v>
       </c>
-      <c r="B29" s="3" t="n"/>
-      <c r="C29" s="3" t="n"/>
+      <c r="B29" s="3" t="inlineStr">
+        <is>
+          <t>ROA ZARATE, ELIZABETH LUCY</t>
+        </is>
+      </c>
+      <c r="C29" s="3" t="inlineStr">
+        <is>
+          <t>18:30-22:15</t>
+        </is>
+      </c>
       <c r="D29" s="3" t="n"/>
       <c r="E29" s="14" t="n">
         <v>13</v>
@@ -1210,8 +1250,16 @@
       <c r="A31" s="14" t="n">
         <v>14</v>
       </c>
-      <c r="B31" s="3" t="n"/>
-      <c r="C31" s="3" t="n"/>
+      <c r="B31" s="3" t="inlineStr">
+        <is>
+          <t>VILCAPOMA CHILIN, JULISSA JAZMIN</t>
+        </is>
+      </c>
+      <c r="C31" s="3" t="inlineStr">
+        <is>
+          <t>18:30-22:15</t>
+        </is>
+      </c>
       <c r="D31" s="3" t="n"/>
       <c r="E31" s="14" t="n">
         <v>14</v>
@@ -1375,7 +1423,7 @@
       </c>
       <c r="C44" s="3" t="inlineStr">
         <is>
-          <t>10:00-19:00</t>
+          <t>09:15-18:15</t>
         </is>
       </c>
       <c r="D44" s="3" t="n"/>
@@ -1390,7 +1438,7 @@
       <c r="A45" s="14" t="n"/>
       <c r="B45" s="3" t="inlineStr">
         <is>
-          <t>IDELFONSO MOTTA, JHOSSEP ANGELO</t>
+          <t>NEIRA CARMEN, MIRIAM DALESKA</t>
         </is>
       </c>
       <c r="C45" s="3" t="inlineStr">
@@ -1424,12 +1472,12 @@
       </c>
       <c r="F46" s="3" t="inlineStr">
         <is>
-          <t>PARIONA CARRASCO, YAZMIN</t>
+          <t>SICHA JORGE, JOSE ANGELO</t>
         </is>
       </c>
       <c r="G46" s="3" t="inlineStr">
         <is>
-          <t>14:45-18:30</t>
+          <t>15:00-18:45</t>
         </is>
       </c>
       <c r="H46" s="3" t="n"/>
@@ -1438,24 +1486,24 @@
       <c r="A47" s="14" t="n"/>
       <c r="B47" s="3" t="inlineStr">
         <is>
-          <t>IDME GOMEZ, MILAGROS</t>
+          <t>CUSI QUISPE, ANDREA ESTEFANY</t>
         </is>
       </c>
       <c r="C47" s="3" t="inlineStr">
         <is>
-          <t>10:45-14:30</t>
+          <t>11:00-14:45</t>
         </is>
       </c>
       <c r="D47" s="3" t="n"/>
       <c r="E47" s="14" t="n"/>
       <c r="F47" s="3" t="inlineStr">
         <is>
-          <t>VILCAPOMA CHILIN, JULISSA JAZMIN</t>
+          <t>IDELFONSO MOTTA, JHOSSEP ANGELO</t>
         </is>
       </c>
       <c r="G47" s="3" t="inlineStr">
         <is>
-          <t>18:30-21:15</t>
+          <t>19:00-22:45</t>
         </is>
       </c>
       <c r="H47" s="3" t="n"/>
@@ -1546,7 +1594,7 @@
       </c>
       <c r="F53" s="8" t="inlineStr">
         <is>
-          <t>CHAHUA BENITO, JEFFERSON ALVARO</t>
+          <t>MACHCO HUARCA, NICOLAS AXEL</t>
         </is>
       </c>
       <c r="G53" s="8" t="inlineStr">
@@ -1580,7 +1628,7 @@
       </c>
       <c r="F54" s="12" t="inlineStr">
         <is>
-          <t>CONDORI FLORES, ROSARIO</t>
+          <t>CHAHUA BENITO, JEFFERSON ALVARO</t>
         </is>
       </c>
       <c r="G54" s="12" t="inlineStr">
@@ -1730,7 +1778,7 @@
       </c>
       <c r="B4" s="8" t="inlineStr">
         <is>
-          <t>JIMENEZ TORERO, ASTRID GERALDINE</t>
+          <t>QUIQUIA RICALDE, LILIA MARIA</t>
         </is>
       </c>
       <c r="C4" s="8" t="inlineStr">
@@ -1751,7 +1799,7 @@
       </c>
       <c r="G4" s="8" t="inlineStr">
         <is>
-          <t>21:00-22:45</t>
+          <t>22:00-22:45</t>
         </is>
       </c>
       <c r="H4" s="8" t="n"/>
@@ -1760,7 +1808,7 @@
       <c r="A5" s="11" t="n"/>
       <c r="B5" s="12" t="inlineStr">
         <is>
-          <t>(T) FABIAN VALDIVIA, LINDSAY ZIYI</t>
+          <t>(T) LEON TICONA, MARIA FERNANDA</t>
         </is>
       </c>
       <c r="C5" s="12" t="inlineStr">
@@ -1783,7 +1831,7 @@
       </c>
       <c r="C6" s="10" t="inlineStr">
         <is>
-          <t>18:45-21:15</t>
+          <t>18:45-22:15</t>
         </is>
       </c>
       <c r="D6" s="10" t="n"/>
@@ -1798,38 +1846,54 @@
       </c>
       <c r="B7" s="3" t="inlineStr">
         <is>
-          <t>QUIQUIA RICALDE, LILIA MARIA</t>
+          <t>QUISPE MONDRAGON, JUAN ALFONSO</t>
         </is>
       </c>
       <c r="C7" s="3" t="inlineStr">
         <is>
-          <t>08:00-17:00</t>
+          <t>07:45-11:30</t>
         </is>
       </c>
       <c r="D7" s="3" t="n"/>
       <c r="E7" s="14" t="n">
         <v>2</v>
       </c>
-      <c r="F7" s="3" t="n"/>
-      <c r="G7" s="3" t="n"/>
+      <c r="F7" s="3" t="inlineStr">
+        <is>
+          <t>SUICA GOÑAZ, KEISY YVONNE</t>
+        </is>
+      </c>
+      <c r="G7" s="3" t="inlineStr">
+        <is>
+          <t>15:15-19:00</t>
+        </is>
+      </c>
       <c r="H7" s="3" t="n"/>
     </row>
     <row r="8" ht="19.5" customHeight="1">
       <c r="A8" s="14" t="n"/>
       <c r="B8" s="3" t="inlineStr">
         <is>
-          <t>LA ROSA EUSEBIO, SHADIA SHAMIRA</t>
+          <t>MUÑOZ SOTOMAYOR, MIRIAN RAQUEL</t>
         </is>
       </c>
       <c r="C8" s="3" t="inlineStr">
         <is>
-          <t>17:00-20:45</t>
+          <t>11:30-15:15</t>
         </is>
       </c>
       <c r="D8" s="3" t="n"/>
       <c r="E8" s="14" t="n"/>
-      <c r="F8" s="3" t="n"/>
-      <c r="G8" s="3" t="n"/>
+      <c r="F8" s="3" t="inlineStr">
+        <is>
+          <t>IDELFONSO MOTTA, JHOSSEP ANGELO</t>
+        </is>
+      </c>
+      <c r="G8" s="3" t="inlineStr">
+        <is>
+          <t>19:00-22:00</t>
+        </is>
+      </c>
       <c r="H8" s="3" t="n"/>
     </row>
     <row r="9" ht="19.5" customHeight="1">
@@ -1838,40 +1902,32 @@
       </c>
       <c r="B9" s="3" t="inlineStr">
         <is>
-          <t>MUÑOZ SOTOMAYOR, MIRIAN RAQUEL</t>
+          <t>JIMENEZ TORERO, ASTRID GERALDINE</t>
         </is>
       </c>
       <c r="C9" s="3" t="inlineStr">
         <is>
-          <t>09:00-12:45</t>
+          <t>08:00-17:00</t>
         </is>
       </c>
       <c r="D9" s="3" t="n"/>
       <c r="E9" s="14" t="n">
         <v>3</v>
       </c>
-      <c r="F9" s="3" t="inlineStr">
-        <is>
-          <t>GARRIDO SOTO, VICTORIA CELESTE</t>
-        </is>
-      </c>
-      <c r="G9" s="3" t="inlineStr">
-        <is>
-          <t>18:00-21:45</t>
-        </is>
-      </c>
+      <c r="F9" s="3" t="n"/>
+      <c r="G9" s="3" t="n"/>
       <c r="H9" s="3" t="n"/>
     </row>
     <row r="10" ht="19.5" customHeight="1">
       <c r="A10" s="14" t="n"/>
       <c r="B10" s="3" t="inlineStr">
         <is>
-          <t>ZAPATA VILLANUEVA, FIORELLA YASMIN</t>
+          <t>HUAMANI HUAMAN, MARICRUZ DESIDE</t>
         </is>
       </c>
       <c r="C10" s="3" t="inlineStr">
         <is>
-          <t>14:15-18:00</t>
+          <t>17:15-21:00</t>
         </is>
       </c>
       <c r="D10" s="3" t="n"/>
@@ -1886,12 +1942,12 @@
       </c>
       <c r="B11" s="3" t="inlineStr">
         <is>
-          <t>TARDILLO COPA, YOVANNA MELISSA</t>
+          <t>ROCA IBARAN, MIRLA VALENTINA</t>
         </is>
       </c>
       <c r="C11" s="3" t="inlineStr">
         <is>
-          <t>09:15-13:00</t>
+          <t>08:45-12:30</t>
         </is>
       </c>
       <c r="D11" s="3" t="n"/>
@@ -1900,12 +1956,12 @@
       </c>
       <c r="F11" s="3" t="inlineStr">
         <is>
-          <t>BONILLA SANCHEZ, RAUL FERNANDO</t>
+          <t>ALARCON SANDOVAL, ADRIANA FERNANDA</t>
         </is>
       </c>
       <c r="G11" s="3" t="inlineStr">
         <is>
-          <t>19:00-22:45</t>
+          <t>18:00-21:45</t>
         </is>
       </c>
       <c r="H11" s="3" t="n"/>
@@ -1914,12 +1970,12 @@
       <c r="A12" s="14" t="n"/>
       <c r="B12" s="3" t="inlineStr">
         <is>
-          <t>HUANCAS SHUAN, JOSELYN JAZMIN</t>
+          <t>YANQUI BRAVO, MIRIAN LUZ</t>
         </is>
       </c>
       <c r="C12" s="3" t="inlineStr">
         <is>
-          <t>15:00-18:45</t>
+          <t>13:15-17:00</t>
         </is>
       </c>
       <c r="D12" s="3" t="n"/>
@@ -1934,12 +1990,12 @@
       </c>
       <c r="B13" s="3" t="inlineStr">
         <is>
-          <t>QUIQUIA MALLQUI, CYNTHIA ANGELLINE</t>
+          <t>CASAPAICO RIVERA, ENZO MANUEL</t>
         </is>
       </c>
       <c r="C13" s="3" t="inlineStr">
         <is>
-          <t>10:30-14:15</t>
+          <t>09:00-12:45</t>
         </is>
       </c>
       <c r="D13" s="3" t="n"/>
@@ -1948,12 +2004,12 @@
       </c>
       <c r="F13" s="3" t="inlineStr">
         <is>
-          <t>SUICA GOÑAZ, KEISY YVONNE</t>
+          <t>NEIRA CARMEN, MIRIAM DALESKA</t>
         </is>
       </c>
       <c r="G13" s="3" t="inlineStr">
         <is>
-          <t>16:00-19:45</t>
+          <t>18:00-21:45</t>
         </is>
       </c>
       <c r="H13" s="3" t="n"/>
@@ -1962,12 +2018,12 @@
       <c r="A14" s="14" t="n"/>
       <c r="B14" s="3" t="inlineStr">
         <is>
-          <t>FABIAN VALDIVIA, LINDSAY ZIYI</t>
+          <t>ZAPATA VILLANUEVA, FIORELLA YASMIN</t>
         </is>
       </c>
       <c r="C14" s="3" t="inlineStr">
         <is>
-          <t>15:15-15:45</t>
+          <t>14:15-18:00</t>
         </is>
       </c>
       <c r="D14" s="3" t="n"/>
@@ -1982,32 +2038,40 @@
       </c>
       <c r="B15" s="3" t="inlineStr">
         <is>
-          <t>YANQUI BRAVO, MIRIAN LUZ</t>
+          <t>ALVITE CORNEJO, ANGIE LUCERO</t>
         </is>
       </c>
       <c r="C15" s="3" t="inlineStr">
         <is>
-          <t>11:00-14:45</t>
+          <t>10:30-14:15</t>
         </is>
       </c>
       <c r="D15" s="3" t="n"/>
       <c r="E15" s="14" t="n">
         <v>6</v>
       </c>
-      <c r="F15" s="3" t="n"/>
-      <c r="G15" s="3" t="n"/>
+      <c r="F15" s="3" t="inlineStr">
+        <is>
+          <t>POVEA CANTARO, FARID YASSER</t>
+        </is>
+      </c>
+      <c r="G15" s="3" t="inlineStr">
+        <is>
+          <t>19:00-22:45</t>
+        </is>
+      </c>
       <c r="H15" s="3" t="n"/>
     </row>
     <row r="16" ht="19.5" customHeight="1">
       <c r="A16" s="14" t="n"/>
       <c r="B16" s="3" t="inlineStr">
         <is>
-          <t>PEREZ GORMAS, ANTHONY</t>
+          <t>FABIAN VALDIVIA, LINDSAY ZIYI</t>
         </is>
       </c>
       <c r="C16" s="3" t="inlineStr">
         <is>
-          <t>16:30-20:15</t>
+          <t>15:15-19:00</t>
         </is>
       </c>
       <c r="D16" s="3" t="n"/>
@@ -2022,32 +2086,40 @@
       </c>
       <c r="B17" s="3" t="inlineStr">
         <is>
-          <t>BRANCACHO RAMIREZ, BRINDY</t>
+          <t>IDME GOMEZ, MILAGROS</t>
         </is>
       </c>
       <c r="C17" s="3" t="inlineStr">
         <is>
-          <t>11:00-14:45</t>
+          <t>10:30-14:15</t>
         </is>
       </c>
       <c r="D17" s="3" t="n"/>
       <c r="E17" s="14" t="n">
         <v>7</v>
       </c>
-      <c r="F17" s="3" t="n"/>
-      <c r="G17" s="3" t="n"/>
+      <c r="F17" s="3" t="inlineStr">
+        <is>
+          <t>BONILLA SANCHEZ, RAUL FERNANDO</t>
+        </is>
+      </c>
+      <c r="G17" s="3" t="inlineStr">
+        <is>
+          <t>16:30-20:15</t>
+        </is>
+      </c>
       <c r="H17" s="3" t="n"/>
     </row>
     <row r="18" ht="19.5" customHeight="1">
       <c r="A18" s="14" t="n"/>
       <c r="B18" s="3" t="inlineStr">
         <is>
-          <t>RAMOS FARFAN, BRYAN ENRIQUE</t>
+          <t>LEON TICONA, MARIA FERNANDA</t>
         </is>
       </c>
       <c r="C18" s="3" t="inlineStr">
         <is>
-          <t>17:15-21:00</t>
+          <t>15:15-15:45</t>
         </is>
       </c>
       <c r="D18" s="3" t="n"/>
@@ -2062,12 +2134,12 @@
       </c>
       <c r="B19" s="3" t="inlineStr">
         <is>
-          <t>CASAPAICO RIVERA, ENZO MANUEL</t>
+          <t>SOTO VELAZCO, EMIR ALESSANDRO</t>
         </is>
       </c>
       <c r="C19" s="3" t="inlineStr">
         <is>
-          <t>11:15-15:00</t>
+          <t>11:00-14:45</t>
         </is>
       </c>
       <c r="D19" s="3" t="n"/>
@@ -2082,12 +2154,12 @@
       <c r="A20" s="14" t="n"/>
       <c r="B20" s="3" t="inlineStr">
         <is>
-          <t>SICHA JORGE, JOSE ANGELO</t>
+          <t>LA ROSA EUSEBIO, SHADIA SHAMIRA</t>
         </is>
       </c>
       <c r="C20" s="3" t="inlineStr">
         <is>
-          <t>17:15-21:00</t>
+          <t>16:45-20:30</t>
         </is>
       </c>
       <c r="D20" s="3" t="n"/>
@@ -2102,12 +2174,12 @@
       </c>
       <c r="B21" s="3" t="inlineStr">
         <is>
-          <t>IDME GOMEZ, MILAGROS</t>
+          <t>CUSI QUISPE, ANDREA ESTEFANY</t>
         </is>
       </c>
       <c r="C21" s="3" t="inlineStr">
         <is>
-          <t>11:15-15:00</t>
+          <t>11:00-14:45</t>
         </is>
       </c>
       <c r="D21" s="3" t="n"/>
@@ -2122,7 +2194,7 @@
       <c r="A22" s="14" t="n"/>
       <c r="B22" s="3" t="inlineStr">
         <is>
-          <t>ALARCON SANDOVAL, ADRIANA FERNANDA</t>
+          <t>MAYTA QUINTANA, ANDY KEVIN</t>
         </is>
       </c>
       <c r="C22" s="3" t="inlineStr">
@@ -2142,12 +2214,12 @@
       </c>
       <c r="B23" s="3" t="inlineStr">
         <is>
-          <t>HUAMANI LOPEZ, DREYDI BELINDA</t>
+          <t>BRANCACHO RAMIREZ, BRINDY</t>
         </is>
       </c>
       <c r="C23" s="3" t="inlineStr">
         <is>
-          <t>12:00-15:45</t>
+          <t>11:00-14:45</t>
         </is>
       </c>
       <c r="D23" s="3" t="n"/>
@@ -2162,12 +2234,12 @@
       <c r="A24" s="14" t="n"/>
       <c r="B24" s="3" t="inlineStr">
         <is>
-          <t>LEON TICONA, MARIA FERNANDA</t>
+          <t>PEREZ GORMAS, ANTHONY</t>
         </is>
       </c>
       <c r="C24" s="3" t="inlineStr">
         <is>
-          <t>18:15-22:00</t>
+          <t>18:00-21:45</t>
         </is>
       </c>
       <c r="D24" s="3" t="n"/>
@@ -2182,12 +2254,12 @@
       </c>
       <c r="B25" s="3" t="inlineStr">
         <is>
-          <t>VILCAPOMA CHILIN, JULISSA JAZMIN</t>
+          <t>HUANCAS SHUAN, JOSELYN JAZMIN</t>
         </is>
       </c>
       <c r="C25" s="3" t="inlineStr">
         <is>
-          <t>18:30-18:45</t>
+          <t>18:00-21:45</t>
         </is>
       </c>
       <c r="D25" s="3" t="n"/>
@@ -2212,8 +2284,16 @@
       <c r="A27" s="14" t="n">
         <v>12</v>
       </c>
-      <c r="B27" s="3" t="n"/>
-      <c r="C27" s="3" t="n"/>
+      <c r="B27" s="3" t="inlineStr">
+        <is>
+          <t>VILCAPOMA CHILIN, JULISSA JAZMIN</t>
+        </is>
+      </c>
+      <c r="C27" s="3" t="inlineStr">
+        <is>
+          <t>18:30-18:45</t>
+        </is>
+      </c>
       <c r="D27" s="3" t="n"/>
       <c r="E27" s="14" t="n">
         <v>12</v>
@@ -2425,7 +2505,7 @@
       </c>
       <c r="C44" s="3" t="inlineStr">
         <is>
-          <t>09:30-18:30</t>
+          <t>10:00-19:00</t>
         </is>
       </c>
       <c r="D44" s="3" t="n"/>
@@ -2460,7 +2540,7 @@
       </c>
       <c r="B46" s="3" t="inlineStr">
         <is>
-          <t>QUISPE MONDRAGON, JUAN ALFONSO</t>
+          <t>JIMENEZ VERGARA, ADRIAN MARCELO</t>
         </is>
       </c>
       <c r="C46" s="3" t="inlineStr">
@@ -2474,12 +2554,12 @@
       </c>
       <c r="F46" s="3" t="inlineStr">
         <is>
-          <t>NEIRA CARMEN, MIRIAM DALESKA</t>
+          <t>HUAMANI LOPEZ, DREYDI BELINDA</t>
         </is>
       </c>
       <c r="G46" s="3" t="inlineStr">
         <is>
-          <t>15:00-18:45</t>
+          <t>14:30-18:15</t>
         </is>
       </c>
       <c r="H46" s="3" t="n"/>
@@ -2488,7 +2568,7 @@
       <c r="A47" s="14" t="n"/>
       <c r="B47" s="3" t="inlineStr">
         <is>
-          <t>JIMENEZ VERGARA, ADRIAN MARCELO</t>
+          <t>QUIQUIA MALLQUI, CYNTHIA ANGELLINE</t>
         </is>
       </c>
       <c r="C47" s="3" t="inlineStr">
@@ -2500,12 +2580,12 @@
       <c r="E47" s="14" t="n"/>
       <c r="F47" s="3" t="inlineStr">
         <is>
-          <t>IDELFONSO MOTTA, JHOSSEP ANGELO</t>
+          <t>GARRIDO SOTO, VICTORIA CELESTE</t>
         </is>
       </c>
       <c r="G47" s="3" t="inlineStr">
         <is>
-          <t>19:00-21:00</t>
+          <t>18:15-22:00</t>
         </is>
       </c>
       <c r="H47" s="3" t="n"/>
@@ -2796,12 +2876,12 @@
       </c>
       <c r="F4" s="8" t="inlineStr">
         <is>
-          <t>(T) ALARCON SANDOVAL, ADRIANA FERNANDA</t>
+          <t>(T) NEIRA CARMEN, MIRIAM DALESKA</t>
         </is>
       </c>
       <c r="G4" s="8" t="inlineStr">
         <is>
-          <t>15:30-19:00</t>
+          <t>16:15-19:45</t>
         </is>
       </c>
       <c r="H4" s="8" t="n"/>
@@ -2810,7 +2890,7 @@
       <c r="A5" s="11" t="n"/>
       <c r="B5" s="12" t="inlineStr">
         <is>
-          <t>ROCA IBARAN, MIRLA VALENTINA</t>
+          <t>TARDILLO COPA, YOVANNA MELISSA</t>
         </is>
       </c>
       <c r="C5" s="12" t="inlineStr">
@@ -2822,12 +2902,12 @@
       <c r="E5" s="11" t="n"/>
       <c r="F5" s="12" t="inlineStr">
         <is>
-          <t>POVEA CANTARO, FARID YASSER</t>
+          <t>(T) JIMENEZ TORERO, ASTRID GERALDINE</t>
         </is>
       </c>
       <c r="G5" s="12" t="inlineStr">
         <is>
-          <t>18:45-22:30</t>
+          <t>19:30-22:45</t>
         </is>
       </c>
       <c r="H5" s="12" t="n"/>
@@ -2836,26 +2916,18 @@
       <c r="A6" s="9" t="n"/>
       <c r="B6" s="10" t="inlineStr">
         <is>
-          <t>(T) HUAMANI LOPEZ, DREYDI BELINDA</t>
+          <t>(T) ALVITE CORNEJO, ANGIE LUCERO</t>
         </is>
       </c>
       <c r="C6" s="10" t="inlineStr">
         <is>
-          <t>13:30-15:45</t>
+          <t>13:30-16:30</t>
         </is>
       </c>
       <c r="D6" s="10" t="n"/>
       <c r="E6" s="9" t="n"/>
-      <c r="F6" s="10" t="inlineStr">
-        <is>
-          <t>(T) JIMENEZ TORERO, ASTRID GERALDINE</t>
-        </is>
-      </c>
-      <c r="G6" s="10" t="inlineStr">
-        <is>
-          <t>22:15-22:45</t>
-        </is>
-      </c>
+      <c r="F6" s="10" t="n"/>
+      <c r="G6" s="10" t="n"/>
       <c r="H6" s="10" t="n"/>
     </row>
     <row r="7" ht="19.5" customHeight="1">
@@ -2864,12 +2936,12 @@
       </c>
       <c r="B7" s="3" t="inlineStr">
         <is>
-          <t>ALVITE CORNEJO, ANGIE LUCERO</t>
+          <t>QUISPE MONDRAGON, JUAN ALFONSO</t>
         </is>
       </c>
       <c r="C7" s="3" t="inlineStr">
         <is>
-          <t>08:00-11:45</t>
+          <t>07:45-11:30</t>
         </is>
       </c>
       <c r="D7" s="3" t="n"/>
@@ -2878,12 +2950,12 @@
       </c>
       <c r="F7" s="3" t="inlineStr">
         <is>
-          <t>JIMENEZ TORERO, ASTRID GERALDINE</t>
+          <t>GARRIDO SOTO, VICTORIA CELESTE</t>
         </is>
       </c>
       <c r="G7" s="3" t="inlineStr">
         <is>
-          <t>13:45-22:15</t>
+          <t>15:15-19:00</t>
         </is>
       </c>
       <c r="H7" s="3" t="n"/>
@@ -2892,18 +2964,26 @@
       <c r="A8" s="14" t="n"/>
       <c r="B8" s="3" t="inlineStr">
         <is>
-          <t>HUAMANI LOPEZ, DREYDI BELINDA</t>
+          <t>SUICA GOÑAZ, KEISY YVONNE</t>
         </is>
       </c>
       <c r="C8" s="3" t="inlineStr">
         <is>
-          <t>12:00-13:30</t>
+          <t>11:30-15:15</t>
         </is>
       </c>
       <c r="D8" s="3" t="n"/>
       <c r="E8" s="14" t="n"/>
-      <c r="F8" s="3" t="n"/>
-      <c r="G8" s="3" t="n"/>
+      <c r="F8" s="3" t="inlineStr">
+        <is>
+          <t>ROA ZARATE, ELIZABETH LUCY</t>
+        </is>
+      </c>
+      <c r="G8" s="3" t="inlineStr">
+        <is>
+          <t>19:00-22:45</t>
+        </is>
+      </c>
       <c r="H8" s="3" t="n"/>
     </row>
     <row r="9" ht="19.5" customHeight="1">
@@ -2912,7 +2992,7 @@
       </c>
       <c r="B9" s="3" t="inlineStr">
         <is>
-          <t>TARDILLO COPA, YOVANNA MELISSA</t>
+          <t>IDME GOMEZ, MILAGROS</t>
         </is>
       </c>
       <c r="C9" s="3" t="inlineStr">
@@ -2926,12 +3006,12 @@
       </c>
       <c r="F9" s="3" t="inlineStr">
         <is>
-          <t>NEIRA CARMEN, MIRIAM DALESKA</t>
+          <t>JIMENEZ TORERO, ASTRID GERALDINE</t>
         </is>
       </c>
       <c r="G9" s="3" t="inlineStr">
         <is>
-          <t>17:45-21:30</t>
+          <t>13:45-19:30</t>
         </is>
       </c>
       <c r="H9" s="3" t="n"/>
@@ -2940,12 +3020,12 @@
       <c r="A10" s="14" t="n"/>
       <c r="B10" s="3" t="inlineStr">
         <is>
-          <t>ZAPATA VILLANUEVA, FIORELLA YASMIN</t>
+          <t>ALVITE CORNEJO, ANGIE LUCERO</t>
         </is>
       </c>
       <c r="C10" s="3" t="inlineStr">
         <is>
-          <t>14:00-17:45</t>
+          <t>12:45-13:30</t>
         </is>
       </c>
       <c r="D10" s="3" t="n"/>
@@ -2960,7 +3040,7 @@
       </c>
       <c r="B11" s="3" t="inlineStr">
         <is>
-          <t>SUICA GOÑAZ, KEISY YVONNE</t>
+          <t>RAMOS FARFAN, BRYAN ENRIQUE</t>
         </is>
       </c>
       <c r="C11" s="3" t="inlineStr">
@@ -2974,12 +3054,12 @@
       </c>
       <c r="F11" s="3" t="inlineStr">
         <is>
-          <t>LEON TICONA, MARIA FERNANDA</t>
+          <t>ALARCON SANDOVAL, ADRIANA FERNANDA</t>
         </is>
       </c>
       <c r="G11" s="3" t="inlineStr">
         <is>
-          <t>18:15-22:00</t>
+          <t>18:00-21:45</t>
         </is>
       </c>
       <c r="H11" s="3" t="n"/>
@@ -2988,12 +3068,12 @@
       <c r="A12" s="14" t="n"/>
       <c r="B12" s="3" t="inlineStr">
         <is>
-          <t>MAYTA QUINTANA, ANDY KEVIN</t>
+          <t>LA ROSA EUSEBIO, SHADIA SHAMIRA</t>
         </is>
       </c>
       <c r="C12" s="3" t="inlineStr">
         <is>
-          <t>14:30-18:15</t>
+          <t>14:15-18:00</t>
         </is>
       </c>
       <c r="D12" s="3" t="n"/>
@@ -3008,42 +3088,26 @@
       </c>
       <c r="B13" s="3" t="inlineStr">
         <is>
-          <t>QUIQUIA MALLQUI, CYNTHIA ANGELLINE</t>
+          <t>QUIQUIA RICALDE, LILIA MARIA</t>
         </is>
       </c>
       <c r="C13" s="3" t="inlineStr">
         <is>
-          <t>10:30-14:15</t>
+          <t>10:30-19:30</t>
         </is>
       </c>
       <c r="D13" s="3" t="n"/>
       <c r="E13" s="14" t="n">
         <v>5</v>
       </c>
-      <c r="F13" s="3" t="inlineStr">
-        <is>
-          <t>ROA ZARATE, ELIZABETH LUCY</t>
-        </is>
-      </c>
-      <c r="G13" s="3" t="inlineStr">
-        <is>
-          <t>19:00-22:45</t>
-        </is>
-      </c>
+      <c r="F13" s="3" t="n"/>
+      <c r="G13" s="3" t="n"/>
       <c r="H13" s="3" t="n"/>
     </row>
     <row r="14" ht="19.5" customHeight="1">
       <c r="A14" s="14" t="n"/>
-      <c r="B14" s="3" t="inlineStr">
-        <is>
-          <t>FABIAN VALDIVIA, LINDSAY ZIYI</t>
-        </is>
-      </c>
-      <c r="C14" s="3" t="inlineStr">
-        <is>
-          <t>15:00-18:45</t>
-        </is>
-      </c>
+      <c r="B14" s="3" t="n"/>
+      <c r="C14" s="3" t="n"/>
       <c r="D14" s="3" t="n"/>
       <c r="E14" s="14" t="n"/>
       <c r="F14" s="3" t="n"/>
@@ -3056,12 +3120,12 @@
       </c>
       <c r="B15" s="3" t="inlineStr">
         <is>
-          <t>JIMENEZ VERGARA, ADRIAN MARCELO</t>
+          <t>CASAPAICO RIVERA, ENZO MANUEL</t>
         </is>
       </c>
       <c r="C15" s="3" t="inlineStr">
         <is>
-          <t>10:45-14:30</t>
+          <t>10:30-14:15</t>
         </is>
       </c>
       <c r="D15" s="3" t="n"/>
@@ -3070,12 +3134,12 @@
       </c>
       <c r="F15" s="3" t="inlineStr">
         <is>
-          <t>BONILLA SANCHEZ, RAUL FERNANDO</t>
+          <t>LEON TICONA, MARIA FERNANDA</t>
         </is>
       </c>
       <c r="G15" s="3" t="inlineStr">
         <is>
-          <t>16:30-20:15</t>
+          <t>18:15-22:00</t>
         </is>
       </c>
       <c r="H15" s="3" t="n"/>
@@ -3084,12 +3148,12 @@
       <c r="A16" s="14" t="n"/>
       <c r="B16" s="3" t="inlineStr">
         <is>
-          <t>ALARCON SANDOVAL, ADRIANA FERNANDA</t>
+          <t>SICHA JORGE, JOSE ANGELO</t>
         </is>
       </c>
       <c r="C16" s="3" t="inlineStr">
         <is>
-          <t>15:15-15:30</t>
+          <t>14:30-18:15</t>
         </is>
       </c>
       <c r="D16" s="3" t="n"/>
@@ -3104,7 +3168,7 @@
       </c>
       <c r="B17" s="3" t="inlineStr">
         <is>
-          <t>MUÑOZ SOTOMAYOR, MIRIAN RAQUEL</t>
+          <t>YANQUI BRAVO, MIRIAN LUZ</t>
         </is>
       </c>
       <c r="C17" s="3" t="inlineStr">
@@ -3116,20 +3180,28 @@
       <c r="E17" s="14" t="n">
         <v>7</v>
       </c>
-      <c r="F17" s="3" t="n"/>
-      <c r="G17" s="3" t="n"/>
+      <c r="F17" s="3" t="inlineStr">
+        <is>
+          <t>BONILLA SANCHEZ, RAUL FERNANDO</t>
+        </is>
+      </c>
+      <c r="G17" s="3" t="inlineStr">
+        <is>
+          <t>17:00-20:45</t>
+        </is>
+      </c>
       <c r="H17" s="3" t="n"/>
     </row>
     <row r="18" ht="19.5" customHeight="1">
       <c r="A18" s="14" t="n"/>
       <c r="B18" s="3" t="inlineStr">
         <is>
-          <t>SICHA JORGE, JOSE ANGELO</t>
+          <t>NEIRA CARMEN, MIRIAM DALESKA</t>
         </is>
       </c>
       <c r="C18" s="3" t="inlineStr">
         <is>
-          <t>17:00-20:45</t>
+          <t>16:00-16:15</t>
         </is>
       </c>
       <c r="D18" s="3" t="n"/>
@@ -3144,12 +3216,12 @@
       </c>
       <c r="B19" s="3" t="inlineStr">
         <is>
-          <t>CASAPAICO RIVERA, ENZO MANUEL</t>
+          <t>BRANCACHO RAMIREZ, BRINDY</t>
         </is>
       </c>
       <c r="C19" s="3" t="inlineStr">
         <is>
-          <t>11:15-15:00</t>
+          <t>11:00-14:45</t>
         </is>
       </c>
       <c r="D19" s="3" t="n"/>
@@ -3164,12 +3236,12 @@
       <c r="A20" s="14" t="n"/>
       <c r="B20" s="3" t="inlineStr">
         <is>
-          <t>PEREZ GORMAS, ANTHONY</t>
+          <t>HUAMANI HUAMAN, MARICRUZ DESIDE</t>
         </is>
       </c>
       <c r="C20" s="3" t="inlineStr">
         <is>
-          <t>17:30-21:15</t>
+          <t>17:15-21:00</t>
         </is>
       </c>
       <c r="D20" s="3" t="n"/>
@@ -3184,12 +3256,12 @@
       </c>
       <c r="B21" s="3" t="inlineStr">
         <is>
-          <t>RAMOS FARFAN, BRYAN ENRIQUE</t>
+          <t>FABIAN VALDIVIA, LINDSAY ZIYI</t>
         </is>
       </c>
       <c r="C21" s="3" t="inlineStr">
         <is>
-          <t>11:30-15:15</t>
+          <t>17:30-21:15</t>
         </is>
       </c>
       <c r="D21" s="3" t="n"/>
@@ -3202,16 +3274,8 @@
     </row>
     <row r="22" ht="19.5" customHeight="1">
       <c r="A22" s="14" t="n"/>
-      <c r="B22" s="3" t="inlineStr">
-        <is>
-          <t>YANQUI BRAVO, MIRIAN LUZ</t>
-        </is>
-      </c>
-      <c r="C22" s="3" t="inlineStr">
-        <is>
-          <t>18:00-21:45</t>
-        </is>
-      </c>
+      <c r="B22" s="3" t="n"/>
+      <c r="C22" s="3" t="n"/>
       <c r="D22" s="3" t="n"/>
       <c r="E22" s="14" t="n"/>
       <c r="F22" s="3" t="n"/>
@@ -3224,12 +3288,12 @@
       </c>
       <c r="B23" s="3" t="inlineStr">
         <is>
-          <t>VILCAPOMA CHILIN, JULISSA JAZMIN</t>
+          <t>PEREZ GORMAS, ANTHONY</t>
         </is>
       </c>
       <c r="C23" s="3" t="inlineStr">
         <is>
-          <t>18:30-21:15</t>
+          <t>18:15-22:00</t>
         </is>
       </c>
       <c r="D23" s="3" t="n"/>
@@ -3254,8 +3318,16 @@
       <c r="A25" s="14" t="n">
         <v>11</v>
       </c>
-      <c r="B25" s="3" t="n"/>
-      <c r="C25" s="3" t="n"/>
+      <c r="B25" s="3" t="inlineStr">
+        <is>
+          <t>VILCAPOMA CHILIN, JULISSA JAZMIN</t>
+        </is>
+      </c>
+      <c r="C25" s="3" t="inlineStr">
+        <is>
+          <t>18:30-22:15</t>
+        </is>
+      </c>
       <c r="D25" s="3" t="n"/>
       <c r="E25" s="14" t="n">
         <v>11</v>
@@ -3491,7 +3563,7 @@
       </c>
       <c r="C44" s="3" t="inlineStr">
         <is>
-          <t>09:30-18:30</t>
+          <t>09:15-18:15</t>
         </is>
       </c>
       <c r="D44" s="3" t="n"/>
@@ -3506,7 +3578,7 @@
       <c r="A45" s="14" t="n"/>
       <c r="B45" s="3" t="inlineStr">
         <is>
-          <t>HUAMANI HUAMAN, MARICRUZ DESIDE</t>
+          <t>IDELFONSO MOTTA, JHOSSEP ANGELO</t>
         </is>
       </c>
       <c r="C45" s="3" t="inlineStr">
@@ -3526,7 +3598,7 @@
       </c>
       <c r="B46" s="3" t="inlineStr">
         <is>
-          <t>QUISPE MONDRAGON, JUAN ALFONSO</t>
+          <t>JIMENEZ VERGARA, ADRIAN MARCELO</t>
         </is>
       </c>
       <c r="C46" s="3" t="inlineStr">
@@ -3538,26 +3610,42 @@
       <c r="E46" s="14" t="n">
         <v>22</v>
       </c>
-      <c r="F46" s="3" t="n"/>
-      <c r="G46" s="3" t="n"/>
+      <c r="F46" s="3" t="inlineStr">
+        <is>
+          <t>CUSI QUISPE, ANDREA ESTEFANY</t>
+        </is>
+      </c>
+      <c r="G46" s="3" t="inlineStr">
+        <is>
+          <t>14:30-18:15</t>
+        </is>
+      </c>
       <c r="H46" s="3" t="n"/>
     </row>
     <row r="47" ht="18.75" customHeight="1">
       <c r="A47" s="14" t="n"/>
       <c r="B47" s="3" t="inlineStr">
         <is>
-          <t>QUIQUIA RICALDE, LILIA MARIA</t>
+          <t>QUIQUIA MALLQUI, CYNTHIA ANGELLINE</t>
         </is>
       </c>
       <c r="C47" s="3" t="inlineStr">
         <is>
-          <t>10:45-19:45</t>
+          <t>10:45-14:30</t>
         </is>
       </c>
       <c r="D47" s="3" t="n"/>
       <c r="E47" s="14" t="n"/>
-      <c r="F47" s="3" t="n"/>
-      <c r="G47" s="3" t="n"/>
+      <c r="F47" s="3" t="inlineStr">
+        <is>
+          <t>POVEA CANTARO, FARID YASSER</t>
+        </is>
+      </c>
+      <c r="G47" s="3" t="inlineStr">
+        <is>
+          <t>18:15-22:00</t>
+        </is>
+      </c>
       <c r="H47" s="3" t="n"/>
     </row>
     <row r="48" ht="18.75" customHeight="1">
@@ -3846,12 +3934,12 @@
       </c>
       <c r="F4" s="8" t="inlineStr">
         <is>
-          <t>LEON TICONA, MARIA FERNANDA</t>
+          <t>(T) HUAMANI LOPEZ, DREYDI BELINDA</t>
         </is>
       </c>
       <c r="G4" s="8" t="inlineStr">
         <is>
-          <t>15:30-19:15</t>
+          <t>16:30-19:45</t>
         </is>
       </c>
       <c r="H4" s="8" t="n"/>
@@ -3860,7 +3948,7 @@
       <c r="A5" s="11" t="n"/>
       <c r="B5" s="12" t="inlineStr">
         <is>
-          <t>ALVITE CORNEJO, ANGIE LUCERO</t>
+          <t>CASAPAICO RIVERA, ENZO MANUEL</t>
         </is>
       </c>
       <c r="C5" s="12" t="inlineStr">
@@ -3877,7 +3965,7 @@
       </c>
       <c r="G5" s="12" t="inlineStr">
         <is>
-          <t>19:00-22:45</t>
+          <t>19:30-22:45</t>
         </is>
       </c>
       <c r="H5" s="12" t="n"/>
@@ -3886,12 +3974,12 @@
       <c r="A6" s="9" t="n"/>
       <c r="B6" s="10" t="inlineStr">
         <is>
-          <t>(T) HUAMANI LOPEZ, DREYDI BELINDA</t>
+          <t>(T) YANQUI BRAVO, MIRIAN LUZ</t>
         </is>
       </c>
       <c r="C6" s="10" t="inlineStr">
         <is>
-          <t>13:30-15:45</t>
+          <t>13:30-16:45</t>
         </is>
       </c>
       <c r="D6" s="10" t="n"/>
@@ -3906,12 +3994,12 @@
       </c>
       <c r="B7" s="3" t="inlineStr">
         <is>
-          <t>QUISPE MONDRAGON, JUAN ALFONSO</t>
+          <t>ROCA IBARAN, MIRLA VALENTINA</t>
         </is>
       </c>
       <c r="C7" s="3" t="inlineStr">
         <is>
-          <t>08:00-11:45</t>
+          <t>07:45-11:30</t>
         </is>
       </c>
       <c r="D7" s="3" t="n"/>
@@ -3920,12 +4008,12 @@
       </c>
       <c r="F7" s="3" t="inlineStr">
         <is>
-          <t>ZAPATA VILLANUEVA, FIORELLA YASMIN</t>
+          <t>FABIAN VALDIVIA, LINDSAY ZIYI</t>
         </is>
       </c>
       <c r="G7" s="3" t="inlineStr">
         <is>
-          <t>14:00-17:45</t>
+          <t>15:15-19:00</t>
         </is>
       </c>
       <c r="H7" s="3" t="n"/>
@@ -3934,24 +4022,24 @@
       <c r="A8" s="14" t="n"/>
       <c r="B8" s="3" t="inlineStr">
         <is>
-          <t>HUAMANI LOPEZ, DREYDI BELINDA</t>
+          <t>MUÑOZ SOTOMAYOR, MIRIAN RAQUEL</t>
         </is>
       </c>
       <c r="C8" s="3" t="inlineStr">
         <is>
-          <t>12:00-13:30</t>
+          <t>11:30-15:15</t>
         </is>
       </c>
       <c r="D8" s="3" t="n"/>
       <c r="E8" s="14" t="n"/>
       <c r="F8" s="3" t="inlineStr">
         <is>
-          <t>POVEA CANTARO, FARID YASSER</t>
+          <t>IDELFONSO MOTTA, JHOSSEP ANGELO</t>
         </is>
       </c>
       <c r="G8" s="3" t="inlineStr">
         <is>
-          <t>17:45-21:30</t>
+          <t>19:00-19:30</t>
         </is>
       </c>
       <c r="H8" s="3" t="n"/>
@@ -3962,40 +4050,32 @@
       </c>
       <c r="B9" s="3" t="inlineStr">
         <is>
-          <t>ROCA IBARAN, MIRLA VALENTINA</t>
+          <t>QUIQUIA RICALDE, LILIA MARIA</t>
         </is>
       </c>
       <c r="C9" s="3" t="inlineStr">
         <is>
-          <t>08:45-12:30</t>
+          <t>08:00-17:00</t>
         </is>
       </c>
       <c r="D9" s="3" t="n"/>
       <c r="E9" s="14" t="n">
         <v>3</v>
       </c>
-      <c r="F9" s="3" t="inlineStr">
-        <is>
-          <t>YANQUI BRAVO, MIRIAN LUZ</t>
-        </is>
-      </c>
-      <c r="G9" s="3" t="inlineStr">
-        <is>
-          <t>18:15-22:00</t>
-        </is>
-      </c>
+      <c r="F9" s="3" t="n"/>
+      <c r="G9" s="3" t="n"/>
       <c r="H9" s="3" t="n"/>
     </row>
     <row r="10" ht="19.5" customHeight="1">
       <c r="A10" s="14" t="n"/>
       <c r="B10" s="3" t="inlineStr">
         <is>
-          <t>MAYTA QUINTANA, ANDY KEVIN</t>
+          <t>BONILLA SANCHEZ, RAUL FERNANDO</t>
         </is>
       </c>
       <c r="C10" s="3" t="inlineStr">
         <is>
-          <t>14:30-18:15</t>
+          <t>17:15-21:00</t>
         </is>
       </c>
       <c r="D10" s="3" t="n"/>
@@ -4010,7 +4090,7 @@
       </c>
       <c r="B11" s="3" t="inlineStr">
         <is>
-          <t>SUICA GOÑAZ, KEISY YVONNE</t>
+          <t>TARDILLO COPA, YOVANNA MELISSA</t>
         </is>
       </c>
       <c r="C11" s="3" t="inlineStr">
@@ -4024,12 +4104,12 @@
       </c>
       <c r="F11" s="3" t="inlineStr">
         <is>
-          <t>HUAMANI HUAMAN, MARICRUZ DESIDE</t>
+          <t>POVEA CANTARO, FARID YASSER</t>
         </is>
       </c>
       <c r="G11" s="3" t="inlineStr">
         <is>
-          <t>18:15-22:00</t>
+          <t>18:00-21:45</t>
         </is>
       </c>
       <c r="H11" s="3" t="n"/>
@@ -4038,12 +4118,12 @@
       <c r="A12" s="14" t="n"/>
       <c r="B12" s="3" t="inlineStr">
         <is>
-          <t>PEREZ GORMAS, ANTHONY</t>
+          <t>ZAPATA VILLANUEVA, FIORELLA YASMIN</t>
         </is>
       </c>
       <c r="C12" s="3" t="inlineStr">
         <is>
-          <t>14:30-18:15</t>
+          <t>14:15-18:00</t>
         </is>
       </c>
       <c r="D12" s="3" t="n"/>
@@ -4058,12 +4138,12 @@
       </c>
       <c r="B13" s="3" t="inlineStr">
         <is>
-          <t>IDME GOMEZ, MILAGROS</t>
+          <t>RAMOS FARFAN, BRYAN ENRIQUE</t>
         </is>
       </c>
       <c r="C13" s="3" t="inlineStr">
         <is>
-          <t>10:15-14:00</t>
+          <t>10:30-14:15</t>
         </is>
       </c>
       <c r="D13" s="3" t="n"/>
@@ -4072,12 +4152,12 @@
       </c>
       <c r="F13" s="3" t="inlineStr">
         <is>
-          <t>IDELFONSO MOTTA, JHOSSEP ANGELO</t>
+          <t>LEON TICONA, MARIA FERNANDA</t>
         </is>
       </c>
       <c r="G13" s="3" t="inlineStr">
         <is>
-          <t>19:00-19:00</t>
+          <t>18:15-22:00</t>
         </is>
       </c>
       <c r="H13" s="3" t="n"/>
@@ -4086,12 +4166,12 @@
       <c r="A14" s="14" t="n"/>
       <c r="B14" s="3" t="inlineStr">
         <is>
-          <t>ALARCON SANDOVAL, ADRIANA FERNANDA</t>
+          <t>SICHA JORGE, JOSE ANGELO</t>
         </is>
       </c>
       <c r="C14" s="3" t="inlineStr">
         <is>
-          <t>15:00-18:45</t>
+          <t>14:30-18:15</t>
         </is>
       </c>
       <c r="D14" s="3" t="n"/>
@@ -4106,7 +4186,7 @@
       </c>
       <c r="B15" s="3" t="inlineStr">
         <is>
-          <t>TARDILLO COPA, YOVANNA MELISSA</t>
+          <t>QUIQUIA MALLQUI, CYNTHIA ANGELLINE</t>
         </is>
       </c>
       <c r="C15" s="3" t="inlineStr">
@@ -4118,20 +4198,28 @@
       <c r="E15" s="14" t="n">
         <v>6</v>
       </c>
-      <c r="F15" s="3" t="n"/>
-      <c r="G15" s="3" t="n"/>
+      <c r="F15" s="3" t="inlineStr">
+        <is>
+          <t>VILCAPOMA CHILIN, JULISSA JAZMIN</t>
+        </is>
+      </c>
+      <c r="G15" s="3" t="inlineStr">
+        <is>
+          <t>18:45-22:30</t>
+        </is>
+      </c>
       <c r="H15" s="3" t="n"/>
     </row>
     <row r="16" ht="19.5" customHeight="1">
       <c r="A16" s="14" t="n"/>
       <c r="B16" s="3" t="inlineStr">
         <is>
-          <t>LA ROSA EUSEBIO, SHADIA SHAMIRA</t>
+          <t>NEIRA CARMEN, MIRIAM DALESKA</t>
         </is>
       </c>
       <c r="C16" s="3" t="inlineStr">
         <is>
-          <t>15:00-18:45</t>
+          <t>14:45-18:30</t>
         </is>
       </c>
       <c r="D16" s="3" t="n"/>
@@ -4158,20 +4246,28 @@
       <c r="E17" s="14" t="n">
         <v>7</v>
       </c>
-      <c r="F17" s="3" t="n"/>
-      <c r="G17" s="3" t="n"/>
+      <c r="F17" s="3" t="inlineStr">
+        <is>
+          <t>SUICA GOÑAZ, KEISY YVONNE</t>
+        </is>
+      </c>
+      <c r="G17" s="3" t="inlineStr">
+        <is>
+          <t>16:45-20:30</t>
+        </is>
+      </c>
       <c r="H17" s="3" t="n"/>
     </row>
     <row r="18" ht="19.5" customHeight="1">
       <c r="A18" s="14" t="n"/>
       <c r="B18" s="3" t="inlineStr">
         <is>
-          <t>GARRIDO SOTO, VICTORIA CELESTE</t>
+          <t>HUAMANI LOPEZ, DREYDI BELINDA</t>
         </is>
       </c>
       <c r="C18" s="3" t="inlineStr">
         <is>
-          <t>17:00-20:45</t>
+          <t>16:00-16:30</t>
         </is>
       </c>
       <c r="D18" s="3" t="n"/>
@@ -4186,12 +4282,12 @@
       </c>
       <c r="B19" s="3" t="inlineStr">
         <is>
-          <t>CASAPAICO RIVERA, ENZO MANUEL</t>
+          <t>BRANCACHO RAMIREZ, BRINDY</t>
         </is>
       </c>
       <c r="C19" s="3" t="inlineStr">
         <is>
-          <t>11:15-15:00</t>
+          <t>11:00-14:45</t>
         </is>
       </c>
       <c r="D19" s="3" t="n"/>
@@ -4206,12 +4302,12 @@
       <c r="A20" s="14" t="n"/>
       <c r="B20" s="3" t="inlineStr">
         <is>
-          <t>BONILLA SANCHEZ, RAUL FERNANDO</t>
+          <t>PEREZ GORMAS, ANTHONY</t>
         </is>
       </c>
       <c r="C20" s="3" t="inlineStr">
         <is>
-          <t>17:00-20:45</t>
+          <t>17:30-21:15</t>
         </is>
       </c>
       <c r="D20" s="3" t="n"/>
@@ -4226,12 +4322,12 @@
       </c>
       <c r="B21" s="3" t="inlineStr">
         <is>
-          <t>QUIQUIA MALLQUI, CYNTHIA ANGELLINE</t>
+          <t>YANQUI BRAVO, MIRIAN LUZ</t>
         </is>
       </c>
       <c r="C21" s="3" t="inlineStr">
         <is>
-          <t>11:15-15:00</t>
+          <t>13:00-13:30</t>
         </is>
       </c>
       <c r="D21" s="3" t="n"/>
@@ -4246,12 +4342,12 @@
       <c r="A22" s="14" t="n"/>
       <c r="B22" s="3" t="inlineStr">
         <is>
-          <t>FABIAN VALDIVIA, LINDSAY ZIYI</t>
+          <t>LA ROSA EUSEBIO, SHADIA SHAMIRA</t>
         </is>
       </c>
       <c r="C22" s="3" t="inlineStr">
         <is>
-          <t>18:00-21:45</t>
+          <t>17:45-21:30</t>
         </is>
       </c>
       <c r="D22" s="3" t="n"/>
@@ -4266,12 +4362,12 @@
       </c>
       <c r="B23" s="3" t="inlineStr">
         <is>
-          <t>NEIRA CARMEN, MIRIAM DALESKA</t>
+          <t>HUANCAS SHUAN, JOSELYN JAZMIN</t>
         </is>
       </c>
       <c r="C23" s="3" t="inlineStr">
         <is>
-          <t>18:00-21:45</t>
+          <t>18:15-22:00</t>
         </is>
       </c>
       <c r="D23" s="3" t="n"/>
@@ -4296,16 +4392,8 @@
       <c r="A25" s="14" t="n">
         <v>11</v>
       </c>
-      <c r="B25" s="3" t="inlineStr">
-        <is>
-          <t>VILCAPOMA CHILIN, JULISSA JAZMIN</t>
-        </is>
-      </c>
-      <c r="C25" s="3" t="inlineStr">
-        <is>
-          <t>18:30-21:15</t>
-        </is>
-      </c>
+      <c r="B25" s="3" t="n"/>
+      <c r="C25" s="3" t="n"/>
       <c r="D25" s="3" t="n"/>
       <c r="E25" s="14" t="n">
         <v>11</v>
@@ -4576,38 +4664,54 @@
       </c>
       <c r="B46" s="3" t="inlineStr">
         <is>
-          <t>QUIQUIA RICALDE, LILIA MARIA</t>
+          <t>QUISPE MONDRAGON, JUAN ALFONSO</t>
         </is>
       </c>
       <c r="C46" s="3" t="inlineStr">
         <is>
-          <t>07:00-16:00</t>
+          <t>07:00-10:45</t>
         </is>
       </c>
       <c r="D46" s="3" t="n"/>
       <c r="E46" s="14" t="n">
         <v>22</v>
       </c>
-      <c r="F46" s="3" t="n"/>
-      <c r="G46" s="3" t="n"/>
+      <c r="F46" s="3" t="inlineStr">
+        <is>
+          <t>ALVITE CORNEJO, ANGIE LUCERO</t>
+        </is>
+      </c>
+      <c r="G46" s="3" t="inlineStr">
+        <is>
+          <t>14:30-18:15</t>
+        </is>
+      </c>
       <c r="H46" s="3" t="n"/>
     </row>
     <row r="47" ht="18.75" customHeight="1">
       <c r="A47" s="14" t="n"/>
       <c r="B47" s="3" t="inlineStr">
         <is>
-          <t>SICHA JORGE, JOSE ANGELO</t>
+          <t>IDME GOMEZ, MILAGROS</t>
         </is>
       </c>
       <c r="C47" s="3" t="inlineStr">
         <is>
-          <t>16:15-20:00</t>
+          <t>10:45-14:30</t>
         </is>
       </c>
       <c r="D47" s="3" t="n"/>
       <c r="E47" s="14" t="n"/>
-      <c r="F47" s="3" t="n"/>
-      <c r="G47" s="3" t="n"/>
+      <c r="F47" s="3" t="inlineStr">
+        <is>
+          <t>MAYTA QUINTANA, ANDY KEVIN</t>
+        </is>
+      </c>
+      <c r="G47" s="3" t="inlineStr">
+        <is>
+          <t>18:15-22:00</t>
+        </is>
+      </c>
       <c r="H47" s="3" t="n"/>
     </row>
     <row r="48" ht="18.75" customHeight="1">
@@ -4696,7 +4800,7 @@
       </c>
       <c r="F53" s="8" t="inlineStr">
         <is>
-          <t>MACHCO HUARCA, NICOLAS AXEL</t>
+          <t>CHAHUA BENITO, JEFFERSON ALVARO</t>
         </is>
       </c>
       <c r="G53" s="8" t="inlineStr">
@@ -4730,7 +4834,7 @@
       </c>
       <c r="F54" s="12" t="inlineStr">
         <is>
-          <t>CHAHUA BENITO, JEFFERSON ALVARO</t>
+          <t>CONDORI FLORES, ROSARIO</t>
         </is>
       </c>
       <c r="G54" s="12" t="inlineStr">
@@ -4880,7 +4984,7 @@
       </c>
       <c r="B4" s="8" t="inlineStr">
         <is>
-          <t>QUISPE MONDRAGON, JUAN ALFONSO</t>
+          <t>JIMENEZ VERGARA, ADRIAN MARCELO</t>
         </is>
       </c>
       <c r="C4" s="8" t="inlineStr">
@@ -4894,23 +4998,15 @@
           <t>1 PREF</t>
         </is>
       </c>
-      <c r="F4" s="8" t="inlineStr">
-        <is>
-          <t>(T) BONILLA SANCHEZ, RAUL FERNANDO</t>
-        </is>
-      </c>
-      <c r="G4" s="8" t="inlineStr">
-        <is>
-          <t>17:30-20:45</t>
-        </is>
-      </c>
+      <c r="F4" s="8" t="n"/>
+      <c r="G4" s="8" t="n"/>
       <c r="H4" s="8" t="n"/>
     </row>
     <row r="5" ht="18.75" customHeight="1">
       <c r="A5" s="11" t="n"/>
       <c r="B5" s="12" t="inlineStr">
         <is>
-          <t>ROCA IBARAN, MIRLA VALENTINA</t>
+          <t>QUIQUIA MALLQUI, CYNTHIA ANGELLINE</t>
         </is>
       </c>
       <c r="C5" s="12" t="inlineStr">
@@ -4920,28 +5016,20 @@
       </c>
       <c r="D5" s="12" t="n"/>
       <c r="E5" s="11" t="n"/>
-      <c r="F5" s="12" t="inlineStr">
-        <is>
-          <t>(T) JIMENEZ TORERO, ASTRID GERALDINE</t>
-        </is>
-      </c>
-      <c r="G5" s="12" t="inlineStr">
-        <is>
-          <t>20:30-22:45</t>
-        </is>
-      </c>
+      <c r="F5" s="12" t="n"/>
+      <c r="G5" s="12" t="n"/>
       <c r="H5" s="12" t="n"/>
     </row>
     <row r="6" ht="19.5" customHeight="1">
       <c r="A6" s="9" t="n"/>
       <c r="B6" s="10" t="inlineStr">
         <is>
-          <t>LEON TICONA, MARIA FERNANDA</t>
+          <t>RAMOS TINOCO, JORDAN JAVIER</t>
         </is>
       </c>
       <c r="C6" s="10" t="inlineStr">
         <is>
-          <t>14:00-17:45</t>
+          <t>14:00-22:45</t>
         </is>
       </c>
       <c r="D6" s="10" t="n"/>
@@ -4956,38 +5044,54 @@
       </c>
       <c r="B7" s="3" t="inlineStr">
         <is>
-          <t>ALVITE CORNEJO, ANGIE LUCERO</t>
+          <t>ROCA IBARAN, MIRLA VALENTINA</t>
         </is>
       </c>
       <c r="C7" s="3" t="inlineStr">
         <is>
-          <t>09:00-12:45</t>
+          <t>07:45-11:30</t>
         </is>
       </c>
       <c r="D7" s="3" t="n"/>
       <c r="E7" s="14" t="n">
         <v>2</v>
       </c>
-      <c r="F7" s="3" t="n"/>
-      <c r="G7" s="3" t="n"/>
+      <c r="F7" s="3" t="inlineStr">
+        <is>
+          <t>HUANCAS SHUAN, JOSELYN JAZMIN</t>
+        </is>
+      </c>
+      <c r="G7" s="3" t="inlineStr">
+        <is>
+          <t>15:15-19:00</t>
+        </is>
+      </c>
       <c r="H7" s="3" t="n"/>
     </row>
     <row r="8" ht="19.5" customHeight="1">
       <c r="A8" s="14" t="n"/>
       <c r="B8" s="3" t="inlineStr">
         <is>
-          <t>JIMENEZ TORERO, ASTRID GERALDINE</t>
+          <t>MUÑOZ SOTOMAYOR, MIRIAN RAQUEL</t>
         </is>
       </c>
       <c r="C8" s="3" t="inlineStr">
         <is>
-          <t>13:45-20:30</t>
+          <t>11:30-15:15</t>
         </is>
       </c>
       <c r="D8" s="3" t="n"/>
       <c r="E8" s="14" t="n"/>
-      <c r="F8" s="3" t="n"/>
-      <c r="G8" s="3" t="n"/>
+      <c r="F8" s="3" t="inlineStr">
+        <is>
+          <t>IDELFONSO MOTTA, JHOSSEP ANGELO</t>
+        </is>
+      </c>
+      <c r="G8" s="3" t="inlineStr">
+        <is>
+          <t>19:00-22:45</t>
+        </is>
+      </c>
       <c r="H8" s="3" t="n"/>
     </row>
     <row r="9" ht="19.5" customHeight="1">
@@ -4996,12 +5100,12 @@
       </c>
       <c r="B9" s="3" t="inlineStr">
         <is>
-          <t>TARDILLO COPA, YOVANNA MELISSA</t>
+          <t>CASAPAICO RIVERA, ENZO MANUEL</t>
         </is>
       </c>
       <c r="C9" s="3" t="inlineStr">
         <is>
-          <t>09:45-13:30</t>
+          <t>08:15-12:00</t>
         </is>
       </c>
       <c r="D9" s="3" t="n"/>
@@ -5015,7 +5119,7 @@
       </c>
       <c r="G9" s="3" t="inlineStr">
         <is>
-          <t>18:00-21:45</t>
+          <t>15:45-19:30</t>
         </is>
       </c>
       <c r="H9" s="3" t="n"/>
@@ -5024,12 +5128,12 @@
       <c r="A10" s="14" t="n"/>
       <c r="B10" s="3" t="inlineStr">
         <is>
-          <t>ZAPATA VILLANUEVA, FIORELLA YASMIN</t>
+          <t>YANQUI BRAVO, MIRIAN LUZ</t>
         </is>
       </c>
       <c r="C10" s="3" t="inlineStr">
         <is>
-          <t>14:15-18:00</t>
+          <t>12:00-15:45</t>
         </is>
       </c>
       <c r="D10" s="3" t="n"/>
@@ -5044,12 +5148,12 @@
       </c>
       <c r="B11" s="3" t="inlineStr">
         <is>
-          <t>IDME GOMEZ, MILAGROS</t>
+          <t>RAMOS FARFAN, BRYAN ENRIQUE</t>
         </is>
       </c>
       <c r="C11" s="3" t="inlineStr">
         <is>
-          <t>10:15-14:00</t>
+          <t>09:45-13:30</t>
         </is>
       </c>
       <c r="D11" s="3" t="n"/>
@@ -5058,12 +5162,12 @@
       </c>
       <c r="F11" s="3" t="inlineStr">
         <is>
-          <t>MAYTA QUINTANA, ANDY KEVIN</t>
+          <t>NEIRA CARMEN, MIRIAM DALESKA</t>
         </is>
       </c>
       <c r="G11" s="3" t="inlineStr">
         <is>
-          <t>18:15-22:00</t>
+          <t>18:00-21:45</t>
         </is>
       </c>
       <c r="H11" s="3" t="n"/>
@@ -5072,12 +5176,12 @@
       <c r="A12" s="14" t="n"/>
       <c r="B12" s="3" t="inlineStr">
         <is>
-          <t>LA ROSA EUSEBIO, SHADIA SHAMIRA</t>
+          <t>ALVITE CORNEJO, ANGIE LUCERO</t>
         </is>
       </c>
       <c r="C12" s="3" t="inlineStr">
         <is>
-          <t>14:30-18:15</t>
+          <t>14:15-18:00</t>
         </is>
       </c>
       <c r="D12" s="3" t="n"/>
@@ -5097,7 +5201,7 @@
       </c>
       <c r="C13" s="3" t="inlineStr">
         <is>
-          <t>10:45-19:45</t>
+          <t>10:00-19:00</t>
         </is>
       </c>
       <c r="D13" s="3" t="n"/>
@@ -5110,8 +5214,16 @@
     </row>
     <row r="14" ht="19.5" customHeight="1">
       <c r="A14" s="14" t="n"/>
-      <c r="B14" s="3" t="n"/>
-      <c r="C14" s="3" t="n"/>
+      <c r="B14" s="3" t="inlineStr">
+        <is>
+          <t>POVEA CANTARO, FARID YASSER</t>
+        </is>
+      </c>
+      <c r="C14" s="3" t="inlineStr">
+        <is>
+          <t>19:00-22:45</t>
+        </is>
+      </c>
       <c r="D14" s="3" t="n"/>
       <c r="E14" s="14" t="n"/>
       <c r="F14" s="3" t="n"/>
@@ -5124,12 +5236,12 @@
       </c>
       <c r="B15" s="3" t="inlineStr">
         <is>
-          <t>MUÑOZ SOTOMAYOR, MIRIAN RAQUEL</t>
+          <t>SOTO VELAZCO, EMIR ALESSANDRO</t>
         </is>
       </c>
       <c r="C15" s="3" t="inlineStr">
         <is>
-          <t>10:45-14:30</t>
+          <t>10:15-14:00</t>
         </is>
       </c>
       <c r="D15" s="3" t="n"/>
@@ -5138,12 +5250,12 @@
       </c>
       <c r="F15" s="3" t="inlineStr">
         <is>
-          <t>IDELFONSO MOTTA, JHOSSEP ANGELO</t>
+          <t>MAYTA QUINTANA, ANDY KEVIN</t>
         </is>
       </c>
       <c r="G15" s="3" t="inlineStr">
         <is>
-          <t>19:00-22:45</t>
+          <t>18:15-22:00</t>
         </is>
       </c>
       <c r="H15" s="3" t="n"/>
@@ -5152,12 +5264,12 @@
       <c r="A16" s="14" t="n"/>
       <c r="B16" s="3" t="inlineStr">
         <is>
-          <t>PEREZ GORMAS, ANTHONY</t>
+          <t>ZAPATA VILLANUEVA, FIORELLA YASMIN</t>
         </is>
       </c>
       <c r="C16" s="3" t="inlineStr">
         <is>
-          <t>15:15-19:00</t>
+          <t>14:15-18:00</t>
         </is>
       </c>
       <c r="D16" s="3" t="n"/>
@@ -5172,12 +5284,12 @@
       </c>
       <c r="B17" s="3" t="inlineStr">
         <is>
-          <t>YANQUI BRAVO, MIRIAN LUZ</t>
+          <t>TARDILLO COPA, YOVANNA MELISSA</t>
         </is>
       </c>
       <c r="C17" s="3" t="inlineStr">
         <is>
-          <t>11:00-14:45</t>
+          <t>10:45-14:30</t>
         </is>
       </c>
       <c r="D17" s="3" t="n"/>
@@ -5186,12 +5298,12 @@
       </c>
       <c r="F17" s="3" t="inlineStr">
         <is>
-          <t>HUANCAS SHUAN, JOSELYN JAZMIN</t>
+          <t>PEREZ GORMAS, ANTHONY</t>
         </is>
       </c>
       <c r="G17" s="3" t="inlineStr">
         <is>
-          <t>19:00-22:45</t>
+          <t>18:15-22:00</t>
         </is>
       </c>
       <c r="H17" s="3" t="n"/>
@@ -5200,12 +5312,12 @@
       <c r="A18" s="14" t="n"/>
       <c r="B18" s="3" t="inlineStr">
         <is>
-          <t>ROMERO HAÑARI, VENUS ANUSKA</t>
+          <t>GARRIDO SOTO, VICTORIA CELESTE</t>
         </is>
       </c>
       <c r="C18" s="3" t="inlineStr">
         <is>
-          <t>15:30-19:00</t>
+          <t>14:30-18:15</t>
         </is>
       </c>
       <c r="D18" s="3" t="n"/>
@@ -5220,7 +5332,7 @@
       </c>
       <c r="B19" s="3" t="inlineStr">
         <is>
-          <t>BRANCACHO RAMIREZ, BRINDY</t>
+          <t>CUSI QUISPE, ANDREA ESTEFANY</t>
         </is>
       </c>
       <c r="C19" s="3" t="inlineStr">
@@ -5240,12 +5352,12 @@
       <c r="A20" s="14" t="n"/>
       <c r="B20" s="3" t="inlineStr">
         <is>
-          <t>POVEA CANTARO, FARID YASSER</t>
+          <t>ROMERO HAÑARI, VENUS ANUSKA</t>
         </is>
       </c>
       <c r="C20" s="3" t="inlineStr">
         <is>
-          <t>16:15-20:00</t>
+          <t>15:15-22:45</t>
         </is>
       </c>
       <c r="D20" s="3" t="n"/>
@@ -5260,42 +5372,26 @@
       </c>
       <c r="B21" s="3" t="inlineStr">
         <is>
-          <t>CASAPAICO RIVERA, ENZO MANUEL</t>
+          <t>SICHA JORGE, JOSE ANGELO</t>
         </is>
       </c>
       <c r="C21" s="3" t="inlineStr">
         <is>
-          <t>11:15-15:00</t>
+          <t>17:00-20:45</t>
         </is>
       </c>
       <c r="D21" s="3" t="n"/>
       <c r="E21" s="14" t="n">
         <v>9</v>
       </c>
-      <c r="F21" s="3" t="inlineStr">
-        <is>
-          <t>FABIAN VALDIVIA, LINDSAY ZIYI</t>
-        </is>
-      </c>
-      <c r="G21" s="3" t="inlineStr">
-        <is>
-          <t>17:45-21:30</t>
-        </is>
-      </c>
+      <c r="F21" s="3" t="n"/>
+      <c r="G21" s="3" t="n"/>
       <c r="H21" s="3" t="n"/>
     </row>
     <row r="22" ht="19.5" customHeight="1">
       <c r="A22" s="14" t="n"/>
-      <c r="B22" s="3" t="inlineStr">
-        <is>
-          <t>BONILLA SANCHEZ, RAUL FERNANDO</t>
-        </is>
-      </c>
-      <c r="C22" s="3" t="inlineStr">
-        <is>
-          <t>17:00-17:30</t>
-        </is>
-      </c>
+      <c r="B22" s="3" t="n"/>
+      <c r="C22" s="3" t="n"/>
       <c r="D22" s="3" t="n"/>
       <c r="E22" s="14" t="n"/>
       <c r="F22" s="3" t="n"/>
@@ -5308,12 +5404,12 @@
       </c>
       <c r="B23" s="3" t="inlineStr">
         <is>
-          <t>RAMOS FARFAN, BRYAN ENRIQUE</t>
+          <t>ALARCON SANDOVAL, ADRIANA FERNANDA</t>
         </is>
       </c>
       <c r="C23" s="3" t="inlineStr">
         <is>
-          <t>18:00-21:45</t>
+          <t>17:45-21:30</t>
         </is>
       </c>
       <c r="D23" s="3" t="n"/>
@@ -5338,8 +5434,16 @@
       <c r="A25" s="14" t="n">
         <v>11</v>
       </c>
-      <c r="B25" s="3" t="n"/>
-      <c r="C25" s="3" t="n"/>
+      <c r="B25" s="3" t="inlineStr">
+        <is>
+          <t>RICAPA RAMOS, MILAGROS PATRICIA</t>
+        </is>
+      </c>
+      <c r="C25" s="3" t="inlineStr">
+        <is>
+          <t>18:30-22:00</t>
+        </is>
+      </c>
       <c r="D25" s="3" t="n"/>
       <c r="E25" s="14" t="n">
         <v>11</v>
@@ -5575,7 +5679,7 @@
       </c>
       <c r="C44" s="3" t="inlineStr">
         <is>
-          <t>09:00-18:00</t>
+          <t>09:15-18:15</t>
         </is>
       </c>
       <c r="D44" s="3" t="n"/>
@@ -5588,16 +5692,8 @@
     </row>
     <row r="45" ht="18.75" customHeight="1">
       <c r="A45" s="14" t="n"/>
-      <c r="B45" s="3" t="inlineStr">
-        <is>
-          <t>RICAPA RAMOS, MILAGROS PATRICIA</t>
-        </is>
-      </c>
-      <c r="C45" s="3" t="inlineStr">
-        <is>
-          <t>18:00-22:45</t>
-        </is>
-      </c>
+      <c r="B45" s="3" t="n"/>
+      <c r="C45" s="3" t="n"/>
       <c r="D45" s="3" t="n"/>
       <c r="E45" s="14" t="n"/>
       <c r="F45" s="3" t="n"/>
@@ -5610,12 +5706,12 @@
       </c>
       <c r="B46" s="3" t="inlineStr">
         <is>
-          <t>JIMENEZ VERGARA, ADRIAN MARCELO</t>
+          <t>QUISPE MONDRAGON, JUAN ALFONSO</t>
         </is>
       </c>
       <c r="C46" s="3" t="inlineStr">
         <is>
-          <t>07:45-11:30</t>
+          <t>07:00-10:45</t>
         </is>
       </c>
       <c r="D46" s="3" t="n"/>
@@ -5624,12 +5720,12 @@
       </c>
       <c r="F46" s="3" t="inlineStr">
         <is>
-          <t>GARRIDO SOTO, VICTORIA CELESTE</t>
+          <t>HUAMANI LOPEZ, DREYDI BELINDA</t>
         </is>
       </c>
       <c r="G46" s="3" t="inlineStr">
         <is>
-          <t>17:00-20:45</t>
+          <t>14:30-18:15</t>
         </is>
       </c>
       <c r="H46" s="3" t="n"/>
@@ -5643,21 +5739,37 @@
       </c>
       <c r="C47" s="3" t="inlineStr">
         <is>
-          <t>12:45-16:30</t>
+          <t>10:45-14:30</t>
         </is>
       </c>
       <c r="D47" s="3" t="n"/>
       <c r="E47" s="14" t="n"/>
-      <c r="F47" s="3" t="n"/>
-      <c r="G47" s="3" t="n"/>
+      <c r="F47" s="3" t="inlineStr">
+        <is>
+          <t>BONILLA SANCHEZ, RAUL FERNANDO</t>
+        </is>
+      </c>
+      <c r="G47" s="3" t="inlineStr">
+        <is>
+          <t>18:15-22:00</t>
+        </is>
+      </c>
       <c r="H47" s="3" t="n"/>
     </row>
     <row r="48" ht="18.75" customHeight="1">
       <c r="A48" s="14" t="n">
         <v>23</v>
       </c>
-      <c r="B48" s="3" t="n"/>
-      <c r="C48" s="3" t="n"/>
+      <c r="B48" s="3" t="inlineStr">
+        <is>
+          <t>ROMERO HAÑARI, VENUS ANUSKA</t>
+        </is>
+      </c>
+      <c r="C48" s="3" t="inlineStr">
+        <is>
+          <t>15:15-22:45</t>
+        </is>
+      </c>
       <c r="D48" s="3" t="n"/>
       <c r="E48" s="14" t="n">
         <v>23</v>
@@ -5738,7 +5850,7 @@
       </c>
       <c r="F53" s="8" t="inlineStr">
         <is>
-          <t>CHAHUA BENITO, JEFFERSON ALVARO</t>
+          <t>MACHCO HUARCA, NICOLAS AXEL</t>
         </is>
       </c>
       <c r="G53" s="8" t="inlineStr">
@@ -5756,7 +5868,7 @@
       </c>
       <c r="B54" s="3" t="inlineStr">
         <is>
-          <t>MACHCO HUARCA, NICOLAS AXEL</t>
+          <t>CHAHUA BENITO, JEFFERSON ALVARO</t>
         </is>
       </c>
       <c r="C54" s="3" t="inlineStr">
@@ -5922,12 +6034,12 @@
       </c>
       <c r="B4" s="8" t="inlineStr">
         <is>
-          <t>LOPEZ SANCHEZ, NELLY ANDREA</t>
+          <t>SOTO VELAZCO, EMIR ALESSANDRO</t>
         </is>
       </c>
       <c r="C4" s="8" t="inlineStr">
         <is>
-          <t>07:30-16:15</t>
+          <t>06:30-10:15</t>
         </is>
       </c>
       <c r="D4" s="8" t="n"/>
@@ -5938,12 +6050,12 @@
       </c>
       <c r="F4" s="8" t="inlineStr">
         <is>
-          <t>(T) IDELFONSO MOTTA, JHOSSEP ANGELO</t>
+          <t>(T) TITO LAURA, NANCY FIORELLA</t>
         </is>
       </c>
       <c r="G4" s="8" t="inlineStr">
         <is>
-          <t>21:00-22:45</t>
+          <t>22:00-22:45</t>
         </is>
       </c>
       <c r="H4" s="8" t="n"/>
@@ -5952,12 +6064,12 @@
       <c r="A5" s="11" t="n"/>
       <c r="B5" s="12" t="inlineStr">
         <is>
-          <t>(T) PEREZ GORMAS, ANTHONY</t>
+          <t>LOPEZ SANCHEZ, NELLY ANDREA</t>
         </is>
       </c>
       <c r="C5" s="12" t="inlineStr">
         <is>
-          <t>16:00-19:00</t>
+          <t>10:00-19:00</t>
         </is>
       </c>
       <c r="D5" s="12" t="n"/>
@@ -5975,7 +6087,7 @@
       </c>
       <c r="C6" s="10" t="inlineStr">
         <is>
-          <t>18:45-21:15</t>
+          <t>18:45-22:15</t>
         </is>
       </c>
       <c r="D6" s="10" t="n"/>
@@ -5990,32 +6102,40 @@
       </c>
       <c r="B7" s="3" t="inlineStr">
         <is>
-          <t>TARDILLO COPA, YOVANNA MELISSA</t>
+          <t>CUSI QUISPE, ANDREA ESTEFANY</t>
         </is>
       </c>
       <c r="C7" s="3" t="inlineStr">
         <is>
-          <t>08:30-12:15</t>
+          <t>08:00-11:45</t>
         </is>
       </c>
       <c r="D7" s="3" t="n"/>
       <c r="E7" s="14" t="n">
         <v>2</v>
       </c>
-      <c r="F7" s="3" t="n"/>
-      <c r="G7" s="3" t="n"/>
+      <c r="F7" s="3" t="inlineStr">
+        <is>
+          <t>ALARCON SANDOVAL, ADRIANA FERNANDA</t>
+        </is>
+      </c>
+      <c r="G7" s="3" t="inlineStr">
+        <is>
+          <t>17:30-21:15</t>
+        </is>
+      </c>
       <c r="H7" s="3" t="n"/>
     </row>
     <row r="8" ht="19.5" customHeight="1">
       <c r="A8" s="14" t="n"/>
       <c r="B8" s="3" t="inlineStr">
         <is>
-          <t>PARIONA CARRASCO, YAZMIN</t>
+          <t>ROMERO HAÑARI, VENUS ANUSKA</t>
         </is>
       </c>
       <c r="C8" s="3" t="inlineStr">
         <is>
-          <t>12:15-21:15</t>
+          <t>12:30-17:30</t>
         </is>
       </c>
       <c r="D8" s="3" t="n"/>
@@ -6030,40 +6150,32 @@
       </c>
       <c r="B9" s="3" t="inlineStr">
         <is>
-          <t>SOTO VELAZCO, EMIR ALESSANDRO</t>
+          <t>JIMENEZ VERGARA, ADRIAN MARCELO</t>
         </is>
       </c>
       <c r="C9" s="3" t="inlineStr">
         <is>
-          <t>09:00-12:45</t>
+          <t>08:30-12:15</t>
         </is>
       </c>
       <c r="D9" s="3" t="n"/>
       <c r="E9" s="14" t="n">
         <v>3</v>
       </c>
-      <c r="F9" s="3" t="inlineStr">
-        <is>
-          <t>SICHA JORGE, JOSE ANGELO</t>
-        </is>
-      </c>
-      <c r="G9" s="3" t="inlineStr">
-        <is>
-          <t>16:30-20:15</t>
-        </is>
-      </c>
+      <c r="F9" s="3" t="n"/>
+      <c r="G9" s="3" t="n"/>
       <c r="H9" s="3" t="n"/>
     </row>
     <row r="10" ht="19.5" customHeight="1">
       <c r="A10" s="14" t="n"/>
       <c r="B10" s="3" t="inlineStr">
         <is>
-          <t>HUAMANI LOPEZ, DREYDI BELINDA</t>
+          <t>RICAPA RAMOS, MILAGROS PATRICIA</t>
         </is>
       </c>
       <c r="C10" s="3" t="inlineStr">
         <is>
-          <t>12:45-16:30</t>
+          <t>12:45-21:45</t>
         </is>
       </c>
       <c r="D10" s="3" t="n"/>
@@ -6078,40 +6190,32 @@
       </c>
       <c r="B11" s="3" t="inlineStr">
         <is>
-          <t>RAMOS TINOCO, JORDAN JAVIER</t>
+          <t>RAMOS FARFAN, BRYAN ENRIQUE</t>
         </is>
       </c>
       <c r="C11" s="3" t="inlineStr">
         <is>
-          <t>09:00-14:00</t>
+          <t>09:00-12:45</t>
         </is>
       </c>
       <c r="D11" s="3" t="n"/>
       <c r="E11" s="14" t="n">
         <v>4</v>
       </c>
-      <c r="F11" s="3" t="inlineStr">
-        <is>
-          <t>FABIAN VALDIVIA, LINDSAY ZIYI</t>
-        </is>
-      </c>
-      <c r="G11" s="3" t="inlineStr">
-        <is>
-          <t>18:00-21:45</t>
-        </is>
-      </c>
+      <c r="F11" s="3" t="n"/>
+      <c r="G11" s="3" t="n"/>
       <c r="H11" s="3" t="n"/>
     </row>
     <row r="12" ht="19.5" customHeight="1">
       <c r="A12" s="14" t="n"/>
       <c r="B12" s="3" t="inlineStr">
         <is>
-          <t>ZAPATA VILLANUEVA, FIORELLA YASMIN</t>
+          <t>TITO LAURA, NANCY FIORELLA</t>
         </is>
       </c>
       <c r="C12" s="3" t="inlineStr">
         <is>
-          <t>14:15-18:00</t>
+          <t>13:45-22:00</t>
         </is>
       </c>
       <c r="D12" s="3" t="n"/>
@@ -6126,32 +6230,40 @@
       </c>
       <c r="B13" s="3" t="inlineStr">
         <is>
-          <t>HUAMANI HUAMAN, MARICRUZ DESIDE</t>
+          <t>RAMOS TINOCO, JORDAN JAVIER</t>
         </is>
       </c>
       <c r="C13" s="3" t="inlineStr">
         <is>
-          <t>10:00-13:45</t>
+          <t>09:30-13:15</t>
         </is>
       </c>
       <c r="D13" s="3" t="n"/>
       <c r="E13" s="14" t="n">
         <v>5</v>
       </c>
-      <c r="F13" s="3" t="n"/>
-      <c r="G13" s="3" t="n"/>
+      <c r="F13" s="3" t="inlineStr">
+        <is>
+          <t>HUAMANI HUAMAN, MARICRUZ DESIDE</t>
+        </is>
+      </c>
+      <c r="G13" s="3" t="inlineStr">
+        <is>
+          <t>18:00-21:45</t>
+        </is>
+      </c>
       <c r="H13" s="3" t="n"/>
     </row>
     <row r="14" ht="19.5" customHeight="1">
       <c r="A14" s="14" t="n"/>
       <c r="B14" s="3" t="inlineStr">
         <is>
-          <t>RICAPA RAMOS, MILAGROS PATRICIA</t>
+          <t>ZAPATA VILLANUEVA, FIORELLA YASMIN</t>
         </is>
       </c>
       <c r="C14" s="3" t="inlineStr">
         <is>
-          <t>14:15-22:00</t>
+          <t>14:00-17:45</t>
         </is>
       </c>
       <c r="D14" s="3" t="n"/>
@@ -6166,12 +6278,12 @@
       </c>
       <c r="B15" s="3" t="inlineStr">
         <is>
-          <t>SUICA GOÑAZ, KEISY YVONNE</t>
+          <t>TARDILLO COPA, YOVANNA MELISSA</t>
         </is>
       </c>
       <c r="C15" s="3" t="inlineStr">
         <is>
-          <t>10:30-14:15</t>
+          <t>10:00-13:45</t>
         </is>
       </c>
       <c r="D15" s="3" t="n"/>
@@ -6180,12 +6292,12 @@
       </c>
       <c r="F15" s="3" t="inlineStr">
         <is>
-          <t>IDELFONSO MOTTA, JHOSSEP ANGELO</t>
+          <t>GARRIDO SOTO, VICTORIA CELESTE</t>
         </is>
       </c>
       <c r="G15" s="3" t="inlineStr">
         <is>
-          <t>19:00-21:00</t>
+          <t>18:30-22:15</t>
         </is>
       </c>
       <c r="H15" s="3" t="n"/>
@@ -6194,12 +6306,12 @@
       <c r="A16" s="14" t="n"/>
       <c r="B16" s="3" t="inlineStr">
         <is>
-          <t>YANQUI BRAVO, MIRIAN LUZ</t>
+          <t>HUAMANI LOPEZ, DREYDI BELINDA</t>
         </is>
       </c>
       <c r="C16" s="3" t="inlineStr">
         <is>
-          <t>15:00-18:45</t>
+          <t>14:45-18:30</t>
         </is>
       </c>
       <c r="D16" s="3" t="n"/>
@@ -6214,12 +6326,12 @@
       </c>
       <c r="B17" s="3" t="inlineStr">
         <is>
-          <t>JIMENEZ VERGARA, ADRIAN MARCELO</t>
+          <t>SUICA GOÑAZ, KEISY YVONNE</t>
         </is>
       </c>
       <c r="C17" s="3" t="inlineStr">
         <is>
-          <t>10:30-14:15</t>
+          <t>10:15-14:00</t>
         </is>
       </c>
       <c r="D17" s="3" t="n"/>
@@ -6228,7 +6340,7 @@
       </c>
       <c r="F17" s="3" t="inlineStr">
         <is>
-          <t>MAYTA QUINTANA, ANDY KEVIN</t>
+          <t>YANQUI BRAVO, MIRIAN LUZ</t>
         </is>
       </c>
       <c r="G17" s="3" t="inlineStr">
@@ -6242,7 +6354,7 @@
       <c r="A18" s="14" t="n"/>
       <c r="B18" s="3" t="inlineStr">
         <is>
-          <t>LA ROSA EUSEBIO, SHADIA SHAMIRA</t>
+          <t>NEIRA CARMEN, MIRIAM DALESKA</t>
         </is>
       </c>
       <c r="C18" s="3" t="inlineStr">
@@ -6262,27 +6374,35 @@
       </c>
       <c r="B19" s="3" t="inlineStr">
         <is>
-          <t>QUIQUIA MALLQUI, CYNTHIA ANGELLINE</t>
+          <t>IDME GOMEZ, MILAGROS</t>
         </is>
       </c>
       <c r="C19" s="3" t="inlineStr">
         <is>
-          <t>10:45-14:30</t>
+          <t>10:30-14:15</t>
         </is>
       </c>
       <c r="D19" s="3" t="n"/>
       <c r="E19" s="14" t="n">
         <v>8</v>
       </c>
-      <c r="F19" s="3" t="n"/>
-      <c r="G19" s="3" t="n"/>
+      <c r="F19" s="3" t="inlineStr">
+        <is>
+          <t>ROA ZARATE, ELIZABETH LUCY</t>
+        </is>
+      </c>
+      <c r="G19" s="3" t="inlineStr">
+        <is>
+          <t>19:00-22:45</t>
+        </is>
+      </c>
       <c r="H19" s="3" t="n"/>
     </row>
     <row r="20" ht="19.5" customHeight="1">
       <c r="A20" s="14" t="n"/>
       <c r="B20" s="3" t="inlineStr">
         <is>
-          <t>NEIRA CARMEN, MIRIAM DALESKA</t>
+          <t>FABIAN VALDIVIA, LINDSAY ZIYI</t>
         </is>
       </c>
       <c r="C20" s="3" t="inlineStr">
@@ -6302,40 +6422,32 @@
       </c>
       <c r="B21" s="3" t="inlineStr">
         <is>
-          <t>IDME GOMEZ, MILAGROS</t>
+          <t>QUIQUIA MALLQUI, CYNTHIA ANGELLINE</t>
         </is>
       </c>
       <c r="C21" s="3" t="inlineStr">
         <is>
-          <t>11:00-14:45</t>
+          <t>10:30-14:15</t>
         </is>
       </c>
       <c r="D21" s="3" t="n"/>
       <c r="E21" s="14" t="n">
         <v>9</v>
       </c>
-      <c r="F21" s="3" t="inlineStr">
-        <is>
-          <t>HUANCAS SHUAN, JOSELYN JAZMIN</t>
-        </is>
-      </c>
-      <c r="G21" s="3" t="inlineStr">
-        <is>
-          <t>17:30-21:15</t>
-        </is>
-      </c>
+      <c r="F21" s="3" t="n"/>
+      <c r="G21" s="3" t="n"/>
       <c r="H21" s="3" t="n"/>
     </row>
     <row r="22" ht="19.5" customHeight="1">
       <c r="A22" s="14" t="n"/>
       <c r="B22" s="3" t="inlineStr">
         <is>
-          <t>PEREZ GORMAS, ANTHONY</t>
+          <t>LEON TICONA, MARIA FERNANDA</t>
         </is>
       </c>
       <c r="C22" s="3" t="inlineStr">
         <is>
-          <t>15:15-16:00</t>
+          <t>16:15-20:00</t>
         </is>
       </c>
       <c r="D22" s="3" t="n"/>
@@ -6350,7 +6462,7 @@
       </c>
       <c r="B23" s="3" t="inlineStr">
         <is>
-          <t>BRANCACHO RAMIREZ, BRINDY</t>
+          <t>MUÑOZ SOTOMAYOR, MIRIAN RAQUEL</t>
         </is>
       </c>
       <c r="C23" s="3" t="inlineStr">
@@ -6390,7 +6502,7 @@
       </c>
       <c r="B25" s="3" t="inlineStr">
         <is>
-          <t>POVEA CANTARO, FARID YASSER</t>
+          <t>ROCA IBARAN, MIRLA VALENTINA</t>
         </is>
       </c>
       <c r="C25" s="3" t="inlineStr">
@@ -6402,20 +6514,28 @@
       <c r="E25" s="14" t="n">
         <v>11</v>
       </c>
-      <c r="F25" s="3" t="n"/>
-      <c r="G25" s="3" t="n"/>
+      <c r="F25" s="3" t="inlineStr">
+        <is>
+          <t>HUANCAS SHUAN, JOSELYN JAZMIN</t>
+        </is>
+      </c>
+      <c r="G25" s="3" t="inlineStr">
+        <is>
+          <t>19:00-22:45</t>
+        </is>
+      </c>
       <c r="H25" s="3" t="n"/>
     </row>
     <row r="26" ht="18.75" customHeight="1">
       <c r="A26" s="14" t="n"/>
       <c r="B26" s="3" t="inlineStr">
         <is>
-          <t>RAMOS FARFAN, BRYAN ENRIQUE</t>
+          <t>VILCAPOMA CHILIN, JULISSA JAZMIN</t>
         </is>
       </c>
       <c r="C26" s="3" t="inlineStr">
         <is>
-          <t>18:15-22:00</t>
+          <t>18:30-18:45</t>
         </is>
       </c>
       <c r="D26" s="3" t="n"/>
@@ -6430,12 +6550,12 @@
       </c>
       <c r="B27" s="3" t="inlineStr">
         <is>
-          <t>ROMERO HAÑARI, VENUS ANUSKA</t>
+          <t>BRANCACHO RAMIREZ, BRINDY</t>
         </is>
       </c>
       <c r="C27" s="3" t="inlineStr">
         <is>
-          <t>11:00-20:00</t>
+          <t>11:00-14:45</t>
         </is>
       </c>
       <c r="D27" s="3" t="n"/>
@@ -6462,12 +6582,12 @@
       </c>
       <c r="B29" s="3" t="inlineStr">
         <is>
-          <t>CASAPAICO RIVERA, ENZO MANUEL</t>
+          <t>POVEA CANTARO, FARID YASSER</t>
         </is>
       </c>
       <c r="C29" s="3" t="inlineStr">
         <is>
-          <t>11:15-15:00</t>
+          <t>11:30-15:15</t>
         </is>
       </c>
       <c r="D29" s="3" t="n"/>
@@ -6480,16 +6600,8 @@
     </row>
     <row r="30" ht="18.75" customHeight="1">
       <c r="A30" s="14" t="n"/>
-      <c r="B30" s="3" t="inlineStr">
-        <is>
-          <t>VILCAPOMA CHILIN, JULISSA JAZMIN</t>
-        </is>
-      </c>
-      <c r="C30" s="3" t="inlineStr">
-        <is>
-          <t>18:30-18:45</t>
-        </is>
-      </c>
+      <c r="B30" s="3" t="n"/>
+      <c r="C30" s="3" t="n"/>
       <c r="D30" s="3" t="n"/>
       <c r="E30" s="14" t="n"/>
       <c r="F30" s="3" t="n"/>
@@ -6660,32 +6772,40 @@
       </c>
       <c r="B44" s="3" t="inlineStr">
         <is>
-          <t>MARTINEZ PAZ, ROCIO ESPERANZA</t>
+          <t>BARRIENTOS JERI, MILAGROS NICOL</t>
         </is>
       </c>
       <c r="C44" s="3" t="inlineStr">
         <is>
-          <t>10:00-19:00</t>
+          <t>07:00-14:30</t>
         </is>
       </c>
       <c r="D44" s="3" t="n"/>
       <c r="E44" s="14" t="n">
         <v>21</v>
       </c>
-      <c r="F44" s="3" t="n"/>
-      <c r="G44" s="3" t="n"/>
+      <c r="F44" s="3" t="inlineStr">
+        <is>
+          <t>MAYTA QUINTANA, ANDY KEVIN</t>
+        </is>
+      </c>
+      <c r="G44" s="3" t="inlineStr">
+        <is>
+          <t>18:15-22:00</t>
+        </is>
+      </c>
       <c r="H44" s="3" t="n"/>
     </row>
     <row r="45" ht="18.75" customHeight="1">
       <c r="A45" s="14" t="n"/>
       <c r="B45" s="3" t="inlineStr">
         <is>
-          <t>ROA ZARATE, ELIZABETH LUCY</t>
+          <t>LA ROSA EUSEBIO, SHADIA SHAMIRA</t>
         </is>
       </c>
       <c r="C45" s="3" t="inlineStr">
         <is>
-          <t>19:00-22:45</t>
+          <t>14:30-18:15</t>
         </is>
       </c>
       <c r="D45" s="3" t="n"/>
@@ -6720,7 +6840,7 @@
       <c r="A47" s="14" t="n"/>
       <c r="B47" s="3" t="inlineStr">
         <is>
-          <t>ALARCON SANDOVAL, ADRIANA FERNANDA</t>
+          <t>SICHA JORGE, JOSE ANGELO</t>
         </is>
       </c>
       <c r="C47" s="3" t="inlineStr">
@@ -6738,8 +6858,16 @@
       <c r="A48" s="14" t="n">
         <v>23</v>
       </c>
-      <c r="B48" s="3" t="n"/>
-      <c r="C48" s="3" t="n"/>
+      <c r="B48" s="3" t="inlineStr">
+        <is>
+          <t>YANQUI BRAVO, MIRIAN LUZ</t>
+        </is>
+      </c>
+      <c r="C48" s="3" t="inlineStr">
+        <is>
+          <t>19:00-22:45</t>
+        </is>
+      </c>
       <c r="D48" s="3" t="n"/>
       <c r="E48" s="14" t="n">
         <v>23</v>
@@ -6804,12 +6932,12 @@
       </c>
       <c r="B53" s="3" t="inlineStr">
         <is>
-          <t>VILLANUEVA RAMIREZ, KAREN SOFIA</t>
+          <t>HUANUCO VICUÑA, ABIGAIL LUZ</t>
         </is>
       </c>
       <c r="C53" s="3" t="inlineStr">
         <is>
-          <t>10:45-14:30</t>
+          <t>07:00-10:45</t>
         </is>
       </c>
       <c r="D53" s="3" t="n"/>
@@ -6838,12 +6966,12 @@
       </c>
       <c r="B54" s="3" t="inlineStr">
         <is>
-          <t>HUANUCO VICUÑA, ABIGAIL LUZ</t>
+          <t>VILLANUEVA RAMIREZ, KAREN SOFIA</t>
         </is>
       </c>
       <c r="C54" s="3" t="inlineStr">
         <is>
-          <t>14:30-18:15</t>
+          <t>10:45-14:30</t>
         </is>
       </c>
       <c r="D54" s="3" t="n"/>
@@ -7009,7 +7137,7 @@
       </c>
       <c r="C4" s="8" t="inlineStr">
         <is>
-          <t>06:30-15:30</t>
+          <t>06:30-15:15</t>
         </is>
       </c>
       <c r="D4" s="8" t="n"/>
@@ -7020,12 +7148,12 @@
       </c>
       <c r="F4" s="8" t="inlineStr">
         <is>
-          <t>(T) NEIRA CARMEN, MIRIAM DALESKA</t>
+          <t>(T) ROMERO HAÑARI, VENUS ANUSKA</t>
         </is>
       </c>
       <c r="G4" s="8" t="inlineStr">
         <is>
-          <t>21:15-22:45</t>
+          <t>22:00-22:45</t>
         </is>
       </c>
       <c r="H4" s="8" t="n"/>
@@ -7034,12 +7162,12 @@
       <c r="A5" s="11" t="n"/>
       <c r="B5" s="12" t="inlineStr">
         <is>
-          <t>MAYTA QUINTANA, ANDY KEVIN</t>
+          <t>MUÑOZ SOTOMAYOR, MIRIAN RAQUEL</t>
         </is>
       </c>
       <c r="C5" s="12" t="inlineStr">
         <is>
-          <t>15:15-19:00</t>
+          <t>15:00-18:45</t>
         </is>
       </c>
       <c r="D5" s="12" t="n"/>
@@ -7052,12 +7180,12 @@
       <c r="A6" s="9" t="n"/>
       <c r="B6" s="10" t="inlineStr">
         <is>
-          <t>(T) VILCAPOMA CHILIN, JULISSA JAZMIN</t>
+          <t>VILCAPOMA CHILIN, JULISSA JAZMIN</t>
         </is>
       </c>
       <c r="C6" s="10" t="inlineStr">
         <is>
-          <t>18:45-21:30</t>
+          <t>18:30-22:15</t>
         </is>
       </c>
       <c r="D6" s="10" t="n"/>
@@ -7072,12 +7200,12 @@
       </c>
       <c r="B7" s="3" t="inlineStr">
         <is>
-          <t>ROCA IBARAN, MIRLA VALENTINA</t>
+          <t>CUSI QUISPE, ANDREA ESTEFANY</t>
         </is>
       </c>
       <c r="C7" s="3" t="inlineStr">
         <is>
-          <t>08:30-12:15</t>
+          <t>08:00-11:45</t>
         </is>
       </c>
       <c r="D7" s="3" t="n"/>
@@ -7097,7 +7225,7 @@
       </c>
       <c r="C8" s="3" t="inlineStr">
         <is>
-          <t>12:45-21:45</t>
+          <t>13:00-22:00</t>
         </is>
       </c>
       <c r="D8" s="3" t="n"/>
@@ -7112,12 +7240,12 @@
       </c>
       <c r="B9" s="3" t="inlineStr">
         <is>
-          <t>IDME GOMEZ, MILAGROS</t>
+          <t>JIMENEZ TORERO, ASTRID GERALDINE</t>
         </is>
       </c>
       <c r="C9" s="3" t="inlineStr">
         <is>
-          <t>09:00-12:45</t>
+          <t>08:45-17:45</t>
         </is>
       </c>
       <c r="D9" s="3" t="n"/>
@@ -7132,12 +7260,12 @@
       <c r="A10" s="14" t="n"/>
       <c r="B10" s="3" t="inlineStr">
         <is>
-          <t>ROMERO HAÑARI, VENUS ANUSKA</t>
+          <t>IDELFONSO MOTTA, JHOSSEP ANGELO</t>
         </is>
       </c>
       <c r="C10" s="3" t="inlineStr">
         <is>
-          <t>13:30-22:30</t>
+          <t>18:00-21:45</t>
         </is>
       </c>
       <c r="D10" s="3" t="n"/>
@@ -7152,40 +7280,32 @@
       </c>
       <c r="B11" s="3" t="inlineStr">
         <is>
-          <t>MUÑOZ SOTOMAYOR, MIRIAN RAQUEL</t>
+          <t>ALVITE CORNEJO, ANGIE LUCERO</t>
         </is>
       </c>
       <c r="C11" s="3" t="inlineStr">
         <is>
-          <t>10:30-14:15</t>
+          <t>09:00-12:45</t>
         </is>
       </c>
       <c r="D11" s="3" t="n"/>
       <c r="E11" s="14" t="n">
         <v>4</v>
       </c>
-      <c r="F11" s="3" t="inlineStr">
-        <is>
-          <t>RAMOS FARFAN, BRYAN ENRIQUE</t>
-        </is>
-      </c>
-      <c r="G11" s="3" t="inlineStr">
-        <is>
-          <t>18:00-21:45</t>
-        </is>
-      </c>
+      <c r="F11" s="3" t="n"/>
+      <c r="G11" s="3" t="n"/>
       <c r="H11" s="3" t="n"/>
     </row>
     <row r="12" ht="19.5" customHeight="1">
       <c r="A12" s="14" t="n"/>
       <c r="B12" s="3" t="inlineStr">
         <is>
-          <t>HUAMANI LOPEZ, DREYDI BELINDA</t>
+          <t>ROMERO HAÑARI, VENUS ANUSKA</t>
         </is>
       </c>
       <c r="C12" s="3" t="inlineStr">
         <is>
-          <t>14:15-18:00</t>
+          <t>13:45-22:00</t>
         </is>
       </c>
       <c r="D12" s="3" t="n"/>
@@ -7200,40 +7320,32 @@
       </c>
       <c r="B13" s="3" t="inlineStr">
         <is>
-          <t>SUICA GOÑAZ, KEISY YVONNE</t>
+          <t>RICAPA RAMOS, MILAGROS PATRICIA</t>
         </is>
       </c>
       <c r="C13" s="3" t="inlineStr">
         <is>
-          <t>10:45-14:30</t>
+          <t>09:15-18:15</t>
         </is>
       </c>
       <c r="D13" s="3" t="n"/>
       <c r="E13" s="14" t="n">
         <v>5</v>
       </c>
-      <c r="F13" s="3" t="inlineStr">
-        <is>
-          <t>BONILLA SANCHEZ, RAUL FERNANDO</t>
-        </is>
-      </c>
-      <c r="G13" s="3" t="inlineStr">
-        <is>
-          <t>19:00-22:45</t>
-        </is>
-      </c>
+      <c r="F13" s="3" t="n"/>
+      <c r="G13" s="3" t="n"/>
       <c r="H13" s="3" t="n"/>
     </row>
     <row r="14" ht="19.5" customHeight="1">
       <c r="A14" s="14" t="n"/>
       <c r="B14" s="3" t="inlineStr">
         <is>
-          <t>IDELFONSO MOTTA, JHOSSEP ANGELO</t>
+          <t>PEREZ GORMAS, ANTHONY</t>
         </is>
       </c>
       <c r="C14" s="3" t="inlineStr">
         <is>
-          <t>15:00-18:45</t>
+          <t>18:15-22:00</t>
         </is>
       </c>
       <c r="D14" s="3" t="n"/>
@@ -7248,12 +7360,12 @@
       </c>
       <c r="B15" s="3" t="inlineStr">
         <is>
-          <t>TARDILLO COPA, YOVANNA MELISSA</t>
+          <t>HUAMANI HUAMAN, MARICRUZ DESIDE</t>
         </is>
       </c>
       <c r="C15" s="3" t="inlineStr">
         <is>
-          <t>10:45-14:30</t>
+          <t>10:00-13:45</t>
         </is>
       </c>
       <c r="D15" s="3" t="n"/>
@@ -7262,12 +7374,12 @@
       </c>
       <c r="F15" s="3" t="inlineStr">
         <is>
-          <t>ZAPATA VILLANUEVA, FIORELLA YASMIN</t>
+          <t>FABIAN VALDIVIA, LINDSAY ZIYI</t>
         </is>
       </c>
       <c r="G15" s="3" t="inlineStr">
         <is>
-          <t>19:00-22:45</t>
+          <t>18:00-21:45</t>
         </is>
       </c>
       <c r="H15" s="3" t="n"/>
@@ -7281,7 +7393,7 @@
       </c>
       <c r="C16" s="3" t="inlineStr">
         <is>
-          <t>15:00-18:45</t>
+          <t>14:15-18:00</t>
         </is>
       </c>
       <c r="D16" s="3" t="n"/>
@@ -7296,26 +7408,42 @@
       </c>
       <c r="B17" s="3" t="inlineStr">
         <is>
-          <t>RAMOS TINOCO, JORDAN JAVIER</t>
+          <t>QUISPE MONDRAGON, JUAN ALFONSO</t>
         </is>
       </c>
       <c r="C17" s="3" t="inlineStr">
         <is>
-          <t>10:45-19:45</t>
+          <t>10:30-14:15</t>
         </is>
       </c>
       <c r="D17" s="3" t="n"/>
       <c r="E17" s="14" t="n">
         <v>7</v>
       </c>
-      <c r="F17" s="3" t="n"/>
-      <c r="G17" s="3" t="n"/>
+      <c r="F17" s="3" t="inlineStr">
+        <is>
+          <t>ROA ZARATE, ELIZABETH LUCY</t>
+        </is>
+      </c>
+      <c r="G17" s="3" t="inlineStr">
+        <is>
+          <t>19:00-22:45</t>
+        </is>
+      </c>
       <c r="H17" s="3" t="n"/>
     </row>
     <row r="18" ht="19.5" customHeight="1">
       <c r="A18" s="14" t="n"/>
-      <c r="B18" s="3" t="n"/>
-      <c r="C18" s="3" t="n"/>
+      <c r="B18" s="3" t="inlineStr">
+        <is>
+          <t>SICHA JORGE, JOSE ANGELO</t>
+        </is>
+      </c>
+      <c r="C18" s="3" t="inlineStr">
+        <is>
+          <t>14:30-18:15</t>
+        </is>
+      </c>
       <c r="D18" s="3" t="n"/>
       <c r="E18" s="14" t="n"/>
       <c r="F18" s="3" t="n"/>
@@ -7328,12 +7456,12 @@
       </c>
       <c r="B19" s="3" t="inlineStr">
         <is>
-          <t>QUIQUIA RICALDE, LILIA MARIA</t>
+          <t>RAMOS TINOCO, JORDAN JAVIER</t>
         </is>
       </c>
       <c r="C19" s="3" t="inlineStr">
         <is>
-          <t>11:00-20:00</t>
+          <t>10:30-19:30</t>
         </is>
       </c>
       <c r="D19" s="3" t="n"/>
@@ -7360,7 +7488,7 @@
       </c>
       <c r="B21" s="3" t="inlineStr">
         <is>
-          <t>SOTO VELAZCO, EMIR ALESSANDRO</t>
+          <t>RAMOS FARFAN, BRYAN ENRIQUE</t>
         </is>
       </c>
       <c r="C21" s="3" t="inlineStr">
@@ -7372,20 +7500,28 @@
       <c r="E21" s="14" t="n">
         <v>9</v>
       </c>
-      <c r="F21" s="3" t="n"/>
-      <c r="G21" s="3" t="n"/>
+      <c r="F21" s="3" t="inlineStr">
+        <is>
+          <t>HUANCAS SHUAN, JOSELYN JAZMIN</t>
+        </is>
+      </c>
+      <c r="G21" s="3" t="inlineStr">
+        <is>
+          <t>19:00-22:45</t>
+        </is>
+      </c>
       <c r="H21" s="3" t="n"/>
     </row>
     <row r="22" ht="19.5" customHeight="1">
       <c r="A22" s="14" t="n"/>
       <c r="B22" s="3" t="inlineStr">
         <is>
-          <t>POVEA CANTARO, FARID YASSER</t>
+          <t>HUAMANI LOPEZ, DREYDI BELINDA</t>
         </is>
       </c>
       <c r="C22" s="3" t="inlineStr">
         <is>
-          <t>15:00-18:45</t>
+          <t>14:45-18:30</t>
         </is>
       </c>
       <c r="D22" s="3" t="n"/>
@@ -7400,7 +7536,7 @@
       </c>
       <c r="B23" s="3" t="inlineStr">
         <is>
-          <t>BRANCACHO RAMIREZ, BRINDY</t>
+          <t>IDME GOMEZ, MILAGROS</t>
         </is>
       </c>
       <c r="C23" s="3" t="inlineStr">
@@ -7412,8 +7548,16 @@
       <c r="E23" s="14" t="n">
         <v>10</v>
       </c>
-      <c r="F23" s="3" t="n"/>
-      <c r="G23" s="3" t="n"/>
+      <c r="F23" s="3" t="inlineStr">
+        <is>
+          <t>ZAPATA VILLANUEVA, FIORELLA YASMIN</t>
+        </is>
+      </c>
+      <c r="G23" s="3" t="inlineStr">
+        <is>
+          <t>19:00-22:45</t>
+        </is>
+      </c>
       <c r="H23" s="3" t="n"/>
     </row>
     <row r="24" ht="18.75" customHeight="1">
@@ -7425,7 +7569,7 @@
       </c>
       <c r="C24" s="3" t="inlineStr">
         <is>
-          <t>17:30-21:15</t>
+          <t>15:15-19:00</t>
         </is>
       </c>
       <c r="D24" s="3" t="n"/>
@@ -7440,12 +7584,12 @@
       </c>
       <c r="B25" s="3" t="inlineStr">
         <is>
-          <t>CASAPAICO RIVERA, ENZO MANUEL</t>
+          <t>BRANCACHO RAMIREZ, BRINDY</t>
         </is>
       </c>
       <c r="C25" s="3" t="inlineStr">
         <is>
-          <t>11:15-15:00</t>
+          <t>11:00-14:45</t>
         </is>
       </c>
       <c r="D25" s="3" t="n"/>
@@ -7460,12 +7604,12 @@
       <c r="A26" s="14" t="n"/>
       <c r="B26" s="3" t="inlineStr">
         <is>
-          <t>PEREZ GORMAS, ANTHONY</t>
+          <t>GARRIDO SOTO, VICTORIA CELESTE</t>
         </is>
       </c>
       <c r="C26" s="3" t="inlineStr">
         <is>
-          <t>17:30-21:15</t>
+          <t>17:00-20:45</t>
         </is>
       </c>
       <c r="D26" s="3" t="n"/>
@@ -7480,7 +7624,7 @@
       </c>
       <c r="B27" s="3" t="inlineStr">
         <is>
-          <t>QUIQUIA MALLQUI, CYNTHIA ANGELLINE</t>
+          <t>CASAPAICO RIVERA, ENZO MANUEL</t>
         </is>
       </c>
       <c r="C27" s="3" t="inlineStr">
@@ -7500,12 +7644,12 @@
       <c r="A28" s="14" t="n"/>
       <c r="B28" s="3" t="inlineStr">
         <is>
-          <t>LEON TICONA, MARIA FERNANDA</t>
+          <t>BONILLA SANCHEZ, RAUL FERNANDO</t>
         </is>
       </c>
       <c r="C28" s="3" t="inlineStr">
         <is>
-          <t>18:00-21:45</t>
+          <t>17:00-20:45</t>
         </is>
       </c>
       <c r="D28" s="3" t="n"/>
@@ -7520,12 +7664,12 @@
       </c>
       <c r="B29" s="3" t="inlineStr">
         <is>
-          <t>RICAPA RAMOS, MILAGROS PATRICIA</t>
+          <t>SUICA GOÑAZ, KEISY YVONNE</t>
         </is>
       </c>
       <c r="C29" s="3" t="inlineStr">
         <is>
-          <t>12:00-21:00</t>
+          <t>11:30-15:15</t>
         </is>
       </c>
       <c r="D29" s="3" t="n"/>
@@ -7538,8 +7682,16 @@
     </row>
     <row r="30" ht="18.75" customHeight="1">
       <c r="A30" s="14" t="n"/>
-      <c r="B30" s="3" t="n"/>
-      <c r="C30" s="3" t="n"/>
+      <c r="B30" s="3" t="inlineStr">
+        <is>
+          <t>MAYTA QUINTANA, ANDY KEVIN</t>
+        </is>
+      </c>
+      <c r="C30" s="3" t="inlineStr">
+        <is>
+          <t>18:00-21:45</t>
+        </is>
+      </c>
       <c r="D30" s="3" t="n"/>
       <c r="E30" s="14" t="n"/>
       <c r="F30" s="3" t="n"/>
@@ -7552,12 +7704,12 @@
       </c>
       <c r="B31" s="3" t="inlineStr">
         <is>
-          <t>PARIONA CARRASCO, YAZMIN</t>
+          <t>LEON TICONA, MARIA FERNANDA</t>
         </is>
       </c>
       <c r="C31" s="3" t="inlineStr">
         <is>
-          <t>12:00-20:45</t>
+          <t>18:00-21:45</t>
         </is>
       </c>
       <c r="D31" s="3" t="n"/>
@@ -7582,16 +7734,8 @@
       <c r="A33" s="14" t="n">
         <v>15</v>
       </c>
-      <c r="B33" s="3" t="inlineStr">
-        <is>
-          <t>HUANCAS SHUAN, JOSELYN JAZMIN</t>
-        </is>
-      </c>
-      <c r="C33" s="3" t="inlineStr">
-        <is>
-          <t>18:00-21:45</t>
-        </is>
-      </c>
+      <c r="B33" s="3" t="n"/>
+      <c r="C33" s="3" t="n"/>
       <c r="D33" s="3" t="n"/>
       <c r="E33" s="14" t="n">
         <v>15</v>
@@ -7726,7 +7870,7 @@
       </c>
       <c r="B44" s="3" t="inlineStr">
         <is>
-          <t>GARRIDO SOTO, VICTORIA CELESTE</t>
+          <t>ROCA IBARAN, MIRLA VALENTINA</t>
         </is>
       </c>
       <c r="C44" s="3" t="inlineStr">
@@ -7738,42 +7882,26 @@
       <c r="E44" s="14" t="n">
         <v>21</v>
       </c>
-      <c r="F44" s="3" t="inlineStr">
-        <is>
-          <t>SICHA JORGE, JOSE ANGELO</t>
-        </is>
-      </c>
-      <c r="G44" s="3" t="inlineStr">
-        <is>
-          <t>14:30-18:15</t>
-        </is>
-      </c>
+      <c r="F44" s="3" t="n"/>
+      <c r="G44" s="3" t="n"/>
       <c r="H44" s="3" t="n"/>
     </row>
     <row r="45" ht="18.75" customHeight="1">
       <c r="A45" s="14" t="n"/>
       <c r="B45" s="3" t="inlineStr">
         <is>
-          <t>ALVITE CORNEJO, ANGIE LUCERO</t>
+          <t>QUIQUIA RICALDE, LILIA MARIA</t>
         </is>
       </c>
       <c r="C45" s="3" t="inlineStr">
         <is>
-          <t>10:45-14:30</t>
+          <t>10:45-19:45</t>
         </is>
       </c>
       <c r="D45" s="3" t="n"/>
       <c r="E45" s="14" t="n"/>
-      <c r="F45" s="3" t="inlineStr">
-        <is>
-          <t>VILCAPOMA CHILIN, JULISSA JAZMIN</t>
-        </is>
-      </c>
-      <c r="G45" s="3" t="inlineStr">
-        <is>
-          <t>18:30-18:45</t>
-        </is>
-      </c>
+      <c r="F45" s="3" t="n"/>
+      <c r="G45" s="3" t="n"/>
       <c r="H45" s="3" t="n"/>
     </row>
     <row r="46" ht="18.75" customHeight="1">
@@ -7782,12 +7910,12 @@
       </c>
       <c r="B46" s="3" t="inlineStr">
         <is>
-          <t>JIMENEZ TORERO, ASTRID GERALDINE</t>
+          <t>TARDILLO COPA, YOVANNA MELISSA</t>
         </is>
       </c>
       <c r="C46" s="3" t="inlineStr">
         <is>
-          <t>08:00-17:00</t>
+          <t>08:00-11:45</t>
         </is>
       </c>
       <c r="D46" s="3" t="n"/>
@@ -7802,12 +7930,12 @@
       <c r="A47" s="14" t="n"/>
       <c r="B47" s="3" t="inlineStr">
         <is>
-          <t>FABIAN VALDIVIA, LINDSAY ZIYI</t>
+          <t>TITO LAURA, NANCY FIORELLA</t>
         </is>
       </c>
       <c r="C47" s="3" t="inlineStr">
         <is>
-          <t>17:30-21:15</t>
+          <t>13:00-22:00</t>
         </is>
       </c>
       <c r="D47" s="3" t="n"/>
@@ -7822,7 +7950,7 @@
       </c>
       <c r="B48" s="3" t="inlineStr">
         <is>
-          <t>BONILLA SANCHEZ, RAUL FERNANDO</t>
+          <t>ROA ZARATE, ELIZABETH LUCY</t>
         </is>
       </c>
       <c r="C48" s="3" t="inlineStr">
@@ -7944,7 +8072,7 @@
       </c>
       <c r="F54" s="12" t="inlineStr">
         <is>
-          <t>CHAHUA BENITO, JEFFERSON ALVARO</t>
+          <t>CONDORI FLORES, ROSARIO</t>
         </is>
       </c>
       <c r="G54" s="12" t="inlineStr">
@@ -7978,7 +8106,7 @@
       </c>
       <c r="F55" s="10" t="inlineStr">
         <is>
-          <t>CONDORI FLORES, ROSARIO</t>
+          <t>CHAHUA BENITO, JEFFERSON ALVARO</t>
         </is>
       </c>
       <c r="G55" s="10" t="inlineStr">

</xml_diff>